<commit_message>
Blueprints added: 	Grey Stairs 	Double Small Column 	Wall Model D Updated spreadsheet, added factory diagram and new savegame
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_tdarksteel forge - Final\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0720A6D8-EB79-4B71-A203-9DA224FDC07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAD899E-2DFE-4958-8F6D-40301E76D12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Chandra Flameworks" sheetId="2" r:id="rId2"/>
+    <sheet name="Darksteel Forge" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Item</t>
   </si>
@@ -130,6 +131,42 @@
   </si>
   <si>
     <t>16327.4 MW</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Cut-Time</t>
+  </si>
+  <si>
+    <t>Darksteel Forge</t>
+  </si>
+  <si>
+    <t>Iron Ore</t>
+  </si>
+  <si>
+    <t>Iron Ingot</t>
+  </si>
+  <si>
+    <t>0 Mw</t>
+  </si>
+  <si>
+    <t>2268.3 MW</t>
+  </si>
+  <si>
+    <t>4600 MW</t>
+  </si>
+  <si>
+    <t>2.02 Hours</t>
+  </si>
+  <si>
+    <t>-2268.3 MW</t>
+  </si>
+  <si>
+    <t>Iron Ingots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darksteel Forge </t>
   </si>
 </sst>
 </file>
@@ -161,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -384,11 +421,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,22 +483,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -801,38 +859,38 @@
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -877,9 +935,15 @@
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C8" s="2"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="12">
+        <v>3342.848</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="15"/>
       <c r="J8" s="9"/>
@@ -1137,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDCCE8D-0CE2-4D53-8FB4-EA2891D6F3B5}">
   <dimension ref="C3:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1153,25 +1217,25 @@
   <sheetData>
     <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="K4" s="17" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+      <c r="K4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1180,7 +1244,7 @@
       <c r="F5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="18" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="21" t="s">
@@ -1189,7 +1253,7 @@
       <c r="K5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="18" t="s">
         <v>1</v>
       </c>
       <c r="M5" s="21" t="s">
@@ -1197,7 +1261,7 @@
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1223,7 +1287,7 @@
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1249,7 +1313,7 @@
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1275,7 +1339,7 @@
       </c>
     </row>
     <row r="9" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1531,6 +1595,399 @@
       <c r="K38" s="3"/>
       <c r="L38" s="13"/>
       <c r="M38" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="K4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A244D34F-6552-48EC-88C9-9BCAF12F75CF}">
+  <dimension ref="C3:M1048576"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="28.90625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="28.90625" customWidth="1"/>
+    <col min="8" max="8" width="28.90625" customWidth="1"/>
+    <col min="11" max="11" width="28.90625" customWidth="1"/>
+    <col min="13" max="13" width="28.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+      <c r="K4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
+    </row>
+    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C6" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1800</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="11">
+        <v>3342.848</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C7" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="12">
+        <v>514.27200000000005</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C8" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="2"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="2"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="2"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="F12" s="2"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="2"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="F13" s="2"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="F14" s="2"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="F15" s="2"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="F16" s="2"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F17" s="2"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F18" s="2"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F19" s="2"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F20" s="2"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F21" s="2"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F22" s="2"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F23" s="2"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F24" s="2"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F25" s="2"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F26" s="2"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F27" s="2"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F28" s="2"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F29" s="2"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F30" s="2"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F31" s="2"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F32" s="2"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F33" s="2"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F34" s="2"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F35" s="2"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F36" s="2"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F37" s="2"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F38" s="3"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="1048576" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K1048576" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated savegame File Updated Factory Diagrams and Spreadsheet Added Wall Model D Blueprint Added Logistic Stairs Blueprint Added new refinery Blueprint
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_tdarksteel forge - Final\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_tdarksteel forge - Final - Copy\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAD899E-2DFE-4958-8F6D-40301E76D12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C815905-7037-4213-AB4C-3A0D059A003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="1" activeTab="3" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Chandra Flameworks" sheetId="2" r:id="rId2"/>
     <sheet name="Darksteel Forge" sheetId="3" r:id="rId3"/>
+    <sheet name="Xantcha's Crucible" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
   <si>
     <t>Item</t>
   </si>
@@ -167,6 +168,30 @@
   </si>
   <si>
     <t xml:space="preserve">Darksteel Forge </t>
+  </si>
+  <si>
+    <t>wa</t>
+  </si>
+  <si>
+    <t>Copper Ingots</t>
+  </si>
+  <si>
+    <t>Xantcha's Crucible</t>
+  </si>
+  <si>
+    <t>2286 MW</t>
+  </si>
+  <si>
+    <t>-2286 MW</t>
+  </si>
+  <si>
+    <t>8800 MWh</t>
+  </si>
+  <si>
+    <t>3.84 Hours</t>
+  </si>
+  <si>
+    <t>Copper Ore</t>
   </si>
 </sst>
 </file>
@@ -438,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,6 +515,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,14 +531,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,34 +867,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="20.6328125" customWidth="1"/>
-    <col min="8" max="8" width="25.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" style="1"/>
     <col min="10" max="10" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="21" t="s">
@@ -949,9 +973,15 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C9" s="2"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2250</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="15"/>
       <c r="J9" s="9"/>
@@ -1151,7 +1181,9 @@
     <row r="34" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C34" s="2"/>
       <c r="D34" s="12"/>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="6"/>
       <c r="I34" s="15"/>
       <c r="J34" s="9"/>
@@ -1202,17 +1234,19 @@
   <dimension ref="C3:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="28.90625" customWidth="1"/>
-    <col min="6" max="6" width="25.6328125" customWidth="1"/>
-    <col min="8" max="8" width="20.6328125" customWidth="1"/>
-    <col min="11" max="11" width="25.6328125" customWidth="1"/>
-    <col min="13" max="13" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1223,16 +1257,16 @@
       <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-      <c r="K4" s="27" t="s">
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="K4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="24" t="s">
@@ -1610,43 +1644,45 @@
   <dimension ref="C3:M1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="28.90625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="28.90625" customWidth="1"/>
-    <col min="8" max="8" width="28.90625" customWidth="1"/>
-    <col min="11" max="11" width="28.90625" customWidth="1"/>
-    <col min="13" max="13" width="28.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-      <c r="K4" s="27" t="s">
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="K4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="32" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="21" t="s">
@@ -1669,10 +1705,10 @@
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="32" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1695,10 +1731,10 @@
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1715,10 +1751,10 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="32" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="2"/>
@@ -1729,10 +1765,10 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="2"/>
@@ -1743,10 +1779,10 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="32" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="2"/>
@@ -1757,10 +1793,10 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="33" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="2"/>
@@ -1996,4 +2032,423 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD23EB3-FE0B-4D28-A04E-DA4ABD2C8717}">
+  <dimension ref="B1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C20:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="J2" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="11">
+        <v>900</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="11">
+        <v>2250</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="12">
+        <v>600</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="2"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="2"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C10" s="30"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C11" s="30"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" s="30"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated savefile, spreadsheet and Factory Diagrams to include Oran-Rief Mines
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_tdarksteel forge - Final - Copy\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Oran-Rief\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C815905-7037-4213-AB4C-3A0D059A003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A039D63-E4D8-4EBC-9BB5-D4650FA0853D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="1" activeTab="3" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Chandra Flameworks" sheetId="2" r:id="rId2"/>
     <sheet name="Darksteel Forge" sheetId="3" r:id="rId3"/>
     <sheet name="Xantcha's Crucible" sheetId="4" r:id="rId4"/>
+    <sheet name="Oran-Rief Mines" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -192,6 +193,27 @@
   </si>
   <si>
     <t>Copper Ore</t>
+  </si>
+  <si>
+    <t>Oran-Rief Mines</t>
+  </si>
+  <si>
+    <t>803.3 MW</t>
+  </si>
+  <si>
+    <t>-803.3 MW</t>
+  </si>
+  <si>
+    <t>2.74 Hours</t>
+  </si>
+  <si>
+    <t>2200 MWh</t>
+  </si>
+  <si>
+    <t>Caterium Ore</t>
+  </si>
+  <si>
+    <t>Caterium Ingots</t>
   </si>
 </sst>
 </file>
@@ -867,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,9 +1009,15 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C10" s="2"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="12">
+        <v>240</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="15"/>
       <c r="J10" s="9"/>
@@ -2038,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD23EB3-FE0B-4D28-A04E-DA4ABD2C8717}">
   <dimension ref="B1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C20:C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2451,4 +2479,423 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1350C4-6C4D-4B59-A3BC-5B1F652DB40B}">
+  <dimension ref="B1:L36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="J2" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="11">
+        <v>480</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="11">
+        <v>240</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="12">
+        <v>480</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="2"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="2"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C10" s="30"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C11" s="30"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" s="30"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added all of the stuff from Thran Foundry!
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Oran-Rief\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Thran Forge\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A039D63-E4D8-4EBC-9BB5-D4650FA0853D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BF1668-77EF-4D28-A2D8-E9C15F7FCA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Darksteel Forge" sheetId="3" r:id="rId3"/>
     <sheet name="Xantcha's Crucible" sheetId="4" r:id="rId4"/>
     <sheet name="Oran-Rief Mines" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
   <si>
     <t>Item</t>
   </si>
@@ -171,9 +172,6 @@
     <t xml:space="preserve">Darksteel Forge </t>
   </si>
   <si>
-    <t>wa</t>
-  </si>
-  <si>
     <t>Copper Ingots</t>
   </si>
   <si>
@@ -214,6 +212,30 @@
   </si>
   <si>
     <t>Caterium Ingots</t>
+  </si>
+  <si>
+    <t>Steel Ingots</t>
+  </si>
+  <si>
+    <t>Thran Foundry</t>
+  </si>
+  <si>
+    <t>Thran Foundy</t>
+  </si>
+  <si>
+    <t>466.8 MW</t>
+  </si>
+  <si>
+    <t>-466.8 MW</t>
+  </si>
+  <si>
+    <t>2900 MWh</t>
+  </si>
+  <si>
+    <t>6.21 Hours</t>
+  </si>
+  <si>
+    <t>Miners</t>
   </si>
 </sst>
 </file>
@@ -890,7 +912,7 @@
   <dimension ref="C3:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -985,7 +1007,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="12">
-        <v>3342.848</v>
+        <v>2382.848</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>42</v>
@@ -996,13 +1018,13 @@
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="12">
         <v>2250</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="15"/>
@@ -1010,22 +1032,28 @@
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="12">
         <v>240</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="15"/>
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C11" s="2"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1440</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="15"/>
       <c r="J11" s="9"/>
@@ -1209,9 +1237,7 @@
     <row r="34" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C34" s="2"/>
       <c r="D34" s="12"/>
-      <c r="E34" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="E34" s="2"/>
       <c r="H34" s="6"/>
       <c r="I34" s="15"/>
       <c r="J34" s="9"/>
@@ -1262,7 +1288,7 @@
   <dimension ref="C3:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1672,7 +1698,7 @@
   <dimension ref="C3:M1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1684,7 +1710,7 @@
     <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1737,7 +1763,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>34</v>
@@ -1752,7 +1778,7 @@
         <v>35</v>
       </c>
       <c r="L6" s="11">
-        <v>3342.848</v>
+        <v>2382.848</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>25</v>
@@ -1774,9 +1800,15 @@
       <c r="H7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="2"/>
+      <c r="K7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="12">
+        <v>960</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C8" s="28" t="s">
@@ -2088,7 +2120,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>15</v>
@@ -2135,7 +2167,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="11">
         <v>900</v>
@@ -2144,7 +2176,7 @@
         <v>21</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="11">
         <v>2250</v>
@@ -2178,7 +2210,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="12"/>
@@ -2192,7 +2224,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="12"/>
@@ -2206,7 +2238,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="12"/>
@@ -2220,7 +2252,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="12"/>
@@ -2486,7 +2518,7 @@
   <dimension ref="B1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B2" sqref="B2:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2507,7 +2539,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>15</v>
@@ -2554,7 +2586,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" s="11">
         <v>480</v>
@@ -2563,7 +2595,7 @@
         <v>21</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K4" s="11">
         <v>240</v>
@@ -2597,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="12"/>
@@ -2611,7 +2643,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="12"/>
@@ -2625,7 +2657,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="12"/>
@@ -2639,7 +2671,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="12"/>
@@ -2898,4 +2930,423 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9AFFE6-32CC-4ED3-90D1-1E871DB3E098}">
+  <dimension ref="B1:L36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="J2" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="11">
+        <v>960</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="11">
+        <v>1440</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="12">
+        <v>960</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="2"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="2"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C10" s="30"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C11" s="30"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" s="30"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
*Added Ketria Crystals Save game, and updated the spread sheets *Added Ketria Crystals factory diagram *Added the new asphalt rails. You can find them under rails. *Does someone read this? If you did read this, comment on a video of mine "Cosmic banana!"
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Thran Forge\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Ketria Crystals\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BF1668-77EF-4D28-A2D8-E9C15F7FCA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7E1AA0-98B9-4BFD-AFF1-DE5FE1D5370C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
@@ -18,7 +18,9 @@
     <sheet name="Darksteel Forge" sheetId="3" r:id="rId3"/>
     <sheet name="Xantcha's Crucible" sheetId="4" r:id="rId4"/>
     <sheet name="Oran-Rief Mines" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Thran Foundry" sheetId="6" r:id="rId6"/>
+    <sheet name="Neko's Nexus" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="102">
   <si>
     <t>Item</t>
   </si>
@@ -220,9 +222,6 @@
     <t>Thran Foundry</t>
   </si>
   <si>
-    <t>Thran Foundy</t>
-  </si>
-  <si>
     <t>466.8 MW</t>
   </si>
   <si>
@@ -236,6 +235,120 @@
   </si>
   <si>
     <t>Miners</t>
+  </si>
+  <si>
+    <t>Limestone</t>
+  </si>
+  <si>
+    <t>Water Extractors</t>
+  </si>
+  <si>
+    <t>Heavy Modular Frame</t>
+  </si>
+  <si>
+    <t>Modular Frames</t>
+  </si>
+  <si>
+    <t>Motors</t>
+  </si>
+  <si>
+    <t>Steel Beam</t>
+  </si>
+  <si>
+    <t>Rotors</t>
+  </si>
+  <si>
+    <t>Encased Industrial Beams</t>
+  </si>
+  <si>
+    <t>Stators</t>
+  </si>
+  <si>
+    <t>Quickwire</t>
+  </si>
+  <si>
+    <t>Portable Miners</t>
+  </si>
+  <si>
+    <t>Steel Pipes</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t>Reinforced Iron Plate</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>Copper Sheet</t>
+  </si>
+  <si>
+    <t>Iron Plate</t>
+  </si>
+  <si>
+    <t>Iron Rods</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t>Neko's Nexus</t>
+  </si>
+  <si>
+    <t>Darksteel Forge, Xantcha's Crucible, Oran-Rief Mines, Thran Foundry</t>
+  </si>
+  <si>
+    <t>822.8 MW</t>
+  </si>
+  <si>
+    <t>-822.8 MW</t>
+  </si>
+  <si>
+    <t>13.1 GWh</t>
+  </si>
+  <si>
+    <t>15.92 Hours</t>
+  </si>
+  <si>
+    <t>Top right belt going to Neko's Nexus has an extra 180 steel on it</t>
+  </si>
+  <si>
+    <t>Top right uncompressed belt going to Neko's Nexus has an extra 142.5 Copper</t>
+  </si>
+  <si>
+    <t>Thran Foundy, Neko's Nexus</t>
+  </si>
+  <si>
+    <t>Middle belt going to Neko's Nexus has an extra 368.75</t>
+  </si>
+  <si>
+    <t>Ketria Crystals</t>
+  </si>
+  <si>
+    <t>Quartz Crystals</t>
+  </si>
+  <si>
+    <t>Silica</t>
+  </si>
+  <si>
+    <t>Raw Quartz</t>
+  </si>
+  <si>
+    <t>1016.2 MW</t>
+  </si>
+  <si>
+    <t>-1016.2 MW</t>
+  </si>
+  <si>
+    <t>4300 Wh</t>
+  </si>
+  <si>
+    <t>4.23 Hours</t>
   </si>
 </sst>
 </file>
@@ -507,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,6 +679,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,6 +699,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,33 +1040,33 @@
   <dimension ref="C3:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="20.6328125" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="21" t="s">
@@ -1007,184 +1135,316 @@
         <v>41</v>
       </c>
       <c r="D8" s="12">
-        <v>2382.848</v>
+        <v>2271.598</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="9"/>
+      <c r="H8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="11">
+        <v>1.4065000000000001</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="12">
-        <v>2250</v>
+        <v>2107.5</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="9"/>
+      <c r="H9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="12">
+        <v>2.25</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="12">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="9"/>
+      <c r="H10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D11" s="12">
-        <v>1440</v>
+        <v>1140</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="9"/>
+      <c r="H11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="12">
+        <v>45</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C12" s="2"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="2"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="9"/>
+      <c r="C12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="12">
+        <v>723.33299999999997</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C13" s="2"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="2"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="9"/>
+      <c r="C13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="12">
+        <v>680.55499999999995</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="12">
+        <v>7.3125</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
       <c r="E14" s="2"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="9"/>
+      <c r="H14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="12">
+        <v>3</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
       <c r="D15" s="12"/>
       <c r="E15" s="2"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="9"/>
+      <c r="H15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="12">
+        <v>30</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
       <c r="E16" s="2"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="9"/>
+      <c r="H16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C17" s="2"/>
       <c r="D17" s="12"/>
       <c r="E17" s="2"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="9"/>
+      <c r="H17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="12">
+        <v>33.125</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="9"/>
+      <c r="H18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="12">
+        <v>61.6875</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C19" s="2"/>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="9"/>
+      <c r="H19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C20" s="2"/>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="9"/>
+      <c r="H20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="12">
+        <v>30</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="9"/>
+      <c r="H21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="12">
+        <v>45</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="9"/>
+      <c r="H22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="12">
+        <v>22.5</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
       <c r="D23" s="12"/>
       <c r="E23" s="2"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="9"/>
+      <c r="H23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
       <c r="D24" s="12"/>
       <c r="E24" s="2"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="9"/>
+      <c r="H24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="12">
+        <v>15</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C25" s="2"/>
       <c r="D25" s="12"/>
       <c r="E25" s="2"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="9"/>
+      <c r="H25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="12">
+        <v>25</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C26" s="2"/>
       <c r="D26" s="12"/>
       <c r="E26" s="2"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="9"/>
+      <c r="H26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I26" s="11">
+        <v>23.332999999999998</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C27" s="2"/>
       <c r="D27" s="12"/>
       <c r="E27" s="2"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="9"/>
+      <c r="H27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="12">
+        <v>19.443999999999999</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C28" s="2"/>
@@ -1311,16 +1571,16 @@
       <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="K4" s="34" t="s">
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="K4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="24" t="s">
@@ -1695,10 +1955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A244D34F-6552-48EC-88C9-9BCAF12F75CF}">
-  <dimension ref="C3:M1048576"/>
+  <dimension ref="C3:S1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1713,240 +1973,213 @@
     <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="K4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-    </row>
-    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C6" s="28" t="s">
+    </row>
+    <row r="6" spans="3:19" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1800</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="11">
-        <v>2382.848</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D6" s="37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12">
-        <v>514.27200000000005</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="12">
-        <v>960</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C8" s="28" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="2"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C9" s="28" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="2"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C10" s="28" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="2"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="29" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="2"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F12" s="2"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="2"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F13" s="2"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F14" s="2"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F15" s="2"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F16" s="2"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F13" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
+      <c r="K13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="39"/>
+      <c r="M13" s="40"/>
+    </row>
+    <row r="14" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="F15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1800</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="11">
+        <v>2271.598</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="F16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="12">
+        <v>514.27200000000005</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="12">
+        <v>960</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="G17" s="12"/>
       <c r="H17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="K17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="12">
+        <v>111.25</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+    </row>
+    <row r="18" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="K18" s="4"/>
       <c r="L18" s="12"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="G19" s="12"/>
       <c r="H19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="K19" s="4"/>
       <c r="L19" s="12"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="G20" s="12"/>
       <c r="H20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="K20" s="4"/>
       <c r="L20" s="12"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="G21" s="12"/>
       <c r="H21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="4"/>
       <c r="L21" s="12"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="G22" s="12"/>
       <c r="H22" s="2"/>
@@ -1954,7 +2187,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="G23" s="12"/>
       <c r="H23" s="2"/>
@@ -1962,7 +2195,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="G24" s="12"/>
       <c r="H24" s="2"/>
@@ -1970,7 +2203,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
@@ -1978,7 +2211,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="G26" s="12"/>
       <c r="H26" s="2"/>
@@ -1986,7 +2219,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="G27" s="12"/>
       <c r="H27" s="2"/>
@@ -1994,7 +2227,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="G28" s="12"/>
       <c r="H28" s="2"/>
@@ -2002,7 +2235,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
@@ -2010,7 +2243,7 @@
       <c r="L29" s="12"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="G30" s="12"/>
       <c r="H30" s="2"/>
@@ -2018,7 +2251,7 @@
       <c r="L30" s="12"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
@@ -2026,7 +2259,7 @@
       <c r="L31" s="12"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="G32" s="12"/>
       <c r="H32" s="2"/>
@@ -2074,21 +2307,94 @@
       <c r="L37" s="12"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F38" s="3"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="3"/>
+    <row r="38" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F38" s="2"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F39" s="2"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F40" s="2"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F41" s="2"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F42" s="2"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F43" s="2"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F44" s="2"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F45" s="2"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F46" s="2"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F47" s="3"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="3"/>
     </row>
     <row r="1048576" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K1048576" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="K4:M4"/>
+  <mergeCells count="3">
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="O14:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2096,10 +2402,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD23EB3-FE0B-4D28-A04E-DA4ABD2C8717}">
-  <dimension ref="B1:L36"/>
+  <dimension ref="B1:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L36"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2111,29 +2417,29 @@
     <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="J2" s="34" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="J2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
-    </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
@@ -2158,13 +2464,21 @@
       <c r="L3" s="21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N3" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>49</v>
@@ -2179,13 +2493,19 @@
         <v>43</v>
       </c>
       <c r="K4" s="11">
-        <v>2250</v>
+        <v>2107.5</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
@@ -2201,11 +2521,23 @@
       <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="J5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="12">
+        <v>142.5</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -2218,8 +2550,14 @@
       <c r="J6" s="4"/>
       <c r="K6" s="12"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
         <v>14</v>
       </c>
@@ -2233,7 +2571,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -2247,7 +2585,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
@@ -2261,7 +2599,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C10" s="30"/>
       <c r="E10" s="2"/>
       <c r="F10" s="12"/>
@@ -2270,7 +2608,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C11" s="30"/>
       <c r="E11" s="2"/>
       <c r="F11" s="12"/>
@@ -2279,7 +2617,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C12" s="30"/>
       <c r="E12" s="2"/>
       <c r="F12" s="12"/>
@@ -2288,7 +2626,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C13" s="30"/>
       <c r="E13" s="2"/>
       <c r="F13" s="12"/>
@@ -2297,7 +2635,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
       <c r="E14" s="2"/>
       <c r="F14" s="12"/>
@@ -2306,7 +2644,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
       <c r="E15" s="2"/>
       <c r="F15" s="12"/>
@@ -2315,7 +2653,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
       <c r="E16" s="2"/>
       <c r="F16" s="12"/>
@@ -2505,9 +2843,10 @@
       <c r="L36" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N3:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2518,7 +2857,7 @@
   <dimension ref="B1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L36"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2530,7 +2869,7 @@
     <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -2541,16 +2880,16 @@
       <c r="C2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="J2" s="34" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="J2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="28" t="s">
@@ -2583,7 +2922,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>55</v>
@@ -2598,7 +2937,7 @@
         <v>56</v>
       </c>
       <c r="K4" s="11">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>25</v>
@@ -2620,9 +2959,15 @@
       <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="2"/>
+      <c r="J5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="12">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
@@ -2934,44 +3279,44 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9AFFE6-32CC-4ED3-90D1-1E871DB3E098}">
-  <dimension ref="B1:L36"/>
+  <dimension ref="B1:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="J2" s="34" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="J2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
-    </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
@@ -2996,13 +3341,21 @@
       <c r="L3" s="21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N3" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>41</v>
@@ -3017,13 +3370,19 @@
         <v>57</v>
       </c>
       <c r="K4" s="11">
-        <v>1440</v>
+        <v>1140</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
@@ -3037,18 +3396,30 @@
         <v>960</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="12">
+        <v>300</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="12"/>
@@ -3056,13 +3427,19 @@
       <c r="J6" s="4"/>
       <c r="K6" s="12"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="12"/>
@@ -3071,12 +3448,12 @@
       <c r="K7" s="12"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="12"/>
@@ -3085,12 +3462,12 @@
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="12"/>
@@ -3099,7 +3476,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C10" s="30"/>
       <c r="E10" s="2"/>
       <c r="F10" s="12"/>
@@ -3108,7 +3485,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C11" s="30"/>
       <c r="E11" s="2"/>
       <c r="F11" s="12"/>
@@ -3117,7 +3494,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C12" s="30"/>
       <c r="E12" s="2"/>
       <c r="F12" s="12"/>
@@ -3126,7 +3503,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C13" s="30"/>
       <c r="E13" s="2"/>
       <c r="F13" s="12"/>
@@ -3135,7 +3512,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
       <c r="E14" s="2"/>
       <c r="F14" s="12"/>
@@ -3144,7 +3521,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
       <c r="E15" s="2"/>
       <c r="F15" s="12"/>
@@ -3153,7 +3530,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
       <c r="E16" s="2"/>
       <c r="F16" s="12"/>
@@ -3343,9 +3720,1033 @@
       <c r="L36" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N3:S6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C5DD3A-A518-4C27-BB69-BA9A009C7B9C}">
+  <dimension ref="B1:L44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="30"/>
+      <c r="E10" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="J10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="30"/>
+      <c r="E11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="11">
+        <v>480</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="11">
+        <v>61.6875</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="12">
+        <v>422.5</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="12">
+        <v>45</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="12">
+        <v>300</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="12">
+        <v>45</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="12">
+        <v>142.5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="12">
+        <v>33.125</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="12">
+        <v>111.25</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="12">
+        <v>30</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="12">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="12">
+        <v>30</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="12">
+        <v>25</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="12">
+        <v>22.5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" s="12">
+        <v>15</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" s="12">
+        <v>7.3125</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="12">
+        <v>5</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" s="12">
+        <v>3</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="12">
+        <v>2.25</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="12">
+        <v>1.4065000000000001</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="30"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E12:G17">
+    <sortCondition descending="1" ref="F12:F17"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:L10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122A4D2D-7EB7-44FE-A97D-7046CE3D43BD}">
+  <dimension ref="B1:L44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="30"/>
+      <c r="E10" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="J10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="30"/>
+      <c r="E11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1260</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="11">
+        <v>23.332999999999998</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="12">
+        <v>500</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="12">
+        <v>19.443999999999999</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="12">
+        <v>533.33299999999997</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="12">
+        <v>723.33299999999997</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K15" s="12">
+        <v>680.55499999999995</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="30"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
*Added new wall, model G *Added column to hold a dimensional depot that will only work if you suspend them at the exact same height that I do. Good luck! *Renamed last savegame now that the factory has a name. Thanks Uolocur! *Added factory diagram of thran foundry that somehow I had forgotten to add *Cheers!
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Thran Forge\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Neko's Nexus\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BF1668-77EF-4D28-A2D8-E9C15F7FCA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1867ABD1-F790-4052-B48A-E8E16270DC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="6" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Darksteel Forge" sheetId="3" r:id="rId3"/>
     <sheet name="Xantcha's Crucible" sheetId="4" r:id="rId4"/>
     <sheet name="Oran-Rief Mines" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Thran Foundry" sheetId="6" r:id="rId6"/>
+    <sheet name="Neko's Nexus" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="94">
   <si>
     <t>Item</t>
   </si>
@@ -220,9 +221,6 @@
     <t>Thran Foundry</t>
   </si>
   <si>
-    <t>Thran Foundy</t>
-  </si>
-  <si>
     <t>466.8 MW</t>
   </si>
   <si>
@@ -236,6 +234,96 @@
   </si>
   <si>
     <t>Miners</t>
+  </si>
+  <si>
+    <t>Limestone</t>
+  </si>
+  <si>
+    <t>Water Extractors</t>
+  </si>
+  <si>
+    <t>Heavy Modular Frame</t>
+  </si>
+  <si>
+    <t>Modular Frames</t>
+  </si>
+  <si>
+    <t>Motors</t>
+  </si>
+  <si>
+    <t>Steel Beam</t>
+  </si>
+  <si>
+    <t>Rotors</t>
+  </si>
+  <si>
+    <t>Encased Industrial Beams</t>
+  </si>
+  <si>
+    <t>Stators</t>
+  </si>
+  <si>
+    <t>Quickwire</t>
+  </si>
+  <si>
+    <t>Portable Miners</t>
+  </si>
+  <si>
+    <t>Steel Pipes</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t>Reinforced Iron Plate</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>Copper Sheet</t>
+  </si>
+  <si>
+    <t>Iron Plate</t>
+  </si>
+  <si>
+    <t>Iron Rods</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t>Neko's Nexus</t>
+  </si>
+  <si>
+    <t>Darksteel Forge, Xantcha's Crucible, Oran-Rief Mines, Thran Foundry</t>
+  </si>
+  <si>
+    <t>822.8 MW</t>
+  </si>
+  <si>
+    <t>-822.8 MW</t>
+  </si>
+  <si>
+    <t>13.1 GWh</t>
+  </si>
+  <si>
+    <t>15.92 Hours</t>
+  </si>
+  <si>
+    <t>Top right belt going to Neko's Nexus has an extra 180 steel on it</t>
+  </si>
+  <si>
+    <t>Top right uncompressed belt going to Neko's Nexus has an extra 142.5 Copper</t>
+  </si>
+  <si>
+    <t>Thran Foundy, Neko's Nexus</t>
+  </si>
+  <si>
+    <t>Middle belt going to Neko's Nexus has an extra 368.75</t>
   </si>
 </sst>
 </file>
@@ -507,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,6 +662,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,18 +1014,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="20.6328125" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1007,168 +1110,276 @@
         <v>41</v>
       </c>
       <c r="D8" s="12">
-        <v>2382.848</v>
+        <v>2271.598</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="9"/>
+      <c r="H8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="11">
+        <v>1.4065000000000001</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="12">
-        <v>2250</v>
+        <v>2107.5</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="9"/>
+      <c r="H9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="12">
+        <v>2.25</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="12">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="9"/>
+      <c r="H10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D11" s="12">
-        <v>1440</v>
+        <v>1140</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="9"/>
+      <c r="H11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="12">
+        <v>45</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C12" s="2"/>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="9"/>
+      <c r="H12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C13" s="2"/>
       <c r="D13" s="12"/>
       <c r="E13" s="2"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="9"/>
+      <c r="H13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="12">
+        <v>7.3125</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
       <c r="E14" s="2"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="9"/>
+      <c r="H14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="12">
+        <v>3</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
       <c r="D15" s="12"/>
       <c r="E15" s="2"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="9"/>
+      <c r="H15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="12">
+        <v>30</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
       <c r="E16" s="2"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="9"/>
+      <c r="H16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C17" s="2"/>
       <c r="D17" s="12"/>
       <c r="E17" s="2"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="9"/>
+      <c r="H17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="12">
+        <v>33.125</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="9"/>
+      <c r="H18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="12">
+        <v>61.6875</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C19" s="2"/>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="9"/>
+      <c r="H19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C20" s="2"/>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="9"/>
+      <c r="H20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="12">
+        <v>30</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="9"/>
+      <c r="H21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="12">
+        <v>45</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="9"/>
+      <c r="H22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="12">
+        <v>22.5</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
       <c r="D23" s="12"/>
       <c r="E23" s="2"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="9"/>
+      <c r="H23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
       <c r="D24" s="12"/>
       <c r="E24" s="2"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="9"/>
+      <c r="H24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="12">
+        <v>15</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C25" s="2"/>
       <c r="D25" s="12"/>
       <c r="E25" s="2"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="9"/>
+      <c r="H25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="12">
+        <v>25</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C26" s="2"/>
@@ -1695,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A244D34F-6552-48EC-88C9-9BCAF12F75CF}">
-  <dimension ref="C3:M1048576"/>
+  <dimension ref="C3:S1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1713,240 +1924,213 @@
     <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="K4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-    </row>
-    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C6" s="28" t="s">
+    </row>
+    <row r="6" spans="3:19" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1800</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="11">
-        <v>2382.848</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D6" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12">
-        <v>514.27200000000005</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="12">
-        <v>960</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C8" s="28" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="2"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C9" s="28" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="2"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C10" s="28" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="2"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="29" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="2"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F12" s="2"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="2"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F13" s="2"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F14" s="2"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F15" s="2"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="F16" s="2"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F13" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="K13" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="35"/>
+      <c r="M13" s="36"/>
+    </row>
+    <row r="14" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="F15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1800</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="11">
+        <v>2271.598</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="F16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="12">
+        <v>514.27200000000005</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="12">
+        <v>960</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="G17" s="12"/>
       <c r="H17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="K17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="12">
+        <v>111.25</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+    </row>
+    <row r="18" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="K18" s="4"/>
       <c r="L18" s="12"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="G19" s="12"/>
       <c r="H19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="K19" s="4"/>
       <c r="L19" s="12"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="G20" s="12"/>
       <c r="H20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="K20" s="4"/>
       <c r="L20" s="12"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="G21" s="12"/>
       <c r="H21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="4"/>
       <c r="L21" s="12"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="G22" s="12"/>
       <c r="H22" s="2"/>
@@ -1954,7 +2138,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="G23" s="12"/>
       <c r="H23" s="2"/>
@@ -1962,7 +2146,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="G24" s="12"/>
       <c r="H24" s="2"/>
@@ -1970,7 +2154,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
@@ -1978,7 +2162,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="G26" s="12"/>
       <c r="H26" s="2"/>
@@ -1986,7 +2170,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="G27" s="12"/>
       <c r="H27" s="2"/>
@@ -1994,7 +2178,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="G28" s="12"/>
       <c r="H28" s="2"/>
@@ -2002,7 +2186,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
@@ -2010,7 +2194,7 @@
       <c r="L29" s="12"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="G30" s="12"/>
       <c r="H30" s="2"/>
@@ -2018,7 +2202,7 @@
       <c r="L30" s="12"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
@@ -2026,7 +2210,7 @@
       <c r="L31" s="12"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="6:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="G32" s="12"/>
       <c r="H32" s="2"/>
@@ -2074,21 +2258,94 @@
       <c r="L37" s="12"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F38" s="3"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="3"/>
+    <row r="38" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F38" s="2"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F39" s="2"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F40" s="2"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F41" s="2"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F42" s="2"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F43" s="2"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F44" s="2"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F45" s="2"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="F46" s="2"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F47" s="3"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="3"/>
     </row>
     <row r="1048576" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K1048576" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="K4:M4"/>
+  <mergeCells count="3">
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="O14:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2096,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD23EB3-FE0B-4D28-A04E-DA4ABD2C8717}">
-  <dimension ref="B1:L36"/>
+  <dimension ref="B1:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L36"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2111,11 +2368,11 @@
     <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
@@ -2133,7 +2390,7 @@
       <c r="K2" s="35"/>
       <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
@@ -2158,13 +2415,21 @@
       <c r="L3" s="21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N3" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>49</v>
@@ -2179,13 +2444,19 @@
         <v>43</v>
       </c>
       <c r="K4" s="11">
-        <v>2250</v>
+        <v>2107.5</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
@@ -2201,11 +2472,23 @@
       <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="J5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="12">
+        <v>142.5</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -2218,8 +2501,14 @@
       <c r="J6" s="4"/>
       <c r="K6" s="12"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
         <v>14</v>
       </c>
@@ -2233,7 +2522,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -2247,7 +2536,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
@@ -2261,7 +2550,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C10" s="30"/>
       <c r="E10" s="2"/>
       <c r="F10" s="12"/>
@@ -2270,7 +2559,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C11" s="30"/>
       <c r="E11" s="2"/>
       <c r="F11" s="12"/>
@@ -2279,7 +2568,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C12" s="30"/>
       <c r="E12" s="2"/>
       <c r="F12" s="12"/>
@@ -2288,7 +2577,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C13" s="30"/>
       <c r="E13" s="2"/>
       <c r="F13" s="12"/>
@@ -2297,7 +2586,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
       <c r="E14" s="2"/>
       <c r="F14" s="12"/>
@@ -2306,7 +2595,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
       <c r="E15" s="2"/>
       <c r="F15" s="12"/>
@@ -2315,7 +2604,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
       <c r="E16" s="2"/>
       <c r="F16" s="12"/>
@@ -2505,9 +2794,10 @@
       <c r="L36" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N3:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2518,7 +2808,7 @@
   <dimension ref="B1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L36"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2530,7 +2820,7 @@
     <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -2583,7 +2873,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>55</v>
@@ -2598,7 +2888,7 @@
         <v>56</v>
       </c>
       <c r="K4" s="11">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>25</v>
@@ -2620,9 +2910,15 @@
       <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="2"/>
+      <c r="J5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="12">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
@@ -2934,26 +3230,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9AFFE6-32CC-4ED3-90D1-1E871DB3E098}">
-  <dimension ref="B1:L36"/>
+  <dimension ref="B1:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
@@ -2971,7 +3267,7 @@
       <c r="K2" s="35"/>
       <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
@@ -2996,13 +3292,21 @@
       <c r="L3" s="21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N3" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>41</v>
@@ -3017,13 +3321,19 @@
         <v>57</v>
       </c>
       <c r="K4" s="11">
-        <v>1440</v>
+        <v>1140</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
@@ -3037,18 +3347,30 @@
         <v>960</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="12">
+        <v>300</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="12"/>
@@ -3056,13 +3378,19 @@
       <c r="J6" s="4"/>
       <c r="K6" s="12"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="12"/>
@@ -3071,12 +3399,12 @@
       <c r="K7" s="12"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="12"/>
@@ -3085,12 +3413,12 @@
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="12"/>
@@ -3099,7 +3427,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C10" s="30"/>
       <c r="E10" s="2"/>
       <c r="F10" s="12"/>
@@ -3108,7 +3436,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C11" s="30"/>
       <c r="E11" s="2"/>
       <c r="F11" s="12"/>
@@ -3117,7 +3445,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C12" s="30"/>
       <c r="E12" s="2"/>
       <c r="F12" s="12"/>
@@ -3126,7 +3454,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C13" s="30"/>
       <c r="E13" s="2"/>
       <c r="F13" s="12"/>
@@ -3135,7 +3463,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
       <c r="E14" s="2"/>
       <c r="F14" s="12"/>
@@ -3144,7 +3472,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
       <c r="E15" s="2"/>
       <c r="F15" s="12"/>
@@ -3153,7 +3481,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
       <c r="E16" s="2"/>
       <c r="F16" s="12"/>
@@ -3343,9 +3671,574 @@
       <c r="L36" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N3:S6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C5DD3A-A518-4C27-BB69-BA9A009C7B9C}">
+  <dimension ref="B1:L44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="30"/>
+      <c r="E10" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="J10" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="36"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="30"/>
+      <c r="E11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="11">
+        <v>480</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="11">
+        <v>61.6875</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="12">
+        <v>422.5</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="12">
+        <v>45</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="12">
+        <v>300</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="12">
+        <v>45</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="12">
+        <v>142.5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="12">
+        <v>33.125</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="12">
+        <v>111.25</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="12">
+        <v>30</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="12">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="12">
+        <v>30</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="12">
+        <v>25</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="12">
+        <v>22.5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" s="12">
+        <v>15</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" s="12">
+        <v>7.3125</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="12">
+        <v>5</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" s="12">
+        <v>3</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="12">
+        <v>2.25</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="12">
+        <v>1.4065000000000001</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="30"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E12:G17">
+    <sortCondition descending="1" ref="F12:F17"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added savegame for Kaladesh Refinery, the factory diagram and updated the Spreadsheet. No new blueprints today
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_KGhirapur Gridworks\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Kaladesh Refinery\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B213EDA-AAC5-47BA-B378-ED15EDA48FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A320A92-3A07-4D60-8BD6-9C718C83A64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="5030" windowWidth="28800" windowHeight="15370" activeTab="8" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="7" activeTab="9" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Neko's Nexus" sheetId="7" r:id="rId7"/>
     <sheet name="Ketria Crystals" sheetId="8" r:id="rId8"/>
     <sheet name="Ghirapur Gridworks" sheetId="10" r:id="rId9"/>
+    <sheet name="Kaladesh Refinery" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="122">
   <si>
     <t>Item</t>
   </si>
@@ -389,6 +390,27 @@
   </si>
   <si>
     <t>Circuit Boards</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Empty Canisters</t>
+  </si>
+  <si>
+    <t>Crude Oil</t>
+  </si>
+  <si>
+    <t>Kaladesh Refinery</t>
+  </si>
+  <si>
+    <t>2217.5 MW</t>
+  </si>
+  <si>
+    <t>-2217.5 MW</t>
+  </si>
+  <si>
+    <t>3.96 Hours</t>
   </si>
 </sst>
 </file>
@@ -734,6 +756,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -745,9 +770,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,7 +1108,7 @@
   <dimension ref="C3:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1101,18 +1123,18 @@
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="21" t="s">
@@ -1149,7 +1171,7 @@
       <c r="H6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="39">
         <v>15</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -1297,9 +1319,15 @@
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C14" s="2"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="12">
+        <v>475</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="H14" s="5" t="s">
         <v>72</v>
       </c>
@@ -1311,9 +1339,15 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C15" s="2"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="12">
+        <v>390</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="H15" s="6" t="s">
         <v>73</v>
       </c>
@@ -1325,9 +1359,9 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C16" s="2"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="4"/>
       <c r="H16" s="6" t="s">
         <v>74</v>
       </c>
@@ -1339,9 +1373,9 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C17" s="2"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="4"/>
       <c r="H17" s="6" t="s">
         <v>75</v>
       </c>
@@ -1566,17 +1600,29 @@
       <c r="C33" s="2"/>
       <c r="D33" s="12"/>
       <c r="E33" s="2"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="9"/>
+      <c r="H33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I33" s="11">
+        <v>25</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C34" s="2"/>
       <c r="D34" s="12"/>
       <c r="E34" s="2"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="9"/>
+      <c r="H34" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34" s="12">
+        <v>20</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C35" s="2"/>
@@ -1614,6 +1660,459 @@
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="H4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBAD9F1-0099-4C27-8F14-6139C4B3501A}">
+  <dimension ref="B1:L44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="30"/>
+      <c r="E10" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="J10" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="30"/>
+      <c r="E11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="11">
+        <v>300</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="11">
+        <v>25</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" s="12">
+        <v>475</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="12">
+        <v>390</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="12">
+        <v>20</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="30"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1647,16 +2146,16 @@
       <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
-      <c r="K4" s="39" t="s">
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+      <c r="K4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="42"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="24" t="s">
@@ -2117,16 +2616,16 @@
     </row>
     <row r="12" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="41"/>
-      <c r="K13" s="39" t="s">
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
+      <c r="K13" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="42"/>
     </row>
     <row r="14" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="21" t="s">
@@ -2147,13 +2646,13 @@
       <c r="M14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="42" t="s">
+      <c r="O14" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
@@ -2174,11 +2673,11 @@
       <c r="M15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
@@ -2199,11 +2698,11 @@
       <c r="M16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
     </row>
     <row r="17" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
@@ -2218,11 +2717,11 @@
       <c r="M17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
     </row>
     <row r="18" spans="6:19" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
@@ -2573,16 +3072,16 @@
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="30"/>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
-      <c r="J11" s="39" t="s">
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="J11" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="30"/>
@@ -2604,14 +3103,14 @@
       <c r="L12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="42" t="s">
+      <c r="N12" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C13" s="30"/>
@@ -2633,12 +3132,12 @@
       <c r="L13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
@@ -2660,12 +3159,12 @@
       <c r="L14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
@@ -2681,12 +3180,12 @@
       <c r="L15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
@@ -3049,16 +3548,16 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="30"/>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
-      <c r="J11" s="39" t="s">
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="J11" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="30"/>
@@ -3436,16 +3935,16 @@
       <c r="C2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="J2" s="39" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="J2" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
     </row>
     <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="28" t="s">
@@ -3472,14 +3971,14 @@
       <c r="L3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="28" t="s">
@@ -3506,12 +4005,12 @@
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
@@ -3538,12 +4037,12 @@
       <c r="L5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
@@ -3558,12 +4057,12 @@
       <c r="J6" s="4"/>
       <c r="K6" s="12"/>
       <c r="L6" s="2"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
@@ -3947,16 +4446,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="30"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="J10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="30"/>
@@ -4429,7 +4928,7 @@
   <dimension ref="B1:P44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L44"/>
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4513,16 +5012,16 @@
     </row>
     <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="30"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="J10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="30"/>
@@ -4907,8 +5406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56653220-9795-4D3E-A3FB-8E6AD78BB38D}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4990,16 +5489,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="30"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="J10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="30"/>

</xml_diff>

<commit_message>
Fixed small error on spreadsheet
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Kaladesh Refinery\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A320A92-3A07-4D60-8BD6-9C718C83A64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBAF7AC-C41F-48E4-BECA-54D4140AFC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="7" activeTab="9" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1607,7 +1607,7 @@
         <v>25</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.35">
@@ -1621,7 +1621,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.35">
@@ -1669,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBAD9F1-0099-4C27-8F14-6139C4B3501A}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added chain blueprints under Architecture/chains Added module sign under Decoration/Furniture Added Rail Bridge support under Rail/Accesories Modiefied 3m ramps under Rail/Ramps Added factory diagram for Abyssal Chains of Shandalar, with really low definition because I screwed up Updated the Savegame Added small readme files to the savegame
Cheers!
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Kaladesh Refinery\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Abyssal chains of shandalar\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBAF7AC-C41F-48E4-BECA-54D4140AFC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF56F2DF-5903-4F0B-A121-7806DE3D8551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="6280" yWindow="3300" windowWidth="28820" windowHeight="15380" firstSheet="6" activeTab="10" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Ketria Crystals" sheetId="8" r:id="rId8"/>
     <sheet name="Ghirapur Gridworks" sheetId="10" r:id="rId9"/>
     <sheet name="Kaladesh Refinery" sheetId="11" r:id="rId10"/>
+    <sheet name="The Abyssal Chains of Shandalar" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="140">
   <si>
     <t>Item</t>
   </si>
@@ -350,9 +351,6 @@
     <t>Neko's Nexus, Ghirapur Gridworks</t>
   </si>
   <si>
-    <t xml:space="preserve">Middle belt going to Neko's Nexus / Ghirapur Gridworks  has an extra 331.25 </t>
-  </si>
-  <si>
     <t>Thran Foundy, Neko's Nexus, Ghirapur Gridworks</t>
   </si>
   <si>
@@ -411,6 +409,63 @@
   </si>
   <si>
     <t>3.96 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottom left belt going to The Abyssal Chains of shandalar has an extra 366.1666 Copper Ingots </t>
+  </si>
+  <si>
+    <t>The Abyssal Chains of Shandalar</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Bottom Left</t>
+  </si>
+  <si>
+    <t>Top Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle belt (Middle row and column) going to Neko's Nexus / Ghirapur Gridworks  has an extra 331.25 </t>
+  </si>
+  <si>
+    <t>Row 2 Column 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row 3 Column 1 and 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Ingot </t>
+  </si>
+  <si>
+    <t>Row 2 Column 1</t>
+  </si>
+  <si>
+    <t>Plastic Belt going to the Abyssal Chains of Shandalar (Middle) has an extra 348 Plastic</t>
+  </si>
+  <si>
+    <t>Rubber Belt going to the Abyssal Chains of Shandalar (Right) has an extra 217.5 Rubber</t>
+  </si>
+  <si>
+    <t>Modular Engines</t>
+  </si>
+  <si>
+    <t>Adaptive Control Units</t>
+  </si>
+  <si>
+    <t>Darksteel Forge, Xantcha's Crucible, Kaladesh Refinery</t>
+  </si>
+  <si>
+    <t>231.9 MW</t>
+  </si>
+  <si>
+    <t>-231.9 MW</t>
+  </si>
+  <si>
+    <t>14.7 GWh</t>
+  </si>
+  <si>
+    <t>63.39 Hours</t>
   </si>
 </sst>
 </file>
@@ -442,7 +497,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -678,11 +733,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -770,6 +860,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,18 +1206,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1203,7 +1302,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="12">
-        <v>2234.098</v>
+        <v>1999.848</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>42</v>
@@ -1223,7 +1322,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="12">
-        <v>2002.85</v>
+        <v>1889.01666</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>44</v>
@@ -1320,13 +1419,13 @@
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C14" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="12">
-        <v>475</v>
+        <v>467.5</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>72</v>
@@ -1343,10 +1442,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="12">
-        <v>390</v>
+        <v>348</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>73</v>
@@ -1531,7 +1630,7 @@
       <c r="D28" s="12"/>
       <c r="E28" s="2"/>
       <c r="H28" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I28" s="15">
         <v>1.5</v>
@@ -1545,7 +1644,7 @@
       <c r="D29" s="12"/>
       <c r="E29" s="2"/>
       <c r="H29" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I29" s="15">
         <v>1.5</v>
@@ -1559,7 +1658,7 @@
       <c r="D30" s="12"/>
       <c r="E30" s="2"/>
       <c r="H30" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I30" s="15">
         <v>2.25</v>
@@ -1573,7 +1672,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="2"/>
       <c r="H31" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I31" s="15">
         <v>3</v>
@@ -1587,7 +1686,7 @@
       <c r="D32" s="12"/>
       <c r="E32" s="2"/>
       <c r="H32" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I32" s="15">
         <v>6</v>
@@ -1601,13 +1700,13 @@
       <c r="D33" s="12"/>
       <c r="E33" s="2"/>
       <c r="H33" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I33" s="11">
         <v>25</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.35">
@@ -1615,30 +1714,42 @@
       <c r="D34" s="12"/>
       <c r="E34" s="2"/>
       <c r="H34" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I34" s="12">
         <v>20</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C35" s="2"/>
       <c r="D35" s="12"/>
       <c r="E35" s="2"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="9"/>
+      <c r="H35" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I35" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C36" s="2"/>
       <c r="D36" s="12"/>
       <c r="E36" s="2"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="9"/>
+      <c r="H36" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I36" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C37" s="2"/>
@@ -1667,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBAD9F1-0099-4C27-8F14-6139C4B3501A}">
-  <dimension ref="B1:L44"/>
+  <dimension ref="B1:T44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1682,6 +1793,563 @@
     <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="30"/>
+      <c r="E10" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="J10" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="42"/>
+    </row>
+    <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="30"/>
+      <c r="E11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C12" s="30"/>
+      <c r="E12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="11">
+        <v>300</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K12" s="11">
+        <v>25</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="O12" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C13" s="30"/>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" s="12">
+        <v>467.5</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C14" s="30"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="12">
+        <v>348</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C15" s="30"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" s="12">
+        <v>20</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C16" s="30"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="O16" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="12">
+        <v>42</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C18" s="30"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="2"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C19" s="30"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="2"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C20" s="30"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C21" s="30"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C22" s="30"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C24" s="30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C26" s="30"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C27" s="30"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C28" s="30"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C29" s="30"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C30" s="30"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C31" s="30"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C33" s="30"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C34" s="30"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C35" s="30"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C36" s="30"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="O12:T15"/>
+    <mergeCell ref="O16:T19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1308C4-E9DD-438E-A79A-D3E0D96AB566}">
+  <dimension ref="B1:L44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1691,15 +2359,15 @@
         <v>9</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B3" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -1723,7 +2391,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -1731,7 +2399,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -1739,7 +2407,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1747,7 +2415,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1787,19 +2455,19 @@
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C12" s="30"/>
       <c r="E12" s="4" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="F12" s="11">
-        <v>300</v>
+        <v>18.75</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="K12" s="11">
-        <v>25</v>
+        <v>0.5</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>8</v>
@@ -1811,65 +2479,77 @@
         <v>19</v>
       </c>
       <c r="F13" s="12">
-        <v>1000</v>
+        <v>28.625</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="K13" s="12">
-        <v>475</v>
+        <v>0.5</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="4"/>
-      <c r="J14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="12">
-        <v>390</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="12">
+        <v>113.833</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="2"/>
-      <c r="J15" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K15" s="12">
-        <v>20</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="12">
+        <v>234.25</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="12">
+        <v>42</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="12"/>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C17" s="30"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="12"/>
       <c r="L17" s="4"/>
@@ -2530,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A244D34F-6552-48EC-88C9-9BCAF12F75CF}">
-  <dimension ref="C3:S1048576"/>
+  <dimension ref="C3:T1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2545,12 +3225,13 @@
     <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
@@ -2558,7 +3239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
@@ -2566,15 +3247,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:19" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:20" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="36" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C7" s="28" t="s">
         <v>12</v>
       </c>
@@ -2582,7 +3263,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C8" s="28" t="s">
         <v>13</v>
       </c>
@@ -2590,7 +3271,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C9" s="28" t="s">
         <v>14</v>
       </c>
@@ -2598,7 +3279,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C10" s="28" t="s">
         <v>31</v>
       </c>
@@ -2606,7 +3287,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="29" t="s">
         <v>32</v>
       </c>
@@ -2614,8 +3295,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F13" s="40" t="s">
         <v>15</v>
       </c>
@@ -2625,9 +3306,10 @@
         <v>16</v>
       </c>
       <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
-    </row>
-    <row r="14" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M13" s="41"/>
+      <c r="N13" s="42"/>
+    </row>
+    <row r="14" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="21" t="s">
         <v>0</v>
       </c>
@@ -2646,15 +3328,18 @@
       <c r="M14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="P14" s="43"/>
+      <c r="N14" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="P14" s="43" t="s">
+        <v>126</v>
+      </c>
       <c r="Q14" s="43"/>
       <c r="R14" s="43"/>
       <c r="S14" s="43"/>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="T14" s="43"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
         <v>34</v>
       </c>
@@ -2668,18 +3353,19 @@
         <v>35</v>
       </c>
       <c r="L15" s="11">
-        <v>2234.098</v>
+        <v>1999.848</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O15" s="43"/>
+      <c r="N15" s="26"/>
       <c r="P15" s="43"/>
       <c r="Q15" s="43"/>
       <c r="R15" s="43"/>
       <c r="S15" s="43"/>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="T15" s="43"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
         <v>19</v>
       </c>
@@ -2698,13 +3384,16 @@
       <c r="M16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O16" s="43"/>
+      <c r="N16" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="P16" s="43"/>
       <c r="Q16" s="43"/>
       <c r="R16" s="43"/>
       <c r="S16" s="43"/>
-    </row>
-    <row r="17" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="T16" s="43"/>
+    </row>
+    <row r="17" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="G17" s="12"/>
       <c r="H17" s="2"/>
@@ -2717,13 +3406,16 @@
       <c r="M17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O17" s="43"/>
+      <c r="N17" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="P17" s="43"/>
       <c r="Q17" s="43"/>
       <c r="R17" s="43"/>
       <c r="S17" s="43"/>
-    </row>
-    <row r="18" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="T17" s="43"/>
+    </row>
+    <row r="18" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="G18" s="12"/>
       <c r="H18" s="2"/>
@@ -2736,238 +3428,282 @@
       <c r="M18" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N18" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="G19" s="12"/>
       <c r="H19" s="2"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="K19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="L19" s="12">
+        <v>234.25</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="G20" s="12"/>
       <c r="H20" s="2"/>
       <c r="K20" s="4"/>
       <c r="L20" s="12"/>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N20" s="2"/>
+      <c r="P20">
+        <f>2234.098-234.25</f>
+        <v>1999.848</v>
+      </c>
+    </row>
+    <row r="21" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="G21" s="12"/>
       <c r="H21" s="2"/>
       <c r="K21" s="4"/>
       <c r="L21" s="12"/>
       <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="G22" s="12"/>
       <c r="H22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="12"/>
       <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="G23" s="12"/>
       <c r="H23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="12"/>
       <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="G24" s="12"/>
       <c r="H24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="12"/>
       <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="G25" s="12"/>
       <c r="H25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="12"/>
       <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="G26" s="12"/>
       <c r="H26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="12"/>
       <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="G27" s="12"/>
       <c r="H27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="12"/>
       <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="G28" s="12"/>
       <c r="H28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="12"/>
       <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="G29" s="12"/>
       <c r="H29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="12"/>
       <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="G30" s="12"/>
       <c r="H30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="12"/>
       <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="12"/>
       <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="G32" s="12"/>
       <c r="H32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="12"/>
       <c r="M32" s="2"/>
-    </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
       <c r="G33" s="12"/>
       <c r="H33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="12"/>
       <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
       <c r="G34" s="12"/>
       <c r="H34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="12"/>
       <c r="M34" s="2"/>
-    </row>
-    <row r="35" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
       <c r="G35" s="12"/>
       <c r="H35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="12"/>
       <c r="M35" s="2"/>
-    </row>
-    <row r="36" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
       <c r="G36" s="12"/>
       <c r="H36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="12"/>
       <c r="M36" s="2"/>
-    </row>
-    <row r="37" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
       <c r="G37" s="12"/>
       <c r="H37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="12"/>
       <c r="M37" s="2"/>
-    </row>
-    <row r="38" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
       <c r="G38" s="12"/>
       <c r="H38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="12"/>
       <c r="M38" s="2"/>
-    </row>
-    <row r="39" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F39" s="2"/>
       <c r="G39" s="12"/>
       <c r="H39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="12"/>
       <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F40" s="2"/>
       <c r="G40" s="12"/>
       <c r="H40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="12"/>
       <c r="M40" s="2"/>
-    </row>
-    <row r="41" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F41" s="2"/>
       <c r="G41" s="12"/>
       <c r="H41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="12"/>
       <c r="M41" s="2"/>
-    </row>
-    <row r="42" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F42" s="2"/>
       <c r="G42" s="12"/>
       <c r="H42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="12"/>
       <c r="M42" s="2"/>
-    </row>
-    <row r="43" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F43" s="2"/>
       <c r="G43" s="12"/>
       <c r="H43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="12"/>
       <c r="M43" s="2"/>
-    </row>
-    <row r="44" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F44" s="2"/>
       <c r="G44" s="12"/>
       <c r="H44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="12"/>
       <c r="M44" s="2"/>
-    </row>
-    <row r="45" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F45" s="2"/>
       <c r="G45" s="12"/>
       <c r="H45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="12"/>
       <c r="M45" s="2"/>
-    </row>
-    <row r="46" spans="6:13" x14ac:dyDescent="0.35">
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F46" s="2"/>
       <c r="G46" s="12"/>
       <c r="H46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="12"/>
       <c r="M46" s="2"/>
-    </row>
-    <row r="47" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F47" s="3"/>
       <c r="G47" s="13"/>
       <c r="H47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="13"/>
       <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
     </row>
     <row r="1048576" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K1048576" s="4"/>
@@ -2975,8 +3711,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="F13:H13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="O14:S17"/>
+    <mergeCell ref="P14:T17"/>
+    <mergeCell ref="K13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2984,10 +3720,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD23EB3-FE0B-4D28-A04E-DA4ABD2C8717}">
-  <dimension ref="B1:S45"/>
+  <dimension ref="B1:T45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12:T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2998,12 +3734,14 @@
     <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.6328125" customWidth="1"/>
+    <col min="15" max="15" width="18.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
@@ -3011,7 +3749,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" s="28" t="s">
         <v>10</v>
       </c>
@@ -3019,7 +3757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="36" t="s">
         <v>11</v>
       </c>
@@ -3027,7 +3765,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
@@ -3035,7 +3773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -3043,7 +3781,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
         <v>14</v>
       </c>
@@ -3051,7 +3789,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -3059,7 +3797,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
@@ -3067,10 +3805,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="30"/>
     </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="30"/>
       <c r="E11" s="40" t="s">
         <v>15</v>
@@ -3081,9 +3819,10 @@
         <v>16</v>
       </c>
       <c r="K11" s="41"/>
-      <c r="L11" s="42"/>
-    </row>
-    <row r="12" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L11" s="41"/>
+      <c r="M11" s="42"/>
+    </row>
+    <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="30"/>
       <c r="E12" s="21" t="s">
         <v>0</v>
@@ -3094,25 +3833,28 @@
       <c r="G12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="O12" s="43"/>
+      <c r="M12" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="O12" s="43" t="s">
+        <v>104</v>
+      </c>
       <c r="P12" s="43"/>
       <c r="Q12" s="43"/>
       <c r="R12" s="43"/>
       <c r="S12" s="43"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="T12" s="43"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="30"/>
       <c r="E13" s="4" t="s">
         <v>49</v>
@@ -3127,19 +3869,20 @@
         <v>43</v>
       </c>
       <c r="K13" s="11">
-        <v>2002.85</v>
-      </c>
-      <c r="L13" s="4" t="s">
+        <v>1889.01666</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N13" s="43"/>
+      <c r="M13" s="26"/>
       <c r="O13" s="43"/>
       <c r="P13" s="43"/>
       <c r="Q13" s="43"/>
       <c r="R13" s="43"/>
       <c r="S13" s="43"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="T13" s="43"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
       <c r="E14" s="2" t="s">
         <v>19</v>
@@ -3156,17 +3899,20 @@
       <c r="K14" s="12">
         <v>142.5</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="43"/>
+      <c r="M14" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="O14" s="43"/>
       <c r="P14" s="43"/>
       <c r="Q14" s="43"/>
       <c r="R14" s="43"/>
       <c r="S14" s="43"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="T14" s="43"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="30"/>
       <c r="E15" s="2"/>
       <c r="F15" s="12"/>
@@ -3177,282 +3923,350 @@
       <c r="K15" s="12">
         <v>104.65</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="43"/>
+      <c r="M15" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="O15" s="43"/>
       <c r="P15" s="43"/>
       <c r="Q15" s="43"/>
       <c r="R15" s="43"/>
       <c r="S15" s="43"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="T15" s="43"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="30"/>
       <c r="E16" s="2"/>
       <c r="F16" s="12"/>
       <c r="G16" s="2"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="J16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="12">
+        <v>113.833</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="O16" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="30"/>
       <c r="E17" s="2"/>
       <c r="F17" s="12"/>
       <c r="G17" s="2"/>
       <c r="J17" s="4"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L17" s="6"/>
+      <c r="M17" s="2"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="30"/>
       <c r="E18" s="2"/>
       <c r="F18" s="12"/>
       <c r="G18" s="2"/>
       <c r="J18" s="4"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L18" s="6"/>
+      <c r="M18" s="2"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="30"/>
       <c r="E19" s="2"/>
       <c r="F19" s="12"/>
       <c r="G19" s="2"/>
       <c r="J19" s="4"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L19" s="6"/>
+      <c r="M19" s="2"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="30"/>
       <c r="E20" s="2"/>
       <c r="F20" s="12"/>
       <c r="G20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L20" s="6"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C21" s="30"/>
       <c r="E21" s="2"/>
       <c r="F21" s="12"/>
       <c r="G21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L21" s="6"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="30"/>
       <c r="E22" s="2"/>
       <c r="F22" s="12"/>
       <c r="G22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="12"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L22" s="6"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C23" s="30"/>
       <c r="E23" s="2"/>
       <c r="F23" s="12"/>
       <c r="G23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="12"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L23" s="6"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="30"/>
       <c r="E24" s="2"/>
       <c r="F24" s="12"/>
       <c r="G24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="12"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L24" s="6"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="30"/>
       <c r="E25" s="2"/>
       <c r="F25" s="12"/>
       <c r="G25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="12"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L25" s="6"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="30"/>
       <c r="E26" s="2"/>
       <c r="F26" s="12"/>
       <c r="G26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L26" s="6"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="30"/>
       <c r="E27" s="2"/>
       <c r="F27" s="12"/>
       <c r="G27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="12"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L27" s="6"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="30"/>
       <c r="E28" s="2"/>
       <c r="F28" s="12"/>
       <c r="G28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="12"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L28" s="6"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="30"/>
       <c r="E29" s="2"/>
       <c r="F29" s="12"/>
       <c r="G29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="12"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L29" s="6"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="30"/>
       <c r="E30" s="2"/>
       <c r="F30" s="12"/>
       <c r="G30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="12"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L30" s="6"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="30"/>
       <c r="E31" s="2"/>
       <c r="F31" s="12"/>
       <c r="G31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="12"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L31" s="6"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C32" s="30"/>
       <c r="E32" s="2"/>
       <c r="F32" s="12"/>
       <c r="G32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L32" s="6"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C33" s="30"/>
       <c r="E33" s="2"/>
       <c r="F33" s="12"/>
       <c r="G33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="12"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L33" s="6"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C34" s="30"/>
       <c r="E34" s="2"/>
       <c r="F34" s="12"/>
       <c r="G34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L34" s="6"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C35" s="30"/>
       <c r="E35" s="2"/>
       <c r="F35" s="12"/>
       <c r="G35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L35" s="6"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C36" s="30"/>
       <c r="E36" s="2"/>
       <c r="F36" s="12"/>
       <c r="G36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L36" s="6"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E37" s="2"/>
       <c r="F37" s="12"/>
       <c r="G37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L37" s="6"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E38" s="2"/>
       <c r="F38" s="12"/>
       <c r="G38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L38" s="6"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E39" s="2"/>
       <c r="F39" s="12"/>
       <c r="G39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L39" s="6"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E40" s="2"/>
       <c r="F40" s="12"/>
       <c r="G40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="12"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L40" s="6"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E41" s="2"/>
       <c r="F41" s="12"/>
       <c r="G41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="12"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L41" s="6"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E42" s="2"/>
       <c r="F42" s="12"/>
       <c r="G42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="12"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L42" s="6"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E43" s="2"/>
       <c r="F43" s="12"/>
       <c r="G43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="12"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="L43" s="6"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.35">
       <c r="E44" s="2"/>
       <c r="F44" s="12"/>
       <c r="G44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="12"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L44" s="6"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E45" s="3"/>
       <c r="F45" s="13"/>
       <c r="G45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="13"/>
-      <c r="L45" s="3"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E11:G11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="N12:S15"/>
+    <mergeCell ref="O12:T15"/>
+    <mergeCell ref="O16:T19"/>
+    <mergeCell ref="J11:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4363,8 +5177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C5DD3A-A518-4C27-BB69-BA9A009C7B9C}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5044,7 +5858,7 @@
         <v>24</v>
       </c>
       <c r="P11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.35">
@@ -5068,7 +5882,7 @@
         <v>8</v>
       </c>
       <c r="P12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.35">
@@ -5460,7 +6274,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -5468,7 +6282,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -5476,7 +6290,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5484,7 +6298,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5533,7 +6347,7 @@
         <v>50</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K12" s="11">
         <v>1.5</v>
@@ -5554,7 +6368,7 @@
         <v>33</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="12">
         <v>1.5</v>
@@ -5575,7 +6389,7 @@
         <v>65</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K14" s="12">
         <v>2.25</v>
@@ -5596,7 +6410,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K15" s="12">
         <v>3</v>
@@ -5617,7 +6431,7 @@
         <v>91</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K16" s="12">
         <v>6</v>

</xml_diff>

<commit_message>
1) Updated spreadsheet for Jund Pyroclast 2) Added factory diagrams for Jund Pyroclast 3) Added Jund Pyroclast Save Game 4) Added expanded module signs blueprint on decoration-furniture 5) Added mk3 casing blueprint on decoration-buildings 6) Added a new swatch12 column blueprint on Decoration-swatch 12 columns 7) Added pipes support blueprint on Logistics-pipes 8) Added 12 purple assemblers Blueprint in Production-Assemblers (This    one is old)
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Nicos Blueprints_Phyrexian Datavault\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\jUND ICONOCLAST\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE4B23D-EA0A-4594-9859-6DBA38760E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F8CFFF-043A-41C0-A981-8B04EF560A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="4" activeTab="11" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="177">
   <si>
     <t>Item</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>1.76 Hours</t>
+  </si>
+  <si>
+    <t>Empty Fluid Tank</t>
+  </si>
+  <si>
+    <t>Jund Pyroclast</t>
   </si>
 </sst>
 </file>
@@ -864,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -944,6 +950,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -957,12 +972,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1301,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="C3:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J59"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1310,25 +1319,25 @@
     <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="41"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="15" t="s">
@@ -1354,13 +1363,13 @@
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C6" s="4" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="D6" s="8">
-        <v>10</v>
+        <v>410</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>5</v>
@@ -1573,15 +1582,9 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="9">
-        <v>410</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="4"/>
       <c r="H17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>140</v>
       </c>
       <c r="I39" s="11">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>134</v>
@@ -1909,7 +1912,7 @@
       </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H41" s="11" t="s">
+      <c r="H41" s="41" t="s">
         <v>169</v>
       </c>
       <c r="I41" s="11">
@@ -1920,7 +1923,7 @@
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="41" t="s">
         <v>170</v>
       </c>
       <c r="I42" s="11">
@@ -1931,14 +1934,26 @@
       </c>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H43" s="2"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I43" s="11">
+        <v>5</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H44" s="2"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" s="11">
+        <v>10</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.35">
       <c r="H45" s="2"/>
@@ -2066,7 +2081,7 @@
       <c r="B4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="39" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2112,17 +2127,17 @@
     </row>
     <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
@@ -2169,14 +2184,14 @@
         <v>8</v>
       </c>
       <c r="M12" s="20"/>
-      <c r="O12" s="42" t="s">
+      <c r="O12" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="24"/>
@@ -2199,12 +2214,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="24"/>
@@ -2221,12 +2236,12 @@
         <v>25</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="24"/>
@@ -2243,12 +2258,12 @@
         <v>8</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="24"/>
@@ -2265,14 +2280,14 @@
         <v>114</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="O16" s="42" t="s">
+      <c r="O16" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="24"/>
@@ -2289,12 +2304,12 @@
         <v>114</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="24"/>
@@ -2311,12 +2326,12 @@
         <v>154</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="24"/>
@@ -2333,12 +2348,12 @@
         <v>154</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="24"/>
@@ -2359,14 +2374,14 @@
       <c r="K21" s="9"/>
       <c r="L21" s="4"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="43" t="s">
+      <c r="O21" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="24"/>
@@ -2387,14 +2402,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="4"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="42" t="s">
+      <c r="O23" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="24"/>
@@ -2405,12 +2420,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="4"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="24"/>
@@ -2421,12 +2436,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="24"/>
@@ -2437,12 +2452,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="24"/>
@@ -2453,14 +2468,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="42" t="s">
+      <c r="O27" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="24"/>
@@ -2471,12 +2486,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="24"/>
@@ -2487,12 +2502,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="24"/>
@@ -2503,12 +2518,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="24"/>
@@ -2743,16 +2758,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
@@ -3125,8 +3140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED21A768-E1F1-4F70-B6C9-A662B38F9ACD}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3209,16 +3224,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
@@ -3319,7 +3334,7 @@
         <v>140</v>
       </c>
       <c r="K15" s="9">
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>8</v>
@@ -3387,18 +3402,30 @@
       <c r="E19" s="2"/>
       <c r="F19" s="9"/>
       <c r="G19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="4"/>
+      <c r="J19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K19" s="9">
+        <v>5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="24"/>
       <c r="E20" s="2"/>
       <c r="F20" s="9"/>
       <c r="G20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="4"/>
+      <c r="J20" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K20" s="9">
+        <v>150</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C21" s="24"/>
@@ -3704,16 +3731,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
@@ -3747,7 +3774,7 @@
       <c r="G12" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J12" s="45">
+      <c r="J12" s="40">
         <v>10</v>
       </c>
       <c r="K12" s="8" t="s">
@@ -3768,7 +3795,7 @@
       <c r="G13" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="45">
+      <c r="J13" s="40">
         <v>10</v>
       </c>
       <c r="K13" s="9" t="s">
@@ -3789,7 +3816,7 @@
       <c r="G14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="45"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="9"/>
       <c r="L14" s="4"/>
     </row>
@@ -3804,7 +3831,7 @@
       <c r="G15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="45"/>
+      <c r="J15" s="40"/>
       <c r="K15" s="9"/>
       <c r="L15" s="4"/>
     </row>
@@ -3819,7 +3846,7 @@
       <c r="G16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J16" s="45"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="9"/>
       <c r="L16" s="4"/>
     </row>
@@ -3834,7 +3861,7 @@
       <c r="G17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J17" s="45"/>
+      <c r="J17" s="40"/>
       <c r="K17" s="9"/>
       <c r="L17" s="4"/>
     </row>
@@ -3849,7 +3876,7 @@
       <c r="G18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="45"/>
+      <c r="J18" s="40"/>
       <c r="K18" s="9"/>
       <c r="L18" s="4"/>
     </row>
@@ -4099,7 +4126,7 @@
   <dimension ref="C3:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4122,16 +4149,16 @@
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
-      <c r="K4" s="39" t="s">
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
+      <c r="K4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="41"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="44"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="18" t="s">
@@ -4259,8 +4286,8 @@
       <c r="L9" s="9">
         <v>10</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>25</v>
+      <c r="M9" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.35">
@@ -4593,17 +4620,17 @@
     </row>
     <row r="12" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="41"/>
-      <c r="K13" s="39" t="s">
+      <c r="G13" s="43"/>
+      <c r="H13" s="44"/>
+      <c r="K13" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="41"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
     </row>
     <row r="14" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="15" t="s">
@@ -4627,13 +4654,13 @@
       <c r="N14" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
@@ -4655,11 +4682,11 @@
         <v>25</v>
       </c>
       <c r="N15" s="20"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
@@ -4683,11 +4710,11 @@
       <c r="N16" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
     </row>
     <row r="17" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
@@ -4705,11 +4732,11 @@
       <c r="N17" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
     </row>
     <row r="18" spans="6:20" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
@@ -5104,16 +5131,16 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
-      <c r="J11" s="39" t="s">
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+      <c r="J11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="44"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="24"/>
@@ -5562,17 +5589,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
-      <c r="J11" s="39" t="s">
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+      <c r="J11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="41"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
     </row>
     <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="24"/>
@@ -5597,14 +5624,14 @@
       <c r="M12" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="O12" s="42" t="s">
+      <c r="O12" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="24"/>
@@ -5628,12 +5655,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="20"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="24"/>
@@ -5658,12 +5685,12 @@
       <c r="M14" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="24"/>
@@ -5682,12 +5709,12 @@
       <c r="M15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="24"/>
@@ -5706,14 +5733,14 @@
       <c r="M16" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="O16" s="42" t="s">
+      <c r="O16" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="24"/>
@@ -5732,12 +5759,12 @@
       <c r="M17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="24"/>
@@ -5754,12 +5781,12 @@
         <v>154</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="24"/>
@@ -5770,12 +5797,12 @@
       <c r="K19" s="9"/>
       <c r="L19" s="6"/>
       <c r="M19" s="2"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
     </row>
     <row r="20" spans="3:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="24"/>
@@ -5796,14 +5823,14 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="43" t="s">
+      <c r="O21" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="24"/>
@@ -5824,14 +5851,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="42" t="s">
+      <c r="O23" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="24"/>
@@ -5842,12 +5869,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="24"/>
@@ -5858,12 +5885,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="24"/>
@@ -5874,12 +5901,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="6"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="24"/>
@@ -5890,14 +5917,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="6"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="42" t="s">
+      <c r="O27" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="24"/>
@@ -5908,12 +5935,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="6"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="24"/>
@@ -5924,12 +5951,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="6"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="24"/>
@@ -5940,12 +5967,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="6"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="24"/>
@@ -5956,14 +5983,14 @@
       <c r="K31" s="9"/>
       <c r="L31" s="6"/>
       <c r="M31" s="2"/>
-      <c r="O31" s="42" t="s">
+      <c r="O31" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
+      <c r="T31" s="45"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C32" s="24"/>
@@ -5974,12 +6001,12 @@
       <c r="K32" s="9"/>
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C33" s="24"/>
@@ -5990,12 +6017,12 @@
       <c r="K33" s="9"/>
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
-      <c r="S33" s="42"/>
-      <c r="T33" s="42"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C34" s="24"/>
@@ -6006,12 +6033,12 @@
       <c r="K34" s="9"/>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
-      <c r="S34" s="42"/>
-      <c r="T34" s="42"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C35" s="24"/>
@@ -6157,16 +6184,16 @@
       <c r="C2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="J2" s="39" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="J2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="41"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
     </row>
     <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="22" t="s">
@@ -6193,14 +6220,14 @@
       <c r="L3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="22" t="s">
@@ -6227,12 +6254,12 @@
       <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
@@ -6259,12 +6286,12 @@
       <c r="L5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="22" t="s">
@@ -6279,12 +6306,12 @@
       <c r="J6" s="4"/>
       <c r="K6" s="9"/>
       <c r="L6" s="2"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
@@ -6668,16 +6695,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
@@ -7188,7 +7215,7 @@
       <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="39" t="s">
         <v>163</v>
       </c>
     </row>
@@ -7234,16 +7261,16 @@
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>
@@ -7307,14 +7334,14 @@
       <c r="L13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="42" t="s">
+      <c r="N13" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="24"/>
@@ -7336,12 +7363,12 @@
       <c r="L14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="24"/>
@@ -7357,12 +7384,12 @@
       <c r="L15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
     </row>
     <row r="16" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="24"/>
@@ -7378,12 +7405,12 @@
       <c r="L16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
     </row>
     <row r="17" spans="3:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="24"/>
@@ -7399,14 +7426,14 @@
       <c r="L17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="24"/>
@@ -7422,12 +7449,12 @@
       <c r="L18" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="24"/>
@@ -7443,12 +7470,12 @@
       <c r="L19" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="24"/>
@@ -7458,12 +7485,12 @@
       <c r="J20" s="2"/>
       <c r="K20" s="9"/>
       <c r="L20" s="4"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="24"/>
@@ -7482,14 +7509,14 @@
       <c r="J22" s="2"/>
       <c r="K22" s="9"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="43" t="s">
+      <c r="N22" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="43"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="24"/>
@@ -7508,14 +7535,14 @@
       <c r="J24" s="2"/>
       <c r="K24" s="9"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="42" t="s">
+      <c r="N24" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C25" s="24"/>
@@ -7525,12 +7552,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="24"/>
@@ -7540,12 +7567,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="24"/>
@@ -7555,12 +7582,12 @@
       <c r="J27" s="2"/>
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="24"/>
@@ -7570,14 +7597,14 @@
       <c r="J28" s="2"/>
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="42" t="s">
+      <c r="N28" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="24"/>
@@ -7587,12 +7614,12 @@
       <c r="J29" s="2"/>
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="24"/>
@@ -7602,12 +7629,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="42"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="24"/>
@@ -7617,12 +7644,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="9"/>
       <c r="L31" s="2"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="24"/>
@@ -7834,16 +7861,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="24"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="J10" s="39" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="24"/>

</xml_diff>

<commit_message>
Added Karn's Conduit Stuff
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Obelisk Of Alara\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Karn's Conduit\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B5D07D-A665-4A27-B6CF-AF9F3E3226C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55E54FA-ACF8-4297-846D-DC0533CFF558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45984" yWindow="-4836" windowWidth="17472" windowHeight="15096" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Keldon Armory" sheetId="18" r:id="rId15"/>
     <sheet name="Urabrask's Refinery" sheetId="16" r:id="rId16"/>
     <sheet name="Obelisks of Alara " sheetId="19" r:id="rId17"/>
+    <sheet name="Karn's Conduit" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="257">
   <si>
     <t>Item</t>
   </si>
@@ -600,12 +601,6 @@
     <t>Middle belt going to has an extra 780 Iron Ingots</t>
   </si>
   <si>
-    <t>Bottom belt going to Keldon Armory has an extra 289.848 Iron Ingots</t>
-  </si>
-  <si>
-    <t>Thran Foundy, Neko's Nexus, Ghirapur Gridworks, The Abyssal Chains of Shandalar, Keldon Armory</t>
-  </si>
-  <si>
     <t>Nobelisk</t>
   </si>
   <si>
@@ -684,12 +679,6 @@
     <t>Obelisk of Alara</t>
   </si>
   <si>
-    <t>Neko's Nexus, Obelisk of Alara</t>
-  </si>
-  <si>
-    <t>Bottom Container has an extra 417.333</t>
-  </si>
-  <si>
     <t>Top Container has an extra 360</t>
   </si>
   <si>
@@ -723,12 +712,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Neko's Nexus, Ghirapur Gridworks, Phyrexian Datavault, Keldon Armory , Obelisks of Alara</t>
-  </si>
-  <si>
-    <t>Phyrexian Datavault, Keldon Armory, Jund Pyroclast, Urabrask's Refinery, Obelisks of Alara</t>
-  </si>
-  <si>
     <t>Oran Rief Mines</t>
   </si>
   <si>
@@ -784,6 +767,63 @@
   </si>
   <si>
     <t>Thermal Propulsion Rocket</t>
+  </si>
+  <si>
+    <t>Karn's Conduit</t>
+  </si>
+  <si>
+    <t>Neko's Nexus, Ghirapur Gridworks, Phyrexian Datavault, Keldon Armory , Obelisks of Alara, Karn's Conduit</t>
+  </si>
+  <si>
+    <t>Phyrexian Datavault, Keldon Armory, Jund Pyroclast, Urabrask's Refinery, Obelisks of Alara, Karn's Conduit</t>
+  </si>
+  <si>
+    <t>Neko's Nexus, Obelisk of Alara, Karn's Conduit</t>
+  </si>
+  <si>
+    <t>Bottom Container has an extra 227.324</t>
+  </si>
+  <si>
+    <t>Thran Foundy, Neko's Nexus, Ghirapur Gridworks, The Abyssal Chains of Shandalar, Keldon Armory, Karn's Conduit</t>
+  </si>
+  <si>
+    <t>Obelisks of Alara, Keldon Armory, Riveteers District, Phyrexian Datavault, Thran Foundry , Darksteel Forge</t>
+  </si>
+  <si>
+    <t>Bottom belt going to Keldon Armory and Karn's Conduit has an extra 277.835 Iron Ingots</t>
+  </si>
+  <si>
+    <t>738.9 MW</t>
+  </si>
+  <si>
+    <t>-738.9 MW</t>
+  </si>
+  <si>
+    <t>3.78 Hours</t>
+  </si>
+  <si>
+    <t>Mk3 Miner</t>
+  </si>
+  <si>
+    <t>Obelisks Of Alara Miner</t>
+  </si>
+  <si>
+    <t>Supercomputer</t>
+  </si>
+  <si>
+    <t>Versatile Framework</t>
+  </si>
+  <si>
+    <t>Automated Wiring</t>
+  </si>
+  <si>
+    <t>Assembly Director System</t>
+  </si>
+  <si>
+    <t>Electromagnetic Control Rods</t>
+  </si>
+  <si>
+    <t>Magnetic Field Generator</t>
   </si>
 </sst>
 </file>
@@ -815,7 +855,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1122,141 +1162,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1302,45 +1207,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1374,6 +1240,55 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1510,6 +1425,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1525,58 +1443,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1915,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="B2:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1934,18 +1843,18 @@
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="35" t="s">
@@ -2014,7 +1923,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="11">
-        <v>1849.848</v>
+        <v>1837.835</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>42</v>
@@ -2094,10 +2003,10 @@
         <v>5</v>
       </c>
       <c r="D12" s="11">
-        <v>391.64166599999999</v>
+        <v>345.64157</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>67</v>
@@ -2154,7 +2063,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="11">
-        <v>226.25</v>
+        <v>197.65</v>
       </c>
       <c r="E15" s="41" t="s">
         <v>131</v>
@@ -2194,7 +2103,7 @@
         <v>54</v>
       </c>
       <c r="D17" s="11">
-        <v>777.33299999999997</v>
+        <v>667.32330000000002</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>55</v>
@@ -2217,7 +2126,7 @@
         <v>1965</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>73</v>
@@ -2536,7 +2445,7 @@
         <v>158</v>
       </c>
       <c r="I41" s="57">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="J41" s="41" t="s">
         <v>151</v>
@@ -2610,7 +2519,7 @@
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.35">
       <c r="H48" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I48" s="58">
         <v>2</v>
@@ -2621,7 +2530,7 @@
     </row>
     <row r="49" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H49" s="39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I49" s="58">
         <v>2</v>
@@ -2632,7 +2541,7 @@
     </row>
     <row r="50" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H50" s="39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I50" s="58">
         <v>2</v>
@@ -2643,7 +2552,7 @@
     </row>
     <row r="51" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H51" s="39" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I51" s="58">
         <v>5</v>
@@ -2654,7 +2563,7 @@
     </row>
     <row r="52" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H52" s="39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I52" s="58">
         <v>5</v>
@@ -2665,7 +2574,7 @@
     </row>
     <row r="53" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H53" s="39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I53" s="58">
         <v>5</v>
@@ -2676,7 +2585,7 @@
     </row>
     <row r="54" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H54" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I54" s="58">
         <v>5</v>
@@ -2687,7 +2596,7 @@
     </row>
     <row r="55" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H55" s="39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I55" s="57">
         <v>5</v>
@@ -2698,7 +2607,7 @@
     </row>
     <row r="56" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H56" s="39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I56" s="57">
         <v>5</v>
@@ -2709,7 +2618,7 @@
     </row>
     <row r="57" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H57" s="39" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I57" s="57">
         <v>5</v>
@@ -2720,7 +2629,7 @@
     </row>
     <row r="58" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H58" s="39" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I58" s="57">
         <v>5</v>
@@ -2731,7 +2640,7 @@
     </row>
     <row r="59" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H59" s="39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I59" s="57">
         <v>5</v>
@@ -2742,7 +2651,7 @@
     </row>
     <row r="60" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H60" s="39" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I60" s="57">
         <v>5</v>
@@ -2753,7 +2662,7 @@
     </row>
     <row r="61" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H61" s="39" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I61" s="57">
         <v>11.41666</v>
@@ -2767,105 +2676,136 @@
         <v>53</v>
       </c>
       <c r="I62" s="57">
-        <v>12.067</v>
+        <v>7.0670000000000002</v>
       </c>
       <c r="J62" s="41" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H63" s="39" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I63" s="58">
         <v>5</v>
       </c>
       <c r="J63" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H64" s="39" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="I64" s="58">
         <v>2.5</v>
       </c>
       <c r="J64" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.35">
       <c r="H65" s="39" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I65" s="58">
         <v>2</v>
       </c>
       <c r="J65" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.35">
       <c r="H66" s="39" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I66" s="58">
         <v>2</v>
       </c>
       <c r="J66" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.35">
       <c r="H67" s="39" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I67" s="58">
         <v>2</v>
       </c>
       <c r="J67" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C68" s="1"/>
       <c r="H68" s="39" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="I68" s="58">
         <v>1</v>
       </c>
       <c r="J68" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C69" s="1"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="57"/>
-      <c r="J69" s="41"/>
+      <c r="H69" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="I69" s="8">
+        <f>5/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C70" s="1"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="57"/>
-      <c r="J70" s="41"/>
+      <c r="H70" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="I70" s="9">
+        <v>1</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H71" s="2"/>
-      <c r="I71" s="57"/>
-      <c r="J71" s="41"/>
+      <c r="H71" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="I71" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="72" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H72" s="2"/>
-      <c r="I72" s="57"/>
-      <c r="J72" s="41"/>
+      <c r="H72" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="I72" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="73" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H73" s="2"/>
-      <c r="I73" s="57"/>
-      <c r="J73" s="41"/>
+      <c r="H73" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="I73" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.35">
       <c r="H74" s="2"/>
@@ -3087,16 +3027,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -3508,7 +3448,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
@@ -3553,17 +3493,17 @@
     </row>
     <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -3610,14 +3550,14 @@
         <v>8</v>
       </c>
       <c r="M12" s="19"/>
-      <c r="O12" s="63" t="s">
+      <c r="O12" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
+      <c r="S12" s="66"/>
+      <c r="T12" s="66"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -3640,12 +3580,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="63"/>
-      <c r="R13" s="63"/>
-      <c r="S13" s="63"/>
-      <c r="T13" s="63"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -3662,12 +3602,12 @@
         <v>25</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="63"/>
-      <c r="T14" s="63"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -3684,12 +3624,12 @@
         <v>8</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="63"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -3706,14 +3646,14 @@
         <v>111</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="O16" s="63" t="s">
+      <c r="O16" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="63"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -3730,12 +3670,12 @@
         <v>111</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="63"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="63"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -3752,12 +3692,12 @@
         <v>151</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="63"/>
-      <c r="S18" s="63"/>
-      <c r="T18" s="63"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -3774,12 +3714,12 @@
         <v>151</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
-      <c r="Q19" s="63"/>
-      <c r="R19" s="63"/>
-      <c r="S19" s="63"/>
-      <c r="T19" s="63"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -3809,17 +3749,17 @@
         <v>109.5</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="O21" s="64" t="s">
+      <c r="O21" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
+      <c r="T21" s="67"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -3840,14 +3780,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="4"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="63"/>
+      <c r="O23" s="66" t="s">
+        <v>217</v>
+      </c>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -3858,12 +3798,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="4"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -3874,12 +3814,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="63"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="66"/>
+      <c r="T25" s="66"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -3890,12 +3830,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="63"/>
-      <c r="T26" s="63"/>
+      <c r="O26" s="66"/>
+      <c r="P26" s="66"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="66"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="66"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -3906,14 +3846,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="63" t="s">
+      <c r="O27" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="63"/>
-      <c r="T27" s="63"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="66"/>
+      <c r="R27" s="66"/>
+      <c r="S27" s="66"/>
+      <c r="T27" s="66"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -3924,12 +3864,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="63"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="63"/>
-      <c r="S28" s="63"/>
-      <c r="T28" s="63"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -3940,12 +3880,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="63"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="63"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="66"/>
+      <c r="T29" s="66"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -3956,12 +3896,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="63"/>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="63"/>
-      <c r="R30" s="63"/>
-      <c r="S30" s="63"/>
-      <c r="T30" s="63"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -4114,7 +4054,7 @@
   <dimension ref="B1:L44"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4152,7 +4092,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -4197,16 +4137,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -4364,7 +4304,7 @@
         <v>87</v>
       </c>
       <c r="K18" s="11">
-        <v>226.25</v>
+        <v>197.65</v>
       </c>
       <c r="L18" s="42" t="s">
         <v>25</v>
@@ -4442,7 +4382,7 @@
         <v>176.4</v>
       </c>
       <c r="L23" s="42" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.35">
@@ -4450,9 +4390,15 @@
       <c r="E24" s="2"/>
       <c r="F24" s="9"/>
       <c r="G24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="42"/>
+      <c r="J24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="11">
+        <v>28.6</v>
+      </c>
+      <c r="L24" s="42" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -4640,7 +4586,7 @@
   <dimension ref="B1:L44"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L44"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4677,7 +4623,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>27</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -4722,16 +4668,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -4766,7 +4712,7 @@
         <v>134</v>
       </c>
       <c r="J12" s="38">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>158</v>
@@ -4807,9 +4753,15 @@
       <c r="G14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="38"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="4"/>
+      <c r="J14" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -5154,7 +5106,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -5199,16 +5151,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -5333,7 +5285,7 @@
         <v>175</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
@@ -5597,10 +5549,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C186B3A-157D-4021-977B-A5A4DB537283}">
-  <dimension ref="D3:N28"/>
+  <dimension ref="D3:N29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5629,7 +5581,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.35">
@@ -5637,7 +5589,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>27</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.35">
@@ -5651,7 +5603,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.35">
@@ -5659,7 +5611,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.35">
@@ -5700,13 +5652,13 @@
       <c r="I13" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="53" t="s">
+      <c r="L13" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="N13" s="55" t="s">
+      <c r="N13" s="62" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5720,13 +5672,13 @@
       <c r="I14" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="47">
         <v>2</v>
       </c>
-      <c r="M14" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="N14" s="42" t="s">
+      <c r="M14" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="N14" s="40" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5744,7 +5696,7 @@
         <v>2</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N15" s="41" t="s">
         <v>8</v>
@@ -5764,7 +5716,7 @@
         <v>2</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N16" s="41" t="s">
         <v>8</v>
@@ -5784,7 +5736,7 @@
         <v>5</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N17" s="41" t="s">
         <v>8</v>
@@ -5804,7 +5756,7 @@
         <v>5</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N18" s="41" t="s">
         <v>8</v>
@@ -5824,7 +5776,7 @@
         <v>5</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N19" s="41" t="s">
         <v>8</v>
@@ -5838,13 +5790,13 @@
         <v>30.4666</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L20" s="6">
         <v>5</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N20" s="41" t="s">
         <v>8</v>
@@ -5858,13 +5810,13 @@
         <v>30.4666</v>
       </c>
       <c r="I21" s="41" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L21" s="6">
         <v>5</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N21" s="41" t="s">
         <v>8</v>
@@ -5884,7 +5836,7 @@
         <v>5</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N22" s="41" t="s">
         <v>8</v>
@@ -5904,7 +5856,7 @@
         <v>5</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N23" s="41" t="s">
         <v>8</v>
@@ -5924,7 +5876,7 @@
         <v>5</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N24" s="41" t="s">
         <v>8</v>
@@ -5935,7 +5887,7 @@
         <v>5</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N25" s="41" t="s">
         <v>8</v>
@@ -5946,7 +5898,7 @@
         <v>5</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N26" s="41" t="s">
         <v>8</v>
@@ -5957,20 +5909,32 @@
         <v>11.41666</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N27" s="41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L28" s="7">
-        <v>391.64166599999999</v>
-      </c>
-      <c r="M28" s="3" t="s">
+    <row r="28" spans="7:14" x14ac:dyDescent="0.35">
+      <c r="L28" s="6">
+        <v>46</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N28" s="43" t="s">
+      <c r="N28" s="41" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L29" s="7">
+        <f>391.64167-46</f>
+        <v>345.64166999999998</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N29" s="43" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6010,7 +5974,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
@@ -6026,7 +5990,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
@@ -6034,7 +5998,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
@@ -6042,7 +6006,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
@@ -6050,7 +6014,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
@@ -6058,7 +6022,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6066,21 +6030,21 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6142,10 +6106,10 @@
         <v>137</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="N13" s="49" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="O13" s="14" t="s">
         <v>25</v>
@@ -6181,7 +6145,7 @@
         <v>180</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="9"/>
@@ -6259,7 +6223,7 @@
         <v>180</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="9"/>
@@ -6495,8 +6459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E188AE-32E3-44FC-A747-B6B7B3960AE2}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:L17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6517,7 +6481,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
@@ -6525,7 +6489,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -6545,7 +6509,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -6553,7 +6517,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -6561,7 +6525,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6569,21 +6533,21 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6609,7 +6573,7 @@
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C12" s="23"/>
       <c r="E12" s="4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F12" s="8">
         <v>485.50555000000003</v>
@@ -6621,7 +6585,7 @@
         <v>5</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>8</v>
@@ -6642,7 +6606,7 @@
         <v>2.5</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>8</v>
@@ -6663,7 +6627,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>8</v>
@@ -6684,7 +6648,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>8</v>
@@ -6693,7 +6657,7 @@
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
       <c r="E16" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F16" s="9">
         <v>72</v>
@@ -6705,7 +6669,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>8</v>
@@ -6726,7 +6690,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>8</v>
@@ -6735,13 +6699,13 @@
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
       <c r="E18" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F18" s="9">
         <v>392.66660000000002</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="J18" s="38"/>
       <c r="K18" s="9"/>
@@ -6765,7 +6729,7 @@
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
       <c r="E20" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F20" s="9">
         <v>72</v>
@@ -6780,13 +6744,13 @@
     <row r="21" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
       <c r="E21" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F21" s="9">
         <v>515</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="9"/>
@@ -6803,6 +6767,504 @@
       <c r="G22" s="2" t="s">
         <v>165</v>
       </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="23"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="23"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="2"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="23"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="23"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="2"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="23"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="2"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="23"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="23"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="2"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="23"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="2"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="23"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="23"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="23"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="23"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="23"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="2"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="23"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="J10:L10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2B3A23-66AC-4695-AC89-14BEBEA38B1D}">
+  <dimension ref="B1:L44"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="23"/>
+      <c r="E10" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="23"/>
+      <c r="E11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="23"/>
+      <c r="E12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="8">
+        <v>12.0138</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="K12" s="8">
+        <f>5/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="23"/>
+      <c r="E13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="9">
+        <v>138.01249999999999</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="K13" s="9">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="23"/>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="9">
+        <v>98.243700000000004</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="23"/>
+      <c r="E15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="9">
+        <v>28.6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="K15" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="23"/>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="9">
+        <v>209.1062</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="23"/>
+      <c r="E17" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1.3887999999999999E-2</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="38"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="23"/>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="9">
+        <v>46</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="38"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="23"/>
+      <c r="E19" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F19" s="9">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="23"/>
+      <c r="E20" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="23"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="23"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="2"/>
       <c r="J22" s="11"/>
       <c r="K22" s="9"/>
       <c r="L22" s="4"/>
@@ -7034,16 +7496,16 @@
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="62"/>
-      <c r="K4" s="60" t="s">
+      <c r="G4" s="64"/>
+      <c r="H4" s="65"/>
+      <c r="K4" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="61"/>
-      <c r="M4" s="62"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="17" t="s">
@@ -7420,8 +7882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A244D34F-6552-48EC-88C9-9BCAF12F75CF}">
   <dimension ref="C3:U1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7434,7 +7896,7 @@
     <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7455,12 +7917,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:21" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:21" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="29" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.35">
@@ -7505,17 +7967,17 @@
     </row>
     <row r="12" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="60" t="s">
+      <c r="F13" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="62"/>
-      <c r="K13" s="60" t="s">
+      <c r="G13" s="64"/>
+      <c r="H13" s="65"/>
+      <c r="K13" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="62"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="65"/>
     </row>
     <row r="14" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="14" t="s">
@@ -7539,14 +8001,14 @@
       <c r="N14" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="P14" s="63" t="s">
+      <c r="P14" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="63"/>
-      <c r="T14" s="63"/>
-      <c r="U14" s="63"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
+      <c r="U14" s="66"/>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
@@ -7562,18 +8024,18 @@
         <v>35</v>
       </c>
       <c r="L15" s="8">
-        <v>1849.848</v>
+        <v>1837.835</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="N15" s="19"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="63"/>
-      <c r="U15" s="63"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
@@ -7597,12 +8059,12 @@
       <c r="N16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="63"/>
-      <c r="U16" s="63"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
     </row>
     <row r="17" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
@@ -7620,12 +8082,12 @@
       <c r="N17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="63"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="63"/>
-      <c r="U17" s="63"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
+      <c r="U17" s="66"/>
     </row>
     <row r="18" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
@@ -7675,22 +8137,28 @@
         <v>177</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="P20" s="64" t="s">
+      <c r="P20" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="64"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="67"/>
+      <c r="U20" s="67"/>
     </row>
     <row r="21" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="G21" s="9"/>
       <c r="H21" s="2"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="2"/>
+      <c r="K21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="9">
+        <v>12.013</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="6:21" x14ac:dyDescent="0.35">
@@ -7701,14 +8169,14 @@
       <c r="L22" s="9"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="P22" s="63" t="s">
+      <c r="P22" s="66" t="s">
         <v>180</v>
       </c>
-      <c r="Q22" s="63"/>
-      <c r="R22" s="63"/>
-      <c r="S22" s="63"/>
-      <c r="T22" s="63"/>
-      <c r="U22" s="63"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
     </row>
     <row r="23" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
@@ -7718,12 +8186,12 @@
       <c r="L23" s="9"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="63"/>
-      <c r="U23" s="63"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
     </row>
     <row r="24" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
@@ -7733,12 +8201,12 @@
       <c r="L24" s="9"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
-      <c r="U24" s="63"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
+      <c r="U24" s="66"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
@@ -7748,12 +8216,12 @@
       <c r="L25" s="9"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="63"/>
-      <c r="U25" s="63"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="66"/>
+      <c r="T25" s="66"/>
+      <c r="U25" s="66"/>
     </row>
     <row r="26" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
@@ -7763,14 +8231,14 @@
       <c r="L26" s="9"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="P26" s="63" t="s">
+      <c r="P26" s="66" t="s">
         <v>181</v>
       </c>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="63"/>
-      <c r="T26" s="63"/>
-      <c r="U26" s="63"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="66"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="66"/>
+      <c r="U26" s="66"/>
     </row>
     <row r="27" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
@@ -7780,12 +8248,12 @@
       <c r="L27" s="9"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="63"/>
-      <c r="T27" s="63"/>
-      <c r="U27" s="63"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="66"/>
+      <c r="R27" s="66"/>
+      <c r="S27" s="66"/>
+      <c r="T27" s="66"/>
+      <c r="U27" s="66"/>
     </row>
     <row r="28" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
@@ -7795,12 +8263,12 @@
       <c r="L28" s="9"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="P28" s="63"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="63"/>
-      <c r="S28" s="63"/>
-      <c r="T28" s="63"/>
-      <c r="U28" s="63"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
     </row>
     <row r="29" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
@@ -7810,12 +8278,12 @@
       <c r="L29" s="9"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="63"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="63"/>
-      <c r="U29" s="63"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="66"/>
+      <c r="T29" s="66"/>
+      <c r="U29" s="66"/>
     </row>
     <row r="30" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
@@ -7825,14 +8293,14 @@
       <c r="L30" s="9"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="P30" s="63" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q30" s="63"/>
-      <c r="R30" s="63"/>
-      <c r="S30" s="63"/>
-      <c r="T30" s="63"/>
-      <c r="U30" s="63"/>
+      <c r="P30" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
     </row>
     <row r="31" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
@@ -7842,12 +8310,12 @@
       <c r="L31" s="9"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="63"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="63"/>
-      <c r="U31" s="63"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="66"/>
+      <c r="U31" s="66"/>
     </row>
     <row r="32" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
@@ -7857,12 +8325,12 @@
       <c r="L32" s="9"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="63"/>
-      <c r="U32" s="63"/>
+      <c r="P32" s="66"/>
+      <c r="Q32" s="66"/>
+      <c r="R32" s="66"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="66"/>
+      <c r="U32" s="66"/>
     </row>
     <row r="33" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
@@ -7872,12 +8340,12 @@
       <c r="L33" s="9"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="63"/>
-      <c r="U33" s="63"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="66"/>
+      <c r="S33" s="66"/>
+      <c r="T33" s="66"/>
+      <c r="U33" s="66"/>
     </row>
     <row r="34" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
@@ -8027,7 +8495,7 @@
   <dimension ref="B1:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8065,7 +8533,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -8113,16 +8581,16 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-      <c r="J11" s="60" t="s">
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="J11" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="61"/>
-      <c r="L11" s="62"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -8160,7 +8628,7 @@
         <v>53</v>
       </c>
       <c r="K13" s="8">
-        <v>12.067</v>
+        <v>7.0670000000000002</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>8</v>
@@ -8244,7 +8712,7 @@
         <v>72</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.35">
@@ -8252,9 +8720,15 @@
       <c r="E19" s="2"/>
       <c r="F19" s="9"/>
       <c r="G19" s="2"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="2"/>
+      <c r="J19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="9">
+        <v>5</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -8483,7 +8957,7 @@
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.35">
       <c r="O48" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -8588,17 +9062,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-      <c r="J11" s="60" t="s">
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="J11" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="62"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="65"/>
     </row>
     <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -8623,14 +9097,14 @@
       <c r="M12" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O12" s="63" t="s">
+      <c r="O12" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
+      <c r="S12" s="66"/>
+      <c r="T12" s="66"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -8654,12 +9128,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="63"/>
-      <c r="R13" s="63"/>
-      <c r="S13" s="63"/>
-      <c r="T13" s="63"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -8684,12 +9158,12 @@
       <c r="M14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="63"/>
-      <c r="T14" s="63"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -8708,12 +9182,12 @@
       <c r="M15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="63"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -8732,14 +9206,14 @@
       <c r="M16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O16" s="63" t="s">
+      <c r="O16" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="63"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -8758,12 +9232,12 @@
       <c r="M17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="63"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="63"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -8780,12 +9254,12 @@
         <v>151</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="63"/>
-      <c r="S18" s="63"/>
-      <c r="T18" s="63"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -8802,12 +9276,12 @@
         <v>177</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
-      <c r="Q19" s="63"/>
-      <c r="R19" s="63"/>
-      <c r="S19" s="63"/>
-      <c r="T19" s="63"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
     </row>
     <row r="20" spans="3:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -8828,14 +9302,14 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="64" t="s">
+      <c r="O21" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
+      <c r="T21" s="67"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -8856,14 +9330,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="63" t="s">
+      <c r="O23" s="66" t="s">
         <v>178</v>
       </c>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="63"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -8874,12 +9348,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -8890,12 +9364,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="63"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="66"/>
+      <c r="T25" s="66"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -8906,12 +9380,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="6"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="63"/>
-      <c r="T26" s="63"/>
+      <c r="O26" s="66"/>
+      <c r="P26" s="66"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="66"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="66"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -8922,14 +9396,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="6"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="63" t="s">
+      <c r="O27" s="66" t="s">
         <v>154</v>
       </c>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="63"/>
-      <c r="T27" s="63"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="66"/>
+      <c r="R27" s="66"/>
+      <c r="S27" s="66"/>
+      <c r="T27" s="66"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -8940,12 +9414,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="6"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="63"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="63"/>
-      <c r="S28" s="63"/>
-      <c r="T28" s="63"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -8956,12 +9430,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="6"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="63"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="63"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="66"/>
+      <c r="T29" s="66"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -8972,12 +9446,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="6"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="63"/>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="63"/>
-      <c r="R30" s="63"/>
-      <c r="S30" s="63"/>
-      <c r="T30" s="63"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -8988,14 +9462,14 @@
       <c r="K31" s="9"/>
       <c r="L31" s="6"/>
       <c r="M31" s="2"/>
-      <c r="O31" s="63" t="s">
+      <c r="O31" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="63"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="63"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="66"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -9006,12 +9480,12 @@
       <c r="K32" s="9"/>
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="63"/>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
+      <c r="Q32" s="66"/>
+      <c r="R32" s="66"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="66"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C33" s="23"/>
@@ -9022,12 +9496,12 @@
       <c r="K33" s="9"/>
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="63"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="66"/>
+      <c r="S33" s="66"/>
+      <c r="T33" s="66"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C34" s="23"/>
@@ -9038,12 +9512,12 @@
       <c r="K34" s="9"/>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
-      <c r="O34" s="63"/>
-      <c r="P34" s="63"/>
-      <c r="Q34" s="63"/>
-      <c r="R34" s="63"/>
-      <c r="S34" s="63"/>
-      <c r="T34" s="63"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="66"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C35" s="23"/>
@@ -9163,108 +9637,48 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9AFFE6-32CC-4ED3-90D1-1E871DB3E098}">
-  <dimension ref="B1:S36"/>
+  <dimension ref="B1:S45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.08984375" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" customWidth="1"/>
     <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="J2" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
-    </row>
-    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+    </row>
+    <row r="4" spans="2:19" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="8">
-        <v>960</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="8">
-        <v>777.33299999999997</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
+      <c r="C4" s="30" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
@@ -9273,30 +9687,6 @@
       <c r="C5" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="9">
-        <v>960</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="9">
-        <v>300</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -9305,24 +9695,6 @@
       <c r="C6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="2"/>
-      <c r="J6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="9">
-        <v>392.666</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
@@ -9331,12 +9703,6 @@
       <c r="C7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="2"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
@@ -9345,12 +9711,6 @@
       <c r="C8" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="2"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="22" t="s">
@@ -9359,152 +9719,178 @@
       <c r="C9" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="2"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="2"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="2"/>
-      <c r="N10" s="74" t="s">
-        <v>150</v>
-      </c>
-      <c r="O10" s="75"/>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
-      <c r="S10" s="76"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="2"/>
-      <c r="N11" s="77" t="s">
-        <v>212</v>
-      </c>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="78"/>
-      <c r="S11" s="79"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="E11" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="J11" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
+    </row>
+    <row r="12" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="2"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
-      <c r="S12" s="70"/>
-    </row>
-    <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
+      <c r="S12" s="66"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="2"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="72"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="73"/>
+      <c r="E13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="8">
+        <v>960</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="8">
+        <v>667.32330000000002</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="2"/>
-      <c r="N14" s="65" t="s">
-        <v>211</v>
-      </c>
+      <c r="E14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="9">
+        <v>960</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="9">
+        <v>300</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N14" s="66"/>
       <c r="O14" s="66"/>
       <c r="P14" s="66"/>
       <c r="Q14" s="66"/>
       <c r="R14" s="66"/>
-      <c r="S14" s="67"/>
+      <c r="S14" s="66"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
       <c r="E15" s="2"/>
       <c r="F15" s="9"/>
       <c r="G15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="2"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="70"/>
-    </row>
-    <row r="16" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="9">
+        <v>392.666</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
       <c r="E16" s="2"/>
       <c r="F16" s="9"/>
       <c r="G16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="2"/>
-      <c r="N16" s="71"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="73"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="J16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="9">
+        <v>110.01</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
       <c r="E17" s="2"/>
       <c r="F17" s="9"/>
       <c r="G17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="9"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="23"/>
       <c r="E18" s="2"/>
       <c r="F18" s="9"/>
       <c r="G18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="4"/>
       <c r="K18" s="9"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="23"/>
       <c r="E19" s="2"/>
       <c r="F19" s="9"/>
       <c r="G19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="4"/>
       <c r="K19" s="9"/>
       <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N19" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78"/>
+      <c r="S19" s="79"/>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
       <c r="E20" s="2"/>
       <c r="F20" s="9"/>
@@ -9512,8 +9898,16 @@
       <c r="J20" s="2"/>
       <c r="K20" s="9"/>
       <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N20" s="68" t="s">
+        <v>208</v>
+      </c>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="70"/>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
       <c r="E21" s="2"/>
       <c r="F21" s="9"/>
@@ -9521,8 +9915,14 @@
       <c r="J21" s="2"/>
       <c r="K21" s="9"/>
       <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N21" s="71"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="73"/>
+    </row>
+    <row r="22" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="23"/>
       <c r="E22" s="2"/>
       <c r="F22" s="9"/>
@@ -9530,8 +9930,14 @@
       <c r="J22" s="2"/>
       <c r="K22" s="9"/>
       <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N22" s="74"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="76"/>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
       <c r="E23" s="2"/>
       <c r="F23" s="9"/>
@@ -9539,8 +9945,16 @@
       <c r="J23" s="2"/>
       <c r="K23" s="9"/>
       <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N23" s="68" t="s">
+        <v>242</v>
+      </c>
+      <c r="O23" s="69"/>
+      <c r="P23" s="69"/>
+      <c r="Q23" s="69"/>
+      <c r="R23" s="69"/>
+      <c r="S23" s="70"/>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
       <c r="E24" s="2"/>
       <c r="F24" s="9"/>
@@ -9548,8 +9962,14 @@
       <c r="J24" s="2"/>
       <c r="K24" s="9"/>
       <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N24" s="71"/>
+      <c r="O24" s="72"/>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="72"/>
+      <c r="R24" s="72"/>
+      <c r="S24" s="73"/>
+    </row>
+    <row r="25" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="23"/>
       <c r="E25" s="2"/>
       <c r="F25" s="9"/>
@@ -9557,8 +9977,14 @@
       <c r="J25" s="2"/>
       <c r="K25" s="9"/>
       <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N25" s="74"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="76"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
       <c r="E26" s="2"/>
       <c r="F26" s="9"/>
@@ -9567,7 +9993,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
       <c r="E27" s="2"/>
       <c r="F27" s="9"/>
@@ -9576,7 +10002,7 @@
       <c r="K27" s="9"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
       <c r="E28" s="2"/>
       <c r="F28" s="9"/>
@@ -9585,7 +10011,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
       <c r="E29" s="2"/>
       <c r="F29" s="9"/>
@@ -9594,7 +10020,7 @@
       <c r="K29" s="9"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
       <c r="E30" s="2"/>
       <c r="F30" s="9"/>
@@ -9603,7 +10029,7 @@
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
       <c r="E31" s="2"/>
       <c r="F31" s="9"/>
@@ -9612,7 +10038,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
       <c r="E32" s="2"/>
       <c r="F32" s="9"/>
@@ -9648,23 +10074,95 @@
       <c r="K35" s="9"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="3"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E37" s="2"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E38" s="2"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E39" s="2"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E44" s="2"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E45" s="3"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="N14:S16"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N3:S6"/>
-    <mergeCell ref="N10:S10"/>
-    <mergeCell ref="N11:S13"/>
+    <mergeCell ref="N20:S22"/>
+    <mergeCell ref="N23:S25"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="N12:S15"/>
+    <mergeCell ref="N19:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9728,7 +10226,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -9736,7 +10234,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -9752,21 +10250,21 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -10278,7 +10776,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
@@ -10323,16 +10821,16 @@
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -10396,14 +10894,14 @@
       <c r="L13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="63" t="s">
+      <c r="N13" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="63"/>
-      <c r="R13" s="63"/>
-      <c r="S13" s="63"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -10425,12 +10923,12 @@
       <c r="L14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="63"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -10446,12 +10944,12 @@
       <c r="L15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="63"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="63"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
     </row>
     <row r="16" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -10467,12 +10965,12 @@
       <c r="L16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="63"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
     </row>
     <row r="17" spans="3:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -10488,14 +10986,14 @@
       <c r="L17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N17" s="63" t="s">
+      <c r="N17" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="63"/>
-      <c r="S17" s="63"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -10511,12 +11009,12 @@
       <c r="L18" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N18" s="63"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="63"/>
-      <c r="S18" s="63"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -10532,12 +11030,12 @@
       <c r="L19" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N19" s="63"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
-      <c r="Q19" s="63"/>
-      <c r="R19" s="63"/>
-      <c r="S19" s="63"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -10553,12 +11051,12 @@
       <c r="L20" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="N20" s="63"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="63"/>
-      <c r="S20" s="63"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="66"/>
+      <c r="R20" s="66"/>
+      <c r="S20" s="66"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -10572,7 +11070,7 @@
         <v>72</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.35">
@@ -10583,14 +11081,14 @@
       <c r="J22" s="2"/>
       <c r="K22" s="9"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="64" t="s">
+      <c r="N22" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="O22" s="64"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -10609,14 +11107,14 @@
       <c r="J24" s="2"/>
       <c r="K24" s="9"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
+      <c r="N24" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="66"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -10626,12 +11124,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="66"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -10641,12 +11139,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
-      <c r="N26" s="63"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="63"/>
+      <c r="N26" s="66"/>
+      <c r="O26" s="66"/>
+      <c r="P26" s="66"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="66"/>
+      <c r="S26" s="66"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -10656,12 +11154,12 @@
       <c r="J27" s="2"/>
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="63"/>
+      <c r="N27" s="66"/>
+      <c r="O27" s="66"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="66"/>
+      <c r="R27" s="66"/>
+      <c r="S27" s="66"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -10671,14 +11169,14 @@
       <c r="J28" s="2"/>
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="63" t="s">
+      <c r="N28" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="O28" s="63"/>
-      <c r="P28" s="63"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="63"/>
-      <c r="S28" s="63"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="66"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -10688,12 +11186,12 @@
       <c r="J29" s="2"/>
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="63"/>
-      <c r="S29" s="63"/>
+      <c r="N29" s="66"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="66"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -10703,12 +11201,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="63"/>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="63"/>
-      <c r="R30" s="63"/>
-      <c r="S30" s="63"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -10718,12 +11216,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="9"/>
       <c r="L31" s="2"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="63"/>
-      <c r="S31" s="63"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="66"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -10935,16 +11433,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>

</xml_diff>

<commit_message>
Added some blueprints and the savegame
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Simic Subline\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Ydris Nexus\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80036F8-AC63-47C1-B3AE-4D74C9D6BE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771AC292-EB9A-4299-BB47-4066EC7424C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49176" yWindow="696" windowWidth="12960" windowHeight="22248" firstSheet="12" activeTab="21" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="46992" yWindow="-3924" windowWidth="12960" windowHeight="22152" firstSheet="18" activeTab="19" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -1175,9 +1175,6 @@
     <t>945.7 MW</t>
   </si>
   <si>
-    <t>121734.4 MW</t>
-  </si>
-  <si>
     <t>4352.7 MW</t>
   </si>
   <si>
@@ -1211,9 +1208,6 @@
     <t>3100 MWh</t>
   </si>
   <si>
-    <t>17390.625 MW</t>
-  </si>
-  <si>
     <t>5530.95 MW</t>
   </si>
   <si>
@@ -1286,12 +1280,6 @@
     <t>Net Gain Unstable</t>
   </si>
   <si>
-    <t>107354.97 MW</t>
-  </si>
-  <si>
-    <t>11859.675 MW</t>
-  </si>
-  <si>
     <t>Simic Subline</t>
   </si>
   <si>
@@ -1350,6 +1338,18 @@
   </si>
   <si>
     <t>2.195 Hours</t>
+  </si>
+  <si>
+    <t>104343.75 MW</t>
+  </si>
+  <si>
+    <t>89964.35 MW</t>
+  </si>
+  <si>
+    <t>34781.25 MW</t>
+  </si>
+  <si>
+    <t>29250.3 MW</t>
   </si>
 </sst>
 </file>
@@ -2036,7 +2036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2307,10 +2307,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2647,7 +2643,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
-  <dimension ref="B2:R100"/>
+  <dimension ref="B2:P100"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R70" sqref="R70"/>
@@ -3741,7 +3737,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C81" s="1"/>
       <c r="H81" s="70" t="s">
         <v>346</v>
@@ -3753,7 +3749,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C82" s="1"/>
       <c r="H82" s="70" t="s">
         <v>347</v>
@@ -3765,7 +3761,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H83" s="39" t="s">
         <v>321</v>
       </c>
@@ -3775,13 +3771,8 @@
       <c r="J83" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="N83" s="126"/>
-      <c r="O83" s="126"/>
-      <c r="P83" s="126"/>
-      <c r="Q83" s="126"/>
-      <c r="R83" s="126"/>
-    </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H84" s="39" t="s">
         <v>319</v>
       </c>
@@ -3791,13 +3782,8 @@
       <c r="J84" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="N84" s="126"/>
-      <c r="O84" s="126"/>
-      <c r="P84" s="126"/>
-      <c r="Q84" s="126"/>
-      <c r="R84" s="126"/>
-    </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H85" s="39" t="s">
         <v>326</v>
       </c>
@@ -3807,13 +3793,8 @@
       <c r="J85" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="N85" s="126"/>
-      <c r="O85" s="126"/>
-      <c r="P85" s="126"/>
-      <c r="Q85" s="126"/>
-      <c r="R85" s="126"/>
-    </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H86" s="39" t="s">
         <v>349</v>
       </c>
@@ -3823,13 +3804,8 @@
       <c r="J86" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="N86" s="126"/>
-      <c r="O86" s="126"/>
-      <c r="P86" s="126"/>
-      <c r="Q86" s="126"/>
-      <c r="R86" s="126"/>
-    </row>
-    <row r="87" spans="2:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H87" s="39" t="s">
         <v>306</v>
       </c>
@@ -3839,13 +3815,9 @@
       <c r="J87" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="N87" s="126"/>
-      <c r="O87" s="126"/>
-      <c r="P87" s="127"/>
-      <c r="Q87" s="126"/>
-      <c r="R87" s="126"/>
-    </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="P87" s="1"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88"/>
@@ -3858,95 +3830,90 @@
       <c r="J88" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="N88" s="126"/>
-      <c r="O88" s="126"/>
-      <c r="P88" s="126"/>
-      <c r="Q88" s="126"/>
-      <c r="R88" s="126"/>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89"/>
       <c r="H89" s="70" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I89" s="8">
         <v>5</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90"/>
       <c r="H90" s="70" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I90" s="9">
         <v>1.75</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="91" spans="2:18" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91"/>
       <c r="H91" s="70" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I91" s="9">
         <v>2.91</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92"/>
       <c r="H92" s="70" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I92" s="9">
         <v>2.83</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H93" s="70" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I93" s="9">
         <f>'The Mirrodin Trigon'!K21</f>
         <v>777.18888888888887</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94"/>
       <c r="H94" s="4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="I94" s="8">
         <v>4</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="95" spans="2:18" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95"/>
@@ -3954,7 +3921,7 @@
       <c r="I95" s="56"/>
       <c r="J95" s="41"/>
     </row>
-    <row r="96" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96"/>
@@ -4502,7 +4469,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
@@ -4845,11 +4812,11 @@
         <v>14</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="M23" s="2"/>
       <c r="O23" s="98" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="P23" s="98"/>
       <c r="Q23" s="98"/>
@@ -5176,7 +5143,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -5184,7 +5151,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -5200,7 +5167,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5514,7 +5481,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="L27" s="42" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.35">
@@ -5713,7 +5680,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -5893,7 +5860,7 @@
         <v>155</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
@@ -6225,7 +6192,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -7214,7 +7181,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F6">
         <f>5800/4352.7</f>
@@ -7226,7 +7193,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
@@ -7403,7 +7370,7 @@
         <v>137</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N16" s="6">
         <v>3</v>
@@ -7747,7 +7714,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -7755,7 +7722,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -7771,7 +7738,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -8777,7 +8744,7 @@
         <v>242</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -9616,8 +9583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918F12F9-7E2B-4B86-8EBD-462FB980EA31}">
   <dimension ref="B1:AF95"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K21:K32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9677,7 +9644,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>372</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -9685,7 +9652,7 @@
         <v>240</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -9693,7 +9660,7 @@
         <v>241</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
@@ -9706,10 +9673,10 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>409</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
@@ -9717,7 +9684,7 @@
         <v>363</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>384</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
@@ -9725,15 +9692,15 @@
         <v>243</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>410</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
@@ -9741,7 +9708,7 @@
         <v>244</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12080,7 +12047,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -12088,7 +12055,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -12108,7 +12075,7 @@
         <v>240</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -12116,7 +12083,7 @@
         <v>241</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -12124,7 +12091,7 @@
         <v>242</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -12132,7 +12099,7 @@
         <v>243</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
@@ -12140,7 +12107,7 @@
         <v>244</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
@@ -12148,23 +12115,23 @@
         <v>245</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>388</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12224,7 +12191,7 @@
         <v>279</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K17" s="8">
         <v>5</v>
@@ -12236,7 +12203,7 @@
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
       <c r="E18" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F18" s="9">
         <v>3000</v>
@@ -12246,7 +12213,7 @@
       </c>
       <c r="H18" s="2"/>
       <c r="J18" s="38" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K18" s="9">
         <v>1.75</v>
@@ -12269,7 +12236,7 @@
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K19" s="9">
         <v>2.91</v>
@@ -12291,7 +12258,7 @@
       </c>
       <c r="H20" s="2"/>
       <c r="J20" s="38" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K20" s="9">
         <v>2.83</v>
@@ -12310,11 +12277,11 @@
         <v>21.837037037037035</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H21" s="2"/>
       <c r="J21" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K21" s="9">
         <f>857+17/90-K22</f>
@@ -12334,17 +12301,17 @@
         <v>543.62222222222226</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H22" s="2"/>
       <c r="J22" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K22" s="9">
         <v>80</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.35">
@@ -12619,8 +12586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9AD2B8-3E41-467A-948D-46D21324EAFF}">
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12642,7 +12609,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="87" x14ac:dyDescent="0.35">
@@ -12650,7 +12617,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -12670,7 +12637,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -12678,7 +12645,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -12686,7 +12653,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12694,7 +12661,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12723,7 +12690,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>0</v>
@@ -12748,7 +12715,7 @@
       </c>
       <c r="H13" s="94"/>
       <c r="J13" s="4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K13" s="8">
         <v>4</v>
@@ -12844,13 +12811,13 @@
     <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
       <c r="E19" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F19" s="9">
         <v>80</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H19" s="85"/>
       <c r="J19" s="4"/>
@@ -12886,7 +12853,7 @@
         <v>128.33333333333334</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H21" s="85"/>
       <c r="J21" s="2"/>
@@ -12903,7 +12870,7 @@
         <v>146.41333333333333</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H22" s="85"/>
       <c r="J22" s="2"/>
@@ -12920,7 +12887,7 @@
         <v>172.6</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H23" s="85"/>
       <c r="J23" s="2"/>
@@ -13196,7 +13163,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.35">
@@ -13494,7 +13461,7 @@
         <v>41.870370370370374</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N24" s="2"/>
       <c r="P24" s="98"/>
@@ -13516,10 +13483,10 @@
         <v>30.94650205761317</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="P25" s="98"/>
       <c r="Q25" s="98"/>
@@ -13599,7 +13566,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="P30" s="98" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="Q30" s="98"/>
       <c r="R30" s="98"/>
@@ -13838,7 +13805,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -14065,7 +14032,7 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.35">
@@ -15028,7 +14995,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
@@ -15296,13 +15263,13 @@
         <v>111.77777777777777</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>260</v>
       </c>
       <c r="O20" s="100" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="P20" s="101"/>
       <c r="Q20" s="101"/>
@@ -16206,7 +16173,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
@@ -16539,7 +16506,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="92" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.35">
@@ -16551,7 +16518,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="92"/>
       <c r="N24" s="98" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="O24" s="98"/>
       <c r="P24" s="98"/>

</xml_diff>

<commit_message>
Added some blueprints, updated spreadsheet and added the save game for part 2 of Aetherflux Reactor
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Ydris Nexus 4\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 2\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DA813C-5D9C-4C67-865B-356F36085470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FFF927-14C5-4C41-8267-B51B177D399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="15" activeTab="23" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="468">
   <si>
     <t>Item</t>
   </si>
@@ -1439,6 +1439,30 @@
   </si>
   <si>
     <t>Alien Power Matrix</t>
+  </si>
+  <si>
+    <t>Aetherflux Reactor</t>
+  </si>
+  <si>
+    <t>Tollarian Metldown, Jund Pyroclast</t>
+  </si>
+  <si>
+    <t>Net gain Stable</t>
+  </si>
+  <si>
+    <t>Net gain Unstable</t>
+  </si>
+  <si>
+    <t>Ficsonium Power plants</t>
+  </si>
+  <si>
+    <t>Plutonium Power Plants</t>
+  </si>
+  <si>
+    <t>Ficsonium Fuel Rods</t>
+  </si>
+  <si>
+    <t>Silica/Quartz Module</t>
   </si>
 </sst>
 </file>
@@ -2156,7 +2180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2337,6 +2361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2428,6 +2453,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2766,8 +2795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="B2:T116"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2785,18 +2814,18 @@
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="100" t="s">
+      <c r="H4" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="101"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
     </row>
     <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="35" t="s">
@@ -3128,14 +3157,14 @@
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C21" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="D21" s="11">
-        <v>4.95</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>255</v>
+      <c r="C21" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="D21" s="38">
+        <v>597</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>427</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>76</v>
@@ -3149,10 +3178,10 @@
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C22" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="D22" s="38">
-        <v>597</v>
+        <v>458</v>
+      </c>
+      <c r="D22" s="11">
+        <v>72.25</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>427</v>
@@ -3169,13 +3198,14 @@
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C23" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="D23" s="11">
-        <v>72.25</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>427</v>
+        <v>86</v>
+      </c>
+      <c r="D23" s="9">
+        <f>'Aetherflux Reactor'!K16</f>
+        <v>398.18666666666667</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>460</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>78</v>
@@ -3188,9 +3218,16 @@
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C24" s="6"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="9">
+        <f>'Aetherflux Reactor'!K17</f>
+        <v>537.22400000000005</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>460</v>
+      </c>
       <c r="H24" s="6" t="s">
         <v>79</v>
       </c>
@@ -3492,7 +3529,7 @@
       </c>
       <c r="I47" s="11">
         <f>'Jund Pyroclast'!J15</f>
-        <v>142.10999999999999</v>
+        <v>140.07999999999998</v>
       </c>
       <c r="J47" s="40" t="s">
         <v>162</v>
@@ -3969,13 +4006,14 @@
       <c r="C89" s="1"/>
       <c r="D89"/>
       <c r="H89" s="48" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="I89" s="11">
-        <v>5</v>
+        <f>7/75</f>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="J89" s="40" t="s">
-        <v>385</v>
+        <v>255</v>
       </c>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.35">
@@ -3983,10 +4021,10 @@
       <c r="C90" s="1"/>
       <c r="D90"/>
       <c r="H90" s="48" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I90" s="11">
-        <v>1.75</v>
+        <v>5</v>
       </c>
       <c r="J90" s="40" t="s">
         <v>385</v>
@@ -3997,10 +4035,10 @@
       <c r="C91" s="1"/>
       <c r="D91"/>
       <c r="H91" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I91" s="11">
-        <v>2.91</v>
+        <v>1.75</v>
       </c>
       <c r="J91" s="40" t="s">
         <v>385</v>
@@ -4011,10 +4049,10 @@
       <c r="C92" s="1"/>
       <c r="D92"/>
       <c r="H92" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I92" s="11">
-        <v>2.83</v>
+        <v>2.91</v>
       </c>
       <c r="J92" s="40" t="s">
         <v>385</v>
@@ -4022,11 +4060,10 @@
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H93" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I93" s="11">
-        <f>'The Mirrodin Trigon'!K21</f>
-        <v>777.18888888888887</v>
+        <v>2.83</v>
       </c>
       <c r="J93" s="40" t="s">
         <v>385</v>
@@ -4036,28 +4073,29 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94"/>
-      <c r="H94" s="6" t="s">
-        <v>422</v>
+      <c r="H94" s="48" t="s">
+        <v>397</v>
       </c>
       <c r="I94" s="11">
-        <v>4</v>
+        <f>'The Mirrodin Trigon'!K22</f>
+        <v>80</v>
       </c>
       <c r="J94" s="40" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
     </row>
     <row r="95" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95"/>
-      <c r="H95" s="4" t="s">
-        <v>365</v>
+      <c r="H95" s="6" t="s">
+        <v>422</v>
       </c>
       <c r="I95" s="11">
-        <v>13.2</v>
+        <v>4</v>
       </c>
       <c r="J95" s="40" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
     </row>
     <row r="96" spans="2:16" x14ac:dyDescent="0.35">
@@ -4065,10 +4103,10 @@
       <c r="C96" s="1"/>
       <c r="D96"/>
       <c r="H96" s="4" t="s">
-        <v>459</v>
+        <v>365</v>
       </c>
       <c r="I96" s="11">
-        <v>0.1</v>
+        <v>13.2</v>
       </c>
       <c r="J96" s="40" t="s">
         <v>427</v>
@@ -4079,11 +4117,10 @@
       <c r="C97" s="1"/>
       <c r="D97"/>
       <c r="H97" s="4" t="s">
-        <v>208</v>
+        <v>459</v>
       </c>
       <c r="I97" s="11">
-        <f>6+1/3</f>
-        <v>6.333333333333333</v>
+        <v>0.1</v>
       </c>
       <c r="J97" s="40" t="s">
         <v>427</v>
@@ -4094,10 +4131,11 @@
       <c r="C98" s="1"/>
       <c r="D98"/>
       <c r="H98" s="4" t="s">
-        <v>439</v>
+        <v>208</v>
       </c>
       <c r="I98" s="11">
-        <v>1</v>
+        <f>6+1/3</f>
+        <v>6.333333333333333</v>
       </c>
       <c r="J98" s="40" t="s">
         <v>427</v>
@@ -4107,73 +4145,122 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="40"/>
+      <c r="H99" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="I99" s="11">
+        <v>1</v>
+      </c>
+      <c r="J99" s="40" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="100" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100"/>
-      <c r="H100" s="6"/>
+      <c r="H100" s="6" t="s">
+        <v>366</v>
+      </c>
       <c r="I100" s="11"/>
       <c r="J100" s="40"/>
     </row>
     <row r="101" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H101" s="6"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="40"/>
+      <c r="H101" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="I101" s="8">
+        <f>364/1215</f>
+        <v>0.29958847736625516</v>
+      </c>
+      <c r="J101" s="4" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="102" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H102" s="6"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="40"/>
+      <c r="H102" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I102" s="9">
+        <v>5</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>460</v>
+      </c>
       <c r="T102" s="1"/>
     </row>
     <row r="103" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H103" s="6"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="40"/>
+      <c r="H103" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I103" s="9">
+        <f>8+1/3</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>460</v>
+      </c>
       <c r="T103" s="1"/>
     </row>
     <row r="104" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H104" s="6"/>
       <c r="I104" s="11"/>
       <c r="J104" s="40"/>
+      <c r="N104" s="132"/>
+      <c r="O104" s="133"/>
+      <c r="P104" s="132"/>
       <c r="T104" s="1"/>
     </row>
     <row r="105" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H105" s="6"/>
       <c r="I105" s="11"/>
       <c r="J105" s="40"/>
+      <c r="N105" s="132"/>
+      <c r="O105" s="133"/>
+      <c r="P105" s="132"/>
       <c r="T105" s="1"/>
     </row>
     <row r="106" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H106" s="6"/>
       <c r="I106" s="11"/>
       <c r="J106" s="40"/>
+      <c r="N106" s="132"/>
+      <c r="O106" s="133"/>
+      <c r="P106" s="132"/>
       <c r="T106" s="1"/>
     </row>
     <row r="107" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H107" s="6"/>
       <c r="I107" s="11"/>
       <c r="J107" s="40"/>
+      <c r="N107" s="132"/>
+      <c r="O107" s="133"/>
+      <c r="P107" s="132"/>
       <c r="T107" s="1"/>
     </row>
     <row r="108" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H108" s="6"/>
       <c r="I108" s="11"/>
       <c r="J108" s="40"/>
+      <c r="N108" s="132"/>
+      <c r="O108" s="133"/>
+      <c r="P108" s="132"/>
     </row>
     <row r="109" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H109" s="6"/>
       <c r="I109" s="11"/>
       <c r="J109" s="40"/>
+      <c r="N109" s="132"/>
+      <c r="O109" s="132"/>
+      <c r="P109" s="132"/>
     </row>
     <row r="110" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H110" s="6"/>
       <c r="I110" s="11"/>
       <c r="J110" s="40"/>
+      <c r="N110" s="132"/>
+      <c r="O110" s="132"/>
+      <c r="P110" s="132"/>
     </row>
     <row r="111" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H111" s="6"/>
@@ -4304,16 +4391,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -4770,17 +4857,17 @@
     </row>
     <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="103"/>
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -4827,14 +4914,14 @@
         <v>8</v>
       </c>
       <c r="M12" s="19"/>
-      <c r="O12" s="103" t="s">
+      <c r="O12" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="P12" s="103"/>
-      <c r="Q12" s="103"/>
-      <c r="R12" s="103"/>
-      <c r="S12" s="103"/>
-      <c r="T12" s="103"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="104"/>
+      <c r="T12" s="104"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -4858,12 +4945,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
-      <c r="S13" s="103"/>
-      <c r="T13" s="103"/>
+      <c r="O13" s="104"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -4880,12 +4967,12 @@
         <v>25</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="103"/>
-      <c r="T14" s="103"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -4902,12 +4989,12 @@
         <v>8</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="O15" s="103"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
-      <c r="S15" s="103"/>
-      <c r="T15" s="103"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
+      <c r="T15" s="104"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -4924,14 +5011,14 @@
         <v>111</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="O16" s="103" t="s">
+      <c r="O16" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
-      <c r="S16" s="103"/>
-      <c r="T16" s="103"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="104"/>
+      <c r="T16" s="104"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -4948,12 +5035,12 @@
         <v>111</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="O17" s="103"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
+      <c r="O17" s="104"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="104"/>
+      <c r="T17" s="104"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -4970,12 +5057,12 @@
         <v>148</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
-      <c r="S18" s="103"/>
-      <c r="T18" s="103"/>
+      <c r="O18" s="104"/>
+      <c r="P18" s="104"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="104"/>
+      <c r="S18" s="104"/>
+      <c r="T18" s="104"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -4992,12 +5079,12 @@
         <v>148</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="103"/>
-      <c r="R19" s="103"/>
-      <c r="S19" s="103"/>
-      <c r="T19" s="103"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="104"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104"/>
+      <c r="T19" s="104"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -5030,14 +5117,14 @@
         <v>203</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="O21" s="104" t="s">
+      <c r="O21" s="105" t="s">
         <v>147</v>
       </c>
-      <c r="P21" s="104"/>
-      <c r="Q21" s="104"/>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="104"/>
+      <c r="P21" s="105"/>
+      <c r="Q21" s="105"/>
+      <c r="R21" s="105"/>
+      <c r="S21" s="105"/>
+      <c r="T21" s="105"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -5071,14 +5158,14 @@
         <v>407</v>
       </c>
       <c r="M23" s="2"/>
-      <c r="O23" s="103" t="s">
+      <c r="O23" s="104" t="s">
         <v>408</v>
       </c>
-      <c r="P23" s="103"/>
-      <c r="Q23" s="103"/>
-      <c r="R23" s="103"/>
-      <c r="S23" s="103"/>
-      <c r="T23" s="103"/>
+      <c r="P23" s="104"/>
+      <c r="Q23" s="104"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="104"/>
+      <c r="T23" s="104"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -5089,12 +5176,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="4"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -5105,12 +5192,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="103"/>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="103"/>
-      <c r="T25" s="103"/>
+      <c r="O25" s="104"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104"/>
+      <c r="T25" s="104"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -5121,12 +5208,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="103"/>
-      <c r="P26" s="103"/>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
-      <c r="S26" s="103"/>
-      <c r="T26" s="103"/>
+      <c r="O26" s="104"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="104"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -5137,14 +5224,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="103" t="s">
+      <c r="O27" s="104" t="s">
         <v>149</v>
       </c>
-      <c r="P27" s="103"/>
-      <c r="Q27" s="103"/>
-      <c r="R27" s="103"/>
-      <c r="S27" s="103"/>
-      <c r="T27" s="103"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
+      <c r="T27" s="104"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -5155,12 +5242,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="103"/>
-      <c r="P28" s="103"/>
-      <c r="Q28" s="103"/>
-      <c r="R28" s="103"/>
-      <c r="S28" s="103"/>
-      <c r="T28" s="103"/>
+      <c r="O28" s="104"/>
+      <c r="P28" s="104"/>
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104"/>
+      <c r="T28" s="104"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -5171,12 +5258,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
-      <c r="T29" s="103"/>
+      <c r="O29" s="104"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
+      <c r="S29" s="104"/>
+      <c r="T29" s="104"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -5187,12 +5274,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
-      <c r="S30" s="103"/>
-      <c r="T30" s="103"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
+      <c r="S30" s="104"/>
+      <c r="T30" s="104"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -5428,16 +5515,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -5981,16 +6068,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6394,8 +6481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1051D7C-48A2-4264-A591-A5BE1589053B}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6477,16 +6564,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6585,7 +6672,7 @@
       </c>
       <c r="J15" s="38">
         <f>150-J16-J19</f>
-        <v>142.10999999999999</v>
+        <v>140.07999999999998</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>171</v>
@@ -6672,7 +6759,7 @@
         <v>50</v>
       </c>
       <c r="J19" s="11">
-        <v>6.34</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>171</v>
@@ -6998,16 +7085,16 @@
       </c>
     </row>
     <row r="12" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G12" s="117" t="s">
+      <c r="G12" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="118"/>
-      <c r="I12" s="119"/>
-      <c r="L12" s="117" t="s">
+      <c r="H12" s="119"/>
+      <c r="I12" s="120"/>
+      <c r="L12" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="118"/>
-      <c r="N12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="120"/>
     </row>
     <row r="13" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G13" s="51" t="s">
@@ -7470,16 +7557,16 @@
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -8006,16 +8093,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -8521,16 +8608,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -9039,16 +9126,16 @@
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="23"/>
-      <c r="E13" s="100" t="s">
+      <c r="E13" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="101"/>
-      <c r="G13" s="102"/>
-      <c r="J13" s="100" t="s">
+      <c r="F13" s="102"/>
+      <c r="G13" s="103"/>
+      <c r="J13" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="101"/>
-      <c r="L13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="103"/>
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
@@ -9460,16 +9547,16 @@
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="100" t="s">
+      <c r="F4" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
-      <c r="K4" s="100" t="s">
+      <c r="G4" s="102"/>
+      <c r="H4" s="103"/>
+      <c r="K4" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="101"/>
-      <c r="M4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="103"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="17" t="s">
@@ -9847,7 +9934,7 @@
   <dimension ref="B1:AF95"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9995,31 +10082,31 @@
     </row>
     <row r="18" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="23"/>
-      <c r="E18" s="100" t="s">
+      <c r="E18" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="102"/>
-      <c r="K18" s="100" t="s">
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="103"/>
+      <c r="K18" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="101"/>
-      <c r="M18" s="102"/>
-      <c r="O18" s="100" t="s">
+      <c r="L18" s="102"/>
+      <c r="M18" s="103"/>
+      <c r="O18" s="101" t="s">
         <v>269</v>
       </c>
-      <c r="P18" s="101"/>
-      <c r="Q18" s="101"/>
-      <c r="R18" s="101"/>
-      <c r="S18" s="101"/>
-      <c r="T18" s="102"/>
-      <c r="V18" s="100" t="s">
+      <c r="P18" s="102"/>
+      <c r="Q18" s="102"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="102"/>
+      <c r="T18" s="103"/>
+      <c r="V18" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="W18" s="101"/>
-      <c r="X18" s="101"/>
-      <c r="Y18" s="102"/>
+      <c r="W18" s="102"/>
+      <c r="X18" s="102"/>
+      <c r="Y18" s="103"/>
       <c r="AA18" s="72" t="s">
         <v>290</v>
       </c>
@@ -10062,26 +10149,26 @@
       <c r="M19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="125" t="s">
+      <c r="O19" s="126" t="s">
         <v>270</v>
       </c>
-      <c r="P19" s="126"/>
-      <c r="Q19" s="123" t="s">
+      <c r="P19" s="127"/>
+      <c r="Q19" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="R19" s="124"/>
-      <c r="S19" s="123" t="s">
+      <c r="R19" s="125"/>
+      <c r="S19" s="124" t="s">
         <v>277</v>
       </c>
-      <c r="T19" s="124"/>
-      <c r="V19" s="125" t="s">
+      <c r="T19" s="125"/>
+      <c r="V19" s="126" t="s">
         <v>260</v>
       </c>
-      <c r="W19" s="126"/>
-      <c r="X19" s="125" t="s">
+      <c r="W19" s="127"/>
+      <c r="X19" s="126" t="s">
         <v>279</v>
       </c>
-      <c r="Y19" s="127"/>
+      <c r="Y19" s="128"/>
       <c r="AA19" s="76" t="s">
         <v>309</v>
       </c>
@@ -10447,10 +10534,11 @@
         <v>366</v>
       </c>
       <c r="L25" s="9">
-        <v>4.95</v>
+        <f>4+64/75</f>
+        <v>4.8533333333333335</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>25</v>
+        <v>460</v>
       </c>
       <c r="O25" s="11">
         <f>72+124/225</f>
@@ -10695,12 +10783,12 @@
       <c r="V29" s="47" t="s">
         <v>284</v>
       </c>
-      <c r="W29" s="120">
+      <c r="W29" s="121">
         <f>W28+Y28</f>
         <v>372.36370370370366</v>
       </c>
-      <c r="X29" s="121"/>
-      <c r="Y29" s="122"/>
+      <c r="X29" s="122"/>
+      <c r="Y29" s="123"/>
       <c r="AA29" s="79" t="s">
         <v>296</v>
       </c>
@@ -10875,9 +10963,16 @@
         <v>173</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="4"/>
+      <c r="K33" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="L33" s="9">
+        <f>7/75</f>
+        <v>9.3333333333333338E-2</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="AA33" s="79" t="s">
         <v>314</v>
       </c>
@@ -11146,7 +11241,7 @@
         <v>370</v>
       </c>
       <c r="F41" s="9">
-        <v>6.34</v>
+        <v>8.73</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>162</v>
@@ -12403,17 +12498,17 @@
     </row>
     <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="23"/>
-      <c r="E15" s="128" t="s">
+      <c r="E15" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="129"/>
-      <c r="G15" s="129"/>
-      <c r="H15" s="130"/>
-      <c r="J15" s="100" t="s">
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="131"/>
+      <c r="J15" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="101"/>
-      <c r="L15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="103"/>
     </row>
     <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="23"/>
@@ -12934,17 +13029,17 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="130"/>
-      <c r="J11" s="100" t="s">
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="131"/>
+      <c r="J11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="101"/>
-      <c r="L11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="103"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -13390,8 +13485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878EF637-2B1F-4BC8-A0FA-F77EC5044F15}">
   <dimension ref="B1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13485,24 +13580,24 @@
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="130"/>
-      <c r="J11" s="100" t="s">
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="131"/>
+      <c r="J11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="101"/>
-      <c r="L11" s="102"/>
-      <c r="N11" s="117" t="s">
+      <c r="K11" s="102"/>
+      <c r="L11" s="103"/>
+      <c r="N11" s="118" t="s">
         <v>435</v>
       </c>
-      <c r="O11" s="118"/>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="119"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="119"/>
+      <c r="Q11" s="119"/>
+      <c r="R11" s="120"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -13973,13 +14068,13 @@
       <c r="N27" s="93" t="s">
         <v>275</v>
       </c>
-      <c r="O27" s="121">
+      <c r="O27" s="122">
         <f>SUM(Q13:Q26)</f>
         <v>36259.599999999999</v>
       </c>
-      <c r="P27" s="121"/>
-      <c r="Q27" s="121"/>
-      <c r="R27" s="122"/>
+      <c r="P27" s="122"/>
+      <c r="Q27" s="122"/>
+      <c r="R27" s="123"/>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -14166,14 +14261,544 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC07E90-6101-47F8-9701-BB9D283EFF37}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C10" s="99"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11" s="99"/>
+    </row>
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="23"/>
+      <c r="E13" s="101" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="131"/>
+      <c r="J13" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="102"/>
+      <c r="L13" s="103"/>
+    </row>
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="23"/>
+      <c r="E14" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="52" t="s">
+        <v>415</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="23"/>
+      <c r="E15" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F15" s="8">
+        <f>4+64/75</f>
+        <v>4.8533333333333335</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H15" s="89"/>
+      <c r="J15" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="K15" s="8">
+        <f>364/1215</f>
+        <v>0.29958847736625516</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="23"/>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="9">
+        <v>11648</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="80" t="s">
+        <v>465</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="9">
+        <f>398+14/75</f>
+        <v>398.18666666666667</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" s="23"/>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="9">
+        <f>5752+8/81</f>
+        <v>5752.0987654320988</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="80" t="s">
+        <v>464</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" s="9">
+        <f>537+28/125</f>
+        <v>537.22400000000005</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="23"/>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="9">
+        <f>333+1/3</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="9">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" s="23"/>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1800</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="80" t="s">
+        <v>467</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="9">
+        <f>8+1/3</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="23"/>
+      <c r="E20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="80" t="s">
+        <v>467</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="23"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="80"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="23"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="80"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="23"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="80"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="23"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="80"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="23"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="80"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="23"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="80"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="23"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="80"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="23"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="80"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="23"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="80"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="23"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="80"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="23"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="80"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="23"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="80"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="23"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="80"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C34" s="23"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="80"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C35" s="23"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="80"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="23"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="80"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C37" s="23"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="80"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C38" s="23"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="80"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C39" s="23"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="80"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E40" s="2"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="80"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E41" s="2"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="80"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E42" s="2"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="80"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E43" s="2"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="80"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E44" s="2"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="80"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E45" s="2"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="80"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E46" s="2"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="80"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E47" s="3"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="83"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J13:L13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14268,17 +14893,17 @@
     </row>
     <row r="12" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="100" t="s">
+      <c r="F13" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="101"/>
-      <c r="H13" s="102"/>
-      <c r="K13" s="100" t="s">
+      <c r="G13" s="102"/>
+      <c r="H13" s="103"/>
+      <c r="K13" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="101"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="103"/>
     </row>
     <row r="14" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="14" t="s">
@@ -14302,14 +14927,14 @@
       <c r="N14" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="P14" s="103" t="s">
+      <c r="P14" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="103"/>
-      <c r="T14" s="103"/>
-      <c r="U14" s="103"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="104"/>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
@@ -14332,12 +14957,12 @@
         <v>25</v>
       </c>
       <c r="N15" s="19"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
-      <c r="S15" s="103"/>
-      <c r="T15" s="103"/>
-      <c r="U15" s="103"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
+      <c r="T15" s="104"/>
+      <c r="U15" s="104"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
@@ -14361,12 +14986,12 @@
       <c r="N16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
-      <c r="S16" s="103"/>
-      <c r="T16" s="103"/>
-      <c r="U16" s="103"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="104"/>
+      <c r="T16" s="104"/>
+      <c r="U16" s="104"/>
     </row>
     <row r="17" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
@@ -14384,12 +15009,12 @@
       <c r="N17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
-      <c r="U17" s="103"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="104"/>
+      <c r="T17" s="104"/>
+      <c r="U17" s="104"/>
     </row>
     <row r="18" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
@@ -14439,14 +15064,14 @@
         <v>173</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="P20" s="104" t="s">
+      <c r="P20" s="105" t="s">
         <v>147</v>
       </c>
-      <c r="Q20" s="104"/>
-      <c r="R20" s="104"/>
-      <c r="S20" s="104"/>
-      <c r="T20" s="104"/>
-      <c r="U20" s="104"/>
+      <c r="Q20" s="105"/>
+      <c r="R20" s="105"/>
+      <c r="S20" s="105"/>
+      <c r="T20" s="105"/>
+      <c r="U20" s="105"/>
     </row>
     <row r="21" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
@@ -14478,14 +15103,14 @@
         <v>162</v>
       </c>
       <c r="N22" s="2"/>
-      <c r="P22" s="103" t="s">
+      <c r="P22" s="104" t="s">
         <v>175</v>
       </c>
-      <c r="Q22" s="103"/>
-      <c r="R22" s="103"/>
-      <c r="S22" s="103"/>
-      <c r="T22" s="103"/>
-      <c r="U22" s="103"/>
+      <c r="Q22" s="104"/>
+      <c r="R22" s="104"/>
+      <c r="S22" s="104"/>
+      <c r="T22" s="104"/>
+      <c r="U22" s="104"/>
     </row>
     <row r="23" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
@@ -14502,12 +15127,12 @@
         <v>255</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="P23" s="103"/>
-      <c r="Q23" s="103"/>
-      <c r="R23" s="103"/>
-      <c r="S23" s="103"/>
-      <c r="T23" s="103"/>
-      <c r="U23" s="103"/>
+      <c r="P23" s="104"/>
+      <c r="Q23" s="104"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="104"/>
+      <c r="T23" s="104"/>
+      <c r="U23" s="104"/>
     </row>
     <row r="24" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
@@ -14524,12 +15149,12 @@
         <v>385</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
-      <c r="U24" s="103"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="104"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
@@ -14548,12 +15173,12 @@
       <c r="N25" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="103"/>
-      <c r="T25" s="103"/>
-      <c r="U25" s="103"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104"/>
+      <c r="T25" s="104"/>
+      <c r="U25" s="104"/>
     </row>
     <row r="26" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
@@ -14569,14 +15194,14 @@
         <v>427</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="P26" s="103" t="s">
+      <c r="P26" s="104" t="s">
         <v>268</v>
       </c>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
-      <c r="S26" s="103"/>
-      <c r="T26" s="103"/>
-      <c r="U26" s="103"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="104"/>
+      <c r="U26" s="104"/>
     </row>
     <row r="27" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
@@ -14586,12 +15211,12 @@
       <c r="L27" s="9"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="P27" s="103"/>
-      <c r="Q27" s="103"/>
-      <c r="R27" s="103"/>
-      <c r="S27" s="103"/>
-      <c r="T27" s="103"/>
-      <c r="U27" s="103"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
+      <c r="T27" s="104"/>
+      <c r="U27" s="104"/>
     </row>
     <row r="28" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
@@ -14601,12 +15226,12 @@
       <c r="L28" s="9"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="P28" s="103"/>
-      <c r="Q28" s="103"/>
-      <c r="R28" s="103"/>
-      <c r="S28" s="103"/>
-      <c r="T28" s="103"/>
-      <c r="U28" s="103"/>
+      <c r="P28" s="104"/>
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104"/>
+      <c r="T28" s="104"/>
+      <c r="U28" s="104"/>
     </row>
     <row r="29" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
@@ -14616,12 +15241,12 @@
       <c r="L29" s="9"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
-      <c r="T29" s="103"/>
-      <c r="U29" s="103"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
+      <c r="S29" s="104"/>
+      <c r="T29" s="104"/>
+      <c r="U29" s="104"/>
     </row>
     <row r="30" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
@@ -14631,14 +15256,14 @@
       <c r="L30" s="9"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="P30" s="103" t="s">
+      <c r="P30" s="104" t="s">
         <v>418</v>
       </c>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
-      <c r="S30" s="103"/>
-      <c r="T30" s="103"/>
-      <c r="U30" s="103"/>
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
+      <c r="S30" s="104"/>
+      <c r="T30" s="104"/>
+      <c r="U30" s="104"/>
     </row>
     <row r="31" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
@@ -14648,12 +15273,12 @@
       <c r="L31" s="9"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
-      <c r="T31" s="103"/>
-      <c r="U31" s="103"/>
+      <c r="P31" s="104"/>
+      <c r="Q31" s="104"/>
+      <c r="R31" s="104"/>
+      <c r="S31" s="104"/>
+      <c r="T31" s="104"/>
+      <c r="U31" s="104"/>
     </row>
     <row r="32" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
@@ -14663,12 +15288,12 @@
       <c r="L32" s="9"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="P32" s="103"/>
-      <c r="Q32" s="103"/>
-      <c r="R32" s="103"/>
-      <c r="S32" s="103"/>
-      <c r="T32" s="103"/>
-      <c r="U32" s="103"/>
+      <c r="P32" s="104"/>
+      <c r="Q32" s="104"/>
+      <c r="R32" s="104"/>
+      <c r="S32" s="104"/>
+      <c r="T32" s="104"/>
+      <c r="U32" s="104"/>
     </row>
     <row r="33" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
@@ -14678,12 +15303,12 @@
       <c r="L33" s="9"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="P33" s="103"/>
-      <c r="Q33" s="103"/>
-      <c r="R33" s="103"/>
-      <c r="S33" s="103"/>
-      <c r="T33" s="103"/>
-      <c r="U33" s="103"/>
+      <c r="P33" s="104"/>
+      <c r="Q33" s="104"/>
+      <c r="R33" s="104"/>
+      <c r="S33" s="104"/>
+      <c r="T33" s="104"/>
+      <c r="U33" s="104"/>
     </row>
     <row r="34" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
@@ -14693,14 +15318,14 @@
       <c r="L34" s="9"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="P34" s="103" t="s">
+      <c r="P34" s="104" t="s">
         <v>428</v>
       </c>
-      <c r="Q34" s="103"/>
-      <c r="R34" s="103"/>
-      <c r="S34" s="103"/>
-      <c r="T34" s="103"/>
-      <c r="U34" s="103"/>
+      <c r="Q34" s="104"/>
+      <c r="R34" s="104"/>
+      <c r="S34" s="104"/>
+      <c r="T34" s="104"/>
+      <c r="U34" s="104"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
@@ -14710,12 +15335,12 @@
       <c r="L35" s="9"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="P35" s="103"/>
-      <c r="Q35" s="103"/>
-      <c r="R35" s="103"/>
-      <c r="S35" s="103"/>
-      <c r="T35" s="103"/>
-      <c r="U35" s="103"/>
+      <c r="P35" s="104"/>
+      <c r="Q35" s="104"/>
+      <c r="R35" s="104"/>
+      <c r="S35" s="104"/>
+      <c r="T35" s="104"/>
+      <c r="U35" s="104"/>
     </row>
     <row r="36" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
@@ -14725,12 +15350,12 @@
       <c r="L36" s="9"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="P36" s="103"/>
-      <c r="Q36" s="103"/>
-      <c r="R36" s="103"/>
-      <c r="S36" s="103"/>
-      <c r="T36" s="103"/>
-      <c r="U36" s="103"/>
+      <c r="P36" s="104"/>
+      <c r="Q36" s="104"/>
+      <c r="R36" s="104"/>
+      <c r="S36" s="104"/>
+      <c r="T36" s="104"/>
+      <c r="U36" s="104"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
@@ -14740,12 +15365,12 @@
       <c r="L37" s="9"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="P37" s="103"/>
-      <c r="Q37" s="103"/>
-      <c r="R37" s="103"/>
-      <c r="S37" s="103"/>
-      <c r="T37" s="103"/>
-      <c r="U37" s="103"/>
+      <c r="P37" s="104"/>
+      <c r="Q37" s="104"/>
+      <c r="R37" s="104"/>
+      <c r="S37" s="104"/>
+      <c r="T37" s="104"/>
+      <c r="U37" s="104"/>
     </row>
     <row r="38" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
@@ -14946,16 +15571,16 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="J11" s="100" t="s">
+      <c r="F11" s="102"/>
+      <c r="G11" s="103"/>
+      <c r="J11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="101"/>
-      <c r="L11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="103"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -15437,17 +16062,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="J11" s="100" t="s">
+      <c r="F11" s="102"/>
+      <c r="G11" s="103"/>
+      <c r="J11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="103"/>
     </row>
     <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -15472,14 +16097,14 @@
       <c r="M12" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O12" s="103" t="s">
+      <c r="O12" s="104" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="103"/>
-      <c r="Q12" s="103"/>
-      <c r="R12" s="103"/>
-      <c r="S12" s="103"/>
-      <c r="T12" s="103"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="104"/>
+      <c r="T12" s="104"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -15503,12 +16128,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
-      <c r="S13" s="103"/>
-      <c r="T13" s="103"/>
+      <c r="O13" s="104"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -15533,12 +16158,12 @@
       <c r="M14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="103"/>
-      <c r="T14" s="103"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -15557,12 +16182,12 @@
       <c r="M15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O15" s="103"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
-      <c r="S15" s="103"/>
-      <c r="T15" s="103"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
+      <c r="T15" s="104"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -15581,14 +16206,14 @@
       <c r="M16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O16" s="103" t="s">
+      <c r="O16" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
-      <c r="S16" s="103"/>
-      <c r="T16" s="103"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="104"/>
+      <c r="T16" s="104"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -15607,12 +16232,12 @@
       <c r="M17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="O17" s="103"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
+      <c r="O17" s="104"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="104"/>
+      <c r="T17" s="104"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -15629,12 +16254,12 @@
         <v>148</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
-      <c r="S18" s="103"/>
-      <c r="T18" s="103"/>
+      <c r="O18" s="104"/>
+      <c r="P18" s="104"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="104"/>
+      <c r="S18" s="104"/>
+      <c r="T18" s="104"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -15651,12 +16276,12 @@
         <v>173</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="103"/>
-      <c r="R19" s="103"/>
-      <c r="S19" s="103"/>
-      <c r="T19" s="103"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="104"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104"/>
+      <c r="T19" s="104"/>
     </row>
     <row r="20" spans="3:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -15684,14 +16309,14 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="104" t="s">
+      <c r="O21" s="105" t="s">
         <v>147</v>
       </c>
-      <c r="P21" s="104"/>
-      <c r="Q21" s="104"/>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="104"/>
+      <c r="P21" s="105"/>
+      <c r="Q21" s="105"/>
+      <c r="R21" s="105"/>
+      <c r="S21" s="105"/>
+      <c r="T21" s="105"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -15712,14 +16337,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="103" t="s">
+      <c r="O23" s="104" t="s">
         <v>174</v>
       </c>
-      <c r="P23" s="103"/>
-      <c r="Q23" s="103"/>
-      <c r="R23" s="103"/>
-      <c r="S23" s="103"/>
-      <c r="T23" s="103"/>
+      <c r="P23" s="104"/>
+      <c r="Q23" s="104"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="104"/>
+      <c r="T23" s="104"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -15730,12 +16355,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -15746,12 +16371,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="103"/>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="103"/>
-      <c r="T25" s="103"/>
+      <c r="O25" s="104"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104"/>
+      <c r="T25" s="104"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -15762,12 +16387,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="6"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="103"/>
-      <c r="P26" s="103"/>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
-      <c r="S26" s="103"/>
-      <c r="T26" s="103"/>
+      <c r="O26" s="104"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="104"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -15778,14 +16403,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="6"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="103" t="s">
+      <c r="O27" s="104" t="s">
         <v>151</v>
       </c>
-      <c r="P27" s="103"/>
-      <c r="Q27" s="103"/>
-      <c r="R27" s="103"/>
-      <c r="S27" s="103"/>
-      <c r="T27" s="103"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
+      <c r="T27" s="104"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -15796,12 +16421,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="6"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="103"/>
-      <c r="P28" s="103"/>
-      <c r="Q28" s="103"/>
-      <c r="R28" s="103"/>
-      <c r="S28" s="103"/>
-      <c r="T28" s="103"/>
+      <c r="O28" s="104"/>
+      <c r="P28" s="104"/>
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104"/>
+      <c r="T28" s="104"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -15812,12 +16437,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="6"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
-      <c r="T29" s="103"/>
+      <c r="O29" s="104"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
+      <c r="S29" s="104"/>
+      <c r="T29" s="104"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -15828,12 +16453,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="6"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
-      <c r="S30" s="103"/>
-      <c r="T30" s="103"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
+      <c r="S30" s="104"/>
+      <c r="T30" s="104"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -15844,14 +16469,14 @@
       <c r="K31" s="9"/>
       <c r="L31" s="6"/>
       <c r="M31" s="2"/>
-      <c r="O31" s="103" t="s">
+      <c r="O31" s="104" t="s">
         <v>152</v>
       </c>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
-      <c r="T31" s="103"/>
+      <c r="P31" s="104"/>
+      <c r="Q31" s="104"/>
+      <c r="R31" s="104"/>
+      <c r="S31" s="104"/>
+      <c r="T31" s="104"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -15862,12 +16487,12 @@
       <c r="K32" s="9"/>
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
-      <c r="O32" s="103"/>
-      <c r="P32" s="103"/>
-      <c r="Q32" s="103"/>
-      <c r="R32" s="103"/>
-      <c r="S32" s="103"/>
-      <c r="T32" s="103"/>
+      <c r="O32" s="104"/>
+      <c r="P32" s="104"/>
+      <c r="Q32" s="104"/>
+      <c r="R32" s="104"/>
+      <c r="S32" s="104"/>
+      <c r="T32" s="104"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C33" s="23"/>
@@ -15878,12 +16503,12 @@
       <c r="K33" s="9"/>
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
-      <c r="O33" s="103"/>
-      <c r="P33" s="103"/>
-      <c r="Q33" s="103"/>
-      <c r="R33" s="103"/>
-      <c r="S33" s="103"/>
-      <c r="T33" s="103"/>
+      <c r="O33" s="104"/>
+      <c r="P33" s="104"/>
+      <c r="Q33" s="104"/>
+      <c r="R33" s="104"/>
+      <c r="S33" s="104"/>
+      <c r="T33" s="104"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C34" s="23"/>
@@ -15894,12 +16519,12 @@
       <c r="K34" s="9"/>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
-      <c r="O34" s="103"/>
-      <c r="P34" s="103"/>
-      <c r="Q34" s="103"/>
-      <c r="R34" s="103"/>
-      <c r="S34" s="103"/>
-      <c r="T34" s="103"/>
+      <c r="O34" s="104"/>
+      <c r="P34" s="104"/>
+      <c r="Q34" s="104"/>
+      <c r="R34" s="104"/>
+      <c r="S34" s="104"/>
+      <c r="T34" s="104"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C35" s="23"/>
@@ -15910,14 +16535,14 @@
       <c r="K35" s="9"/>
       <c r="L35" s="6"/>
       <c r="M35" s="2"/>
-      <c r="O35" s="103" t="s">
+      <c r="O35" s="104" t="s">
         <v>266</v>
       </c>
-      <c r="P35" s="103"/>
-      <c r="Q35" s="103"/>
-      <c r="R35" s="103"/>
-      <c r="S35" s="103"/>
-      <c r="T35" s="103"/>
+      <c r="P35" s="104"/>
+      <c r="Q35" s="104"/>
+      <c r="R35" s="104"/>
+      <c r="S35" s="104"/>
+      <c r="T35" s="104"/>
     </row>
     <row r="36" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
@@ -15928,12 +16553,12 @@
       <c r="K36" s="9"/>
       <c r="L36" s="6"/>
       <c r="M36" s="2"/>
-      <c r="O36" s="103"/>
-      <c r="P36" s="103"/>
-      <c r="Q36" s="103"/>
-      <c r="R36" s="103"/>
-      <c r="S36" s="103"/>
-      <c r="T36" s="103"/>
+      <c r="O36" s="104"/>
+      <c r="P36" s="104"/>
+      <c r="Q36" s="104"/>
+      <c r="R36" s="104"/>
+      <c r="S36" s="104"/>
+      <c r="T36" s="104"/>
     </row>
     <row r="37" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E37" s="2"/>
@@ -15943,12 +16568,12 @@
       <c r="K37" s="9"/>
       <c r="L37" s="6"/>
       <c r="M37" s="2"/>
-      <c r="O37" s="103"/>
-      <c r="P37" s="103"/>
-      <c r="Q37" s="103"/>
-      <c r="R37" s="103"/>
-      <c r="S37" s="103"/>
-      <c r="T37" s="103"/>
+      <c r="O37" s="104"/>
+      <c r="P37" s="104"/>
+      <c r="Q37" s="104"/>
+      <c r="R37" s="104"/>
+      <c r="S37" s="104"/>
+      <c r="T37" s="104"/>
     </row>
     <row r="38" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E38" s="2"/>
@@ -15958,12 +16583,12 @@
       <c r="K38" s="9"/>
       <c r="L38" s="6"/>
       <c r="M38" s="2"/>
-      <c r="O38" s="103"/>
-      <c r="P38" s="103"/>
-      <c r="Q38" s="103"/>
-      <c r="R38" s="103"/>
-      <c r="S38" s="103"/>
-      <c r="T38" s="103"/>
+      <c r="O38" s="104"/>
+      <c r="P38" s="104"/>
+      <c r="Q38" s="104"/>
+      <c r="R38" s="104"/>
+      <c r="S38" s="104"/>
+      <c r="T38" s="104"/>
     </row>
     <row r="39" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E39" s="2"/>
@@ -16136,17 +16761,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="J11" s="100" t="s">
+      <c r="F11" s="102"/>
+      <c r="G11" s="103"/>
+      <c r="J11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="103"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -16171,14 +16796,14 @@
       <c r="M12" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="O12" s="103" t="s">
+      <c r="O12" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="P12" s="103"/>
-      <c r="Q12" s="103"/>
-      <c r="R12" s="103"/>
-      <c r="S12" s="103"/>
-      <c r="T12" s="103"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="104"/>
+      <c r="T12" s="104"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -16202,12 +16827,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
-      <c r="S13" s="103"/>
-      <c r="T13" s="103"/>
+      <c r="O13" s="104"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -16230,12 +16855,12 @@
         <v>81</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="103"/>
-      <c r="T14" s="103"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -16254,12 +16879,12 @@
       <c r="M15" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="O15" s="103"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
-      <c r="S15" s="103"/>
-      <c r="T15" s="103"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
+      <c r="T15" s="104"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -16334,14 +16959,14 @@
       <c r="M19" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="O19" s="114" t="s">
+      <c r="O19" s="115" t="s">
         <v>147</v>
       </c>
-      <c r="P19" s="115"/>
-      <c r="Q19" s="115"/>
-      <c r="R19" s="115"/>
-      <c r="S19" s="115"/>
-      <c r="T19" s="116"/>
+      <c r="P19" s="116"/>
+      <c r="Q19" s="116"/>
+      <c r="R19" s="116"/>
+      <c r="S19" s="116"/>
+      <c r="T19" s="117"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -16361,14 +16986,14 @@
       <c r="M20" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="O20" s="105" t="s">
+      <c r="O20" s="106" t="s">
         <v>414</v>
       </c>
-      <c r="P20" s="106"/>
-      <c r="Q20" s="106"/>
-      <c r="R20" s="106"/>
-      <c r="S20" s="106"/>
-      <c r="T20" s="107"/>
+      <c r="P20" s="107"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="107"/>
+      <c r="S20" s="107"/>
+      <c r="T20" s="108"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -16379,12 +17004,12 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="108"/>
-      <c r="P21" s="109"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="109"/>
-      <c r="S21" s="109"/>
-      <c r="T21" s="110"/>
+      <c r="O21" s="109"/>
+      <c r="P21" s="110"/>
+      <c r="Q21" s="110"/>
+      <c r="R21" s="110"/>
+      <c r="S21" s="110"/>
+      <c r="T21" s="111"/>
     </row>
     <row r="22" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="23"/>
@@ -16395,12 +17020,12 @@
       <c r="K22" s="9"/>
       <c r="L22" s="6"/>
       <c r="M22" s="2"/>
-      <c r="O22" s="111"/>
-      <c r="P22" s="112"/>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="112"/>
-      <c r="S22" s="112"/>
-      <c r="T22" s="113"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="113"/>
+      <c r="Q22" s="113"/>
+      <c r="R22" s="113"/>
+      <c r="S22" s="113"/>
+      <c r="T22" s="114"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -16411,14 +17036,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="105" t="s">
+      <c r="O23" s="106" t="s">
         <v>286</v>
       </c>
-      <c r="P23" s="106"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="106"/>
-      <c r="S23" s="106"/>
-      <c r="T23" s="107"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
+      <c r="S23" s="107"/>
+      <c r="T23" s="108"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -16429,12 +17054,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="108"/>
-      <c r="P24" s="109"/>
-      <c r="Q24" s="109"/>
-      <c r="R24" s="109"/>
-      <c r="S24" s="109"/>
-      <c r="T24" s="110"/>
+      <c r="O24" s="109"/>
+      <c r="P24" s="110"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="110"/>
+      <c r="S24" s="110"/>
+      <c r="T24" s="111"/>
     </row>
     <row r="25" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="23"/>
@@ -16445,12 +17070,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="111"/>
-      <c r="P25" s="112"/>
-      <c r="Q25" s="112"/>
-      <c r="R25" s="112"/>
-      <c r="S25" s="112"/>
-      <c r="T25" s="113"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="113"/>
+      <c r="Q25" s="113"/>
+      <c r="R25" s="113"/>
+      <c r="S25" s="113"/>
+      <c r="T25" s="114"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -16745,16 +17370,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -17311,16 +17936,16 @@
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -17384,14 +18009,14 @@
       <c r="L13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="103" t="s">
+      <c r="N13" s="104" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
-      <c r="S13" s="103"/>
+      <c r="O13" s="104"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -17414,12 +18039,12 @@
       <c r="L14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="103"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="103"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -17435,12 +18060,12 @@
       <c r="L15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="103"/>
-      <c r="O15" s="103"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
-      <c r="S15" s="103"/>
+      <c r="N15" s="104"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
     </row>
     <row r="16" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -17456,12 +18081,12 @@
       <c r="L16" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="N16" s="103"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
-      <c r="S16" s="103"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="104"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="104"/>
     </row>
     <row r="17" spans="3:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -17477,14 +18102,14 @@
       <c r="L17" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="N17" s="103" t="s">
+      <c r="N17" s="104" t="s">
         <v>92</v>
       </c>
-      <c r="O17" s="103"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="103"/>
+      <c r="O17" s="104"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="104"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -17500,12 +18125,12 @@
       <c r="L18" s="87" t="s">
         <v>148</v>
       </c>
-      <c r="N18" s="103"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
-      <c r="S18" s="103"/>
+      <c r="N18" s="104"/>
+      <c r="O18" s="104"/>
+      <c r="P18" s="104"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="104"/>
+      <c r="S18" s="104"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -17521,12 +18146,12 @@
       <c r="L19" s="87" t="s">
         <v>148</v>
       </c>
-      <c r="N19" s="103"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="103"/>
-      <c r="R19" s="103"/>
-      <c r="S19" s="103"/>
+      <c r="N19" s="104"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="104"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -17542,12 +18167,12 @@
       <c r="L20" s="87" t="s">
         <v>173</v>
       </c>
-      <c r="N20" s="103"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
-      <c r="S20" s="103"/>
+      <c r="N20" s="104"/>
+      <c r="O20" s="104"/>
+      <c r="P20" s="104"/>
+      <c r="Q20" s="104"/>
+      <c r="R20" s="104"/>
+      <c r="S20" s="104"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -17578,14 +18203,14 @@
       <c r="L22" s="87" t="s">
         <v>258</v>
       </c>
-      <c r="N22" s="104" t="s">
+      <c r="N22" s="105" t="s">
         <v>147</v>
       </c>
-      <c r="O22" s="104"/>
-      <c r="P22" s="104"/>
-      <c r="Q22" s="104"/>
-      <c r="R22" s="104"/>
-      <c r="S22" s="104"/>
+      <c r="O22" s="105"/>
+      <c r="P22" s="105"/>
+      <c r="Q22" s="105"/>
+      <c r="R22" s="105"/>
+      <c r="S22" s="105"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -17610,14 +18235,14 @@
       <c r="J24" s="2"/>
       <c r="K24" s="9"/>
       <c r="L24" s="87"/>
-      <c r="N24" s="103" t="s">
+      <c r="N24" s="104" t="s">
         <v>409</v>
       </c>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -17627,12 +18252,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="9"/>
       <c r="L25" s="87"/>
-      <c r="N25" s="103"/>
-      <c r="O25" s="103"/>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="103"/>
+      <c r="N25" s="104"/>
+      <c r="O25" s="104"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -17642,12 +18267,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
-      <c r="N26" s="103"/>
-      <c r="O26" s="103"/>
-      <c r="P26" s="103"/>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
-      <c r="S26" s="103"/>
+      <c r="N26" s="104"/>
+      <c r="O26" s="104"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -17657,12 +18282,12 @@
       <c r="J27" s="2"/>
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
-      <c r="N27" s="103"/>
-      <c r="O27" s="103"/>
-      <c r="P27" s="103"/>
-      <c r="Q27" s="103"/>
-      <c r="R27" s="103"/>
-      <c r="S27" s="103"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="104"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -17672,14 +18297,14 @@
       <c r="J28" s="2"/>
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="103" t="s">
+      <c r="N28" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="O28" s="103"/>
-      <c r="P28" s="103"/>
-      <c r="Q28" s="103"/>
-      <c r="R28" s="103"/>
-      <c r="S28" s="103"/>
+      <c r="O28" s="104"/>
+      <c r="P28" s="104"/>
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -17689,12 +18314,12 @@
       <c r="J29" s="2"/>
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
-      <c r="N29" s="103"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
+      <c r="N29" s="104"/>
+      <c r="O29" s="104"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
+      <c r="S29" s="104"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -17704,12 +18329,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
-      <c r="N30" s="103"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
-      <c r="S30" s="103"/>
+      <c r="N30" s="104"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
+      <c r="S30" s="104"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -17719,12 +18344,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="9"/>
       <c r="L31" s="2"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
+      <c r="N31" s="104"/>
+      <c r="O31" s="104"/>
+      <c r="P31" s="104"/>
+      <c r="Q31" s="104"/>
+      <c r="R31" s="104"/>
+      <c r="S31" s="104"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -17936,16 +18561,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="100" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>

</xml_diff>

<commit_message>
Added savegame, updated spreadsheet and factory design
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 3\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 4\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E683BBAA-67B0-4F00-8E82-D0DA43F33B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0319DEE-EDAD-4921-998B-DE02996CA9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="14" activeTab="23" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="476">
   <si>
     <t>Item</t>
   </si>
@@ -829,9 +829,6 @@
     <t>Karn's Conduit, Tollarian Meltdown</t>
   </si>
   <si>
-    <t>Phyrexian Datavault, Keldon Armory, Jund Pyroclast, Urabrask's Refinery, Obelisks of Alara, Karn's Conduit, Tollarian Meltdown</t>
-  </si>
-  <si>
     <t>Tollarian Meltown</t>
   </si>
   <si>
@@ -1468,9 +1465,6 @@
     <t>2 Modules</t>
   </si>
   <si>
-    <t>Tollarian Metldown, Jund Pyroclast, Urabrask Refinery, Kaladesh Refinery</t>
-  </si>
-  <si>
     <t>Phyrexian Datavault, The Abyssal Chains of Shandalar, Keldon Armory, Obelisks of Alara, Tollarian Meltdown, Simic Subline, Aetherflux Reactor</t>
   </si>
   <si>
@@ -1478,6 +1472,21 @@
   </si>
   <si>
     <t>Ydris Nexus</t>
+  </si>
+  <si>
+    <t>Ingots Module</t>
+  </si>
+  <si>
+    <t>Tollarian Metldown, Jund Pyroclast, Urabrask Refinery, Kaladesh Refinery, Riveteers District</t>
+  </si>
+  <si>
+    <t>Phyrexian Datavault, Keldon Armory, Jund Pyroclast, Urabrask's Refinery, Obelisks of Alara, Karn's Conduit, Tollarian Meltdown. Aetherflux Reactor</t>
+  </si>
+  <si>
+    <t>Packaged Alumina Solution</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -2195,7 +2204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2468,6 +2477,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2804,10 +2817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
-  <dimension ref="B2:T116"/>
+  <dimension ref="B2:T119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2947,7 +2960,7 @@
       </c>
       <c r="D10" s="11">
         <f>'Kaladesh Refinery'!K14</f>
-        <v>33.333333333333336</v>
+        <v>30.833333333333336</v>
       </c>
       <c r="E10" s="40" t="s">
         <v>106</v>
@@ -3170,14 +3183,14 @@
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C21" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D21" s="38">
         <f>'Ydris’ Nexus'!K13</f>
         <v>456.55555555555554</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>76</v>
@@ -3191,13 +3204,13 @@
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C22" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D22" s="11">
         <v>72.25</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>77</v>
@@ -3218,7 +3231,7 @@
         <v>398.18666666666667</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>78</v>
@@ -3239,7 +3252,7 @@
         <v>537.22400000000005</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>79</v>
@@ -3252,9 +3265,16 @@
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C25" s="6"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="9">
+        <f>759+971/1350</f>
+        <v>759.71925925925927</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="H25" s="6" t="s">
         <v>80</v>
       </c>
@@ -3266,9 +3286,16 @@
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C26" s="6"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="9">
+        <f>996+25/36</f>
+        <v>996.69444444444446</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="H26" s="6" t="s">
         <v>86</v>
       </c>
@@ -3280,9 +3307,15 @@
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C27" s="6"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="40"/>
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="9">
+        <v>590</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="H27" s="6" t="s">
         <v>87</v>
       </c>
@@ -3899,7 +3932,7 @@
     <row r="79" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C79" s="1"/>
       <c r="H79" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I79" s="11">
         <v>11.52</v>
@@ -3911,7 +3944,7 @@
     <row r="80" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C80" s="1"/>
       <c r="H80" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I80" s="11">
         <v>10</v>
@@ -3923,7 +3956,7 @@
     <row r="81" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C81" s="1"/>
       <c r="H81" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I81" s="11">
         <v>5</v>
@@ -3935,7 +3968,7 @@
     <row r="82" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C82" s="1"/>
       <c r="H82" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I82" s="11">
         <v>4.2</v>
@@ -3946,7 +3979,7 @@
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H83" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I83" s="11">
         <v>2.73</v>
@@ -3957,7 +3990,7 @@
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H84" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I84" s="11">
         <v>2.73</v>
@@ -3968,7 +4001,7 @@
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H85" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I85" s="11">
         <v>1.54</v>
@@ -3979,7 +4012,7 @@
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H86" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I86" s="11">
         <v>1</v>
@@ -3990,7 +4023,7 @@
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H87" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I87" s="11">
         <v>0.25</v>
@@ -4005,7 +4038,7 @@
       <c r="C88" s="1"/>
       <c r="D88"/>
       <c r="H88" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I88" s="11">
         <v>0.21</v>
@@ -4019,7 +4052,7 @@
       <c r="C89" s="1"/>
       <c r="D89"/>
       <c r="H89" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I89" s="11">
         <f>7/75</f>
@@ -4034,13 +4067,13 @@
       <c r="C90" s="1"/>
       <c r="D90"/>
       <c r="H90" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I90" s="11">
         <v>5</v>
       </c>
       <c r="J90" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.35">
@@ -4048,13 +4081,13 @@
       <c r="C91" s="1"/>
       <c r="D91"/>
       <c r="H91" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I91" s="11">
         <v>1.75</v>
       </c>
       <c r="J91" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="92" spans="2:16" x14ac:dyDescent="0.35">
@@ -4062,24 +4095,24 @@
       <c r="C92" s="1"/>
       <c r="D92"/>
       <c r="H92" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I92" s="11">
         <v>2.91</v>
       </c>
       <c r="J92" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H93" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I93" s="11">
         <v>2.83</v>
       </c>
       <c r="J93" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="94" spans="2:16" x14ac:dyDescent="0.35">
@@ -4087,14 +4120,14 @@
       <c r="C94" s="1"/>
       <c r="D94"/>
       <c r="H94" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I94" s="11">
         <f>'The Mirrodin Trigon'!K21</f>
         <v>17.188888888888869</v>
       </c>
       <c r="J94" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="95" spans="2:16" x14ac:dyDescent="0.35">
@@ -4102,13 +4135,13 @@
       <c r="C95" s="1"/>
       <c r="D95"/>
       <c r="H95" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I95" s="11">
         <v>4</v>
       </c>
       <c r="J95" s="40" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="96" spans="2:16" x14ac:dyDescent="0.35">
@@ -4116,13 +4149,13 @@
       <c r="C96" s="1"/>
       <c r="D96"/>
       <c r="H96" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I96" s="11">
         <v>13.2</v>
       </c>
       <c r="J96" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="97" spans="2:20" x14ac:dyDescent="0.35">
@@ -4130,13 +4163,13 @@
       <c r="C97" s="1"/>
       <c r="D97"/>
       <c r="H97" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I97" s="11">
         <v>0.1</v>
       </c>
       <c r="J97" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" spans="2:20" x14ac:dyDescent="0.35">
@@ -4151,7 +4184,7 @@
         <v>6.333333333333333</v>
       </c>
       <c r="J98" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R98" s="1"/>
     </row>
@@ -4160,13 +4193,13 @@
       <c r="C99" s="1"/>
       <c r="D99"/>
       <c r="H99" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I99" s="11">
         <v>1</v>
       </c>
       <c r="J99" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R99" s="1"/>
     </row>
@@ -4175,14 +4208,14 @@
       <c r="C100" s="1"/>
       <c r="D100"/>
       <c r="H100" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I100" s="8">
         <f>364/1215</f>
         <v>0.29958847736625516</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="101" spans="2:20" x14ac:dyDescent="0.35">
@@ -4193,7 +4226,7 @@
         <v>5</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="102" spans="2:20" x14ac:dyDescent="0.35">
@@ -4205,9 +4238,15 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="T102" s="1"/>
+        <v>455</v>
+      </c>
+      <c r="N102" s="132"/>
+      <c r="O102" s="132"/>
+      <c r="P102" s="132"/>
+      <c r="Q102" s="132"/>
+      <c r="R102" s="132"/>
+      <c r="S102" s="132"/>
+      <c r="T102" s="133"/>
     </row>
     <row r="103" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H103" s="4" t="s">
@@ -4217,9 +4256,15 @@
         <v>45</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="T103" s="1"/>
+        <v>455</v>
+      </c>
+      <c r="N103" s="132"/>
+      <c r="O103" s="132"/>
+      <c r="P103" s="132"/>
+      <c r="Q103" s="132"/>
+      <c r="R103" s="132"/>
+      <c r="S103" s="132"/>
+      <c r="T103" s="133"/>
     </row>
     <row r="104" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H104" s="4" t="s">
@@ -4229,77 +4274,216 @@
         <v>45</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="O104" s="1"/>
-      <c r="T104" s="1"/>
+        <v>455</v>
+      </c>
+      <c r="N104" s="132"/>
+      <c r="O104" s="133"/>
+      <c r="P104" s="132"/>
+      <c r="Q104" s="132"/>
+      <c r="R104" s="132"/>
+      <c r="S104" s="132"/>
+      <c r="T104" s="133"/>
     </row>
     <row r="105" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H105" s="6"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="40"/>
-      <c r="O105" s="1"/>
-      <c r="T105" s="1"/>
+      <c r="H105" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I105" s="9">
+        <v>5</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="N105" s="132"/>
+      <c r="O105" s="133"/>
+      <c r="P105" s="132"/>
+      <c r="Q105" s="132"/>
+      <c r="R105" s="132"/>
+      <c r="S105" s="132"/>
+      <c r="T105" s="133"/>
     </row>
     <row r="106" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H106" s="6"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="40"/>
-      <c r="O106" s="1"/>
-      <c r="T106" s="1"/>
+      <c r="H106" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="I106" s="9">
+        <v>5</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="N106" s="132"/>
+      <c r="O106" s="133"/>
+      <c r="P106" s="132"/>
+      <c r="Q106" s="132"/>
+      <c r="R106" s="132"/>
+      <c r="S106" s="132"/>
+      <c r="T106" s="133"/>
     </row>
     <row r="107" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H107" s="6"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="40"/>
-      <c r="O107" s="1"/>
-      <c r="T107" s="1"/>
+      <c r="H107" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I107" s="9">
+        <v>5</v>
+      </c>
+      <c r="J107" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="N107" s="132"/>
+      <c r="O107" s="132"/>
+      <c r="P107" s="133"/>
+      <c r="Q107" s="132"/>
+      <c r="R107" s="132"/>
+      <c r="S107" s="132"/>
+      <c r="T107" s="133"/>
     </row>
     <row r="108" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H108" s="6"/>
-      <c r="I108" s="11"/>
-      <c r="J108" s="40"/>
-      <c r="O108" s="1"/>
+      <c r="H108" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I108" s="9">
+        <v>3.75</v>
+      </c>
+      <c r="J108" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="N108" s="132"/>
+      <c r="O108" s="132"/>
+      <c r="P108" s="133"/>
+      <c r="Q108" s="132"/>
+      <c r="R108" s="132"/>
+      <c r="S108" s="132"/>
+      <c r="T108" s="132"/>
     </row>
     <row r="109" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H109" s="6"/>
-      <c r="I109" s="11"/>
-      <c r="J109" s="40"/>
+      <c r="H109" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="I109" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="J109" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="N109" s="132"/>
+      <c r="O109" s="132"/>
+      <c r="P109" s="133"/>
+      <c r="Q109" s="132"/>
+      <c r="R109" s="132"/>
+      <c r="S109" s="132"/>
+      <c r="T109" s="132"/>
     </row>
     <row r="110" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H110" s="6"/>
       <c r="I110" s="11"/>
       <c r="J110" s="40"/>
+      <c r="N110" s="132"/>
+      <c r="O110" s="132"/>
+      <c r="P110" s="133"/>
+      <c r="Q110" s="132"/>
+      <c r="R110" s="132"/>
+      <c r="S110" s="132"/>
+      <c r="T110" s="132"/>
     </row>
     <row r="111" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H111" s="6"/>
       <c r="I111" s="11"/>
       <c r="J111" s="40"/>
+      <c r="N111" s="132"/>
+      <c r="O111" s="132"/>
+      <c r="P111" s="133"/>
+      <c r="Q111" s="132"/>
+      <c r="R111" s="132"/>
+      <c r="S111" s="132"/>
+      <c r="T111" s="132"/>
     </row>
     <row r="112" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H112" s="6"/>
       <c r="I112" s="11"/>
       <c r="J112" s="40"/>
-    </row>
-    <row r="113" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="N112" s="132"/>
+      <c r="O112" s="132"/>
+      <c r="P112" s="133"/>
+      <c r="Q112" s="132"/>
+      <c r="R112" s="132"/>
+      <c r="S112" s="132"/>
+      <c r="T112" s="132"/>
+    </row>
+    <row r="113" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H113" s="6"/>
       <c r="I113" s="11"/>
       <c r="J113" s="40"/>
-    </row>
-    <row r="114" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="N113" s="132"/>
+      <c r="O113" s="132"/>
+      <c r="P113" s="133"/>
+      <c r="Q113" s="132"/>
+      <c r="R113" s="132"/>
+      <c r="S113" s="132"/>
+      <c r="T113" s="132"/>
+    </row>
+    <row r="114" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H114" s="6"/>
       <c r="I114" s="11"/>
       <c r="J114" s="40"/>
-    </row>
-    <row r="115" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="N114" s="132"/>
+      <c r="O114" s="132"/>
+      <c r="P114" s="132"/>
+      <c r="Q114" s="132"/>
+      <c r="R114" s="132"/>
+      <c r="S114" s="132"/>
+      <c r="T114" s="132"/>
+    </row>
+    <row r="115" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H115" s="6"/>
       <c r="I115" s="11"/>
       <c r="J115" s="40"/>
-    </row>
-    <row r="116" spans="8:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N115" s="132"/>
+      <c r="O115" s="132"/>
+      <c r="P115" s="132"/>
+      <c r="Q115" s="132"/>
+      <c r="R115" s="132"/>
+      <c r="S115" s="132"/>
+      <c r="T115" s="132"/>
+    </row>
+    <row r="116" spans="8:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H116" s="7"/>
       <c r="I116" s="44"/>
       <c r="J116" s="42"/>
+      <c r="N116" s="132"/>
+      <c r="O116" s="132"/>
+      <c r="P116" s="132"/>
+      <c r="Q116" s="132"/>
+      <c r="R116" s="132"/>
+      <c r="S116" s="132"/>
+      <c r="T116" s="132"/>
+    </row>
+    <row r="117" spans="8:20" x14ac:dyDescent="0.35">
+      <c r="N117" s="132"/>
+      <c r="O117" s="132"/>
+      <c r="P117" s="132"/>
+      <c r="Q117" s="132"/>
+      <c r="R117" s="132"/>
+      <c r="S117" s="132"/>
+      <c r="T117" s="132"/>
+    </row>
+    <row r="118" spans="8:20" x14ac:dyDescent="0.35">
+      <c r="N118" s="132"/>
+      <c r="O118" s="132"/>
+      <c r="P118" s="132"/>
+      <c r="Q118" s="132"/>
+      <c r="R118" s="132"/>
+      <c r="S118" s="132"/>
+      <c r="T118" s="132"/>
+    </row>
+    <row r="119" spans="8:20" x14ac:dyDescent="0.35">
+      <c r="N119" s="132"/>
+      <c r="O119" s="132"/>
+      <c r="P119" s="132"/>
+      <c r="Q119" s="132"/>
+      <c r="R119" s="132"/>
+      <c r="S119" s="132"/>
+      <c r="T119" s="132"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:E18">
@@ -4783,7 +4967,7 @@
   <dimension ref="B1:T44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4821,7 +5005,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
@@ -4974,7 +5158,7 @@
       </c>
       <c r="K14" s="9">
         <f>390-K17-K19-K24</f>
-        <v>33.333333333333336</v>
+        <v>30.833333333333336</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>25</v>
@@ -5168,11 +5352,11 @@
         <v>14</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M23" s="2"/>
       <c r="O23" s="104" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P23" s="104"/>
       <c r="Q23" s="104"/>
@@ -5189,11 +5373,11 @@
         <v>5</v>
       </c>
       <c r="K24" s="9">
-        <f>34+2/3</f>
-        <v>34.666666666666664</v>
+        <f>34+2/3+2.5</f>
+        <v>37.166666666666664</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M24" s="2"/>
       <c r="O24" s="104"/>
@@ -5245,7 +5429,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
       <c r="O27" s="104" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="P27" s="104"/>
       <c r="Q27" s="104"/>
@@ -5451,8 +5635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED21A768-E1F1-4F70-B6C9-A662B38F9ACD}">
   <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5485,12 +5669,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>256</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -5506,7 +5690,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -5514,7 +5698,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -5530,7 +5714,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5844,7 +6028,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="L27" s="41" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.35">
@@ -6043,7 +6227,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -6223,7 +6407,7 @@
         <v>154</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
@@ -6555,7 +6739,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -7055,7 +7239,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.35">
@@ -7528,7 +7712,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
@@ -7544,7 +7728,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F6">
         <f>5800/4352.7</f>
@@ -7556,7 +7740,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
@@ -7734,7 +7918,7 @@
         <v>137</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N16" s="6">
         <v>3</v>
@@ -7761,7 +7945,7 @@
         <v>137</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N17" s="7">
         <v>4</v>
@@ -7789,7 +7973,7 @@
         <v>137</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
@@ -8087,7 +8271,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -8095,7 +8279,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -8111,7 +8295,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -9101,7 +9285,7 @@
         <v>239</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -9117,7 +9301,7 @@
         <v>241</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -10003,7 +10187,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
@@ -10014,10 +10198,10 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -10025,7 +10209,7 @@
         <v>239</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -10033,7 +10217,7 @@
         <v>240</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
@@ -10046,18 +10230,18 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
@@ -10065,15 +10249,15 @@
         <v>242</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
@@ -10081,7 +10265,7 @@
         <v>243</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10089,7 +10273,7 @@
         <v>244</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
@@ -10117,7 +10301,7 @@
       <c r="L18" s="102"/>
       <c r="M18" s="103"/>
       <c r="O18" s="101" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P18" s="102"/>
       <c r="Q18" s="102"/>
@@ -10125,28 +10309,28 @@
       <c r="S18" s="102"/>
       <c r="T18" s="103"/>
       <c r="V18" s="101" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="W18" s="102"/>
       <c r="X18" s="102"/>
       <c r="Y18" s="103"/>
       <c r="AA18" s="72" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AB18" s="73" t="s">
         <v>1</v>
       </c>
       <c r="AC18" s="73" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD18" s="73" t="s">
         <v>289</v>
       </c>
-      <c r="AD18" s="73" t="s">
+      <c r="AE18" s="86" t="s">
+        <v>298</v>
+      </c>
+      <c r="AF18" s="74" t="s">
         <v>290</v>
-      </c>
-      <c r="AE18" s="86" t="s">
-        <v>299</v>
-      </c>
-      <c r="AF18" s="74" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="19" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10161,7 +10345,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>0</v>
@@ -10173,27 +10357,27 @@
         <v>24</v>
       </c>
       <c r="O19" s="126" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P19" s="127"/>
       <c r="Q19" s="124" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="R19" s="125"/>
       <c r="S19" s="124" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T19" s="125"/>
       <c r="V19" s="126" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="W19" s="127"/>
       <c r="X19" s="126" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y19" s="128"/>
       <c r="AA19" s="76" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB19" s="84">
         <v>1</v>
@@ -10202,10 +10386,10 @@
         <v>0.2</v>
       </c>
       <c r="AD19" s="77" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE19" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AF19" s="78" t="s">
         <v>175</v>
@@ -10263,7 +10447,7 @@
         <v>24</v>
       </c>
       <c r="AA20" s="79" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB20" s="85">
         <v>1</v>
@@ -10272,13 +10456,13 @@
         <v>0.2</v>
       </c>
       <c r="AD20" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE20" s="75" t="s">
         <v>104</v>
       </c>
       <c r="AF20" s="80" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="3:32" x14ac:dyDescent="0.35">
@@ -10327,17 +10511,17 @@
         <v>170.1</v>
       </c>
       <c r="W21" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="X21" s="43">
         <f>158+22/75</f>
         <v>158.29333333333332</v>
       </c>
       <c r="Y21" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA21" s="79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AB21" s="85">
         <v>1</v>
@@ -10346,13 +10530,13 @@
         <v>0.2</v>
       </c>
       <c r="AD21" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE21" s="75" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF21" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="3:32" x14ac:dyDescent="0.35">
@@ -10369,7 +10553,7 @@
       </c>
       <c r="H22" s="2"/>
       <c r="K22" s="38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L22" s="9">
         <v>11.52</v>
@@ -10382,7 +10566,7 @@
         <v>125.58</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q22" s="2">
         <f>148+2/5</f>
@@ -10402,12 +10586,12 @@
         <v>43.970370370370368</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X22" s="11"/>
       <c r="Y22" s="2"/>
       <c r="AA22" s="79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AB22" s="85">
         <v>1</v>
@@ -10416,13 +10600,13 @@
         <v>0.3</v>
       </c>
       <c r="AD22" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE22" s="75" t="s">
+        <v>316</v>
+      </c>
+      <c r="AF22" s="80" t="s">
         <v>317</v>
-      </c>
-      <c r="AF22" s="80" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="23" spans="3:32" x14ac:dyDescent="0.35">
@@ -10438,7 +10622,7 @@
       </c>
       <c r="H23" s="2"/>
       <c r="K23" s="38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L23" s="9">
         <v>10</v>
@@ -10450,13 +10634,13 @@
         <v>2.73</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q23" s="2">
         <v>226.8</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
@@ -10465,7 +10649,7 @@
       <c r="X23" s="11"/>
       <c r="Y23" s="2"/>
       <c r="AA23" s="79" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB23" s="85">
         <v>1</v>
@@ -10474,13 +10658,13 @@
         <v>0.3</v>
       </c>
       <c r="AD23" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE23" s="75" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF23" s="80" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="3:32" x14ac:dyDescent="0.35">
@@ -10496,7 +10680,7 @@
       </c>
       <c r="H24" s="2"/>
       <c r="K24" s="38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L24" s="9">
         <v>5</v>
@@ -10520,7 +10704,7 @@
       <c r="X24" s="11"/>
       <c r="Y24" s="2"/>
       <c r="AA24" s="79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AB24" s="85">
         <v>1</v>
@@ -10529,13 +10713,13 @@
         <v>0.4</v>
       </c>
       <c r="AD24" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE24" s="75" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AF24" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="3:32" x14ac:dyDescent="0.35">
@@ -10551,24 +10735,24 @@
         <v>55</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K25" s="38" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L25" s="9">
         <f>4+64/75</f>
         <v>4.8533333333333335</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="O25" s="11">
         <f>72+124/225</f>
         <v>72.551111111111112</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -10579,7 +10763,7 @@
       <c r="X25" s="11"/>
       <c r="Y25" s="2"/>
       <c r="AA25" s="79" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AB25" s="85">
         <v>1</v>
@@ -10588,13 +10772,13 @@
         <v>0.6</v>
       </c>
       <c r="AD25" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE25" s="75" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF25" s="80" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="3:32" x14ac:dyDescent="0.35">
@@ -10611,7 +10795,7 @@
       </c>
       <c r="H26" s="2"/>
       <c r="K26" s="38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L26" s="9">
         <v>4.2</v>
@@ -10630,7 +10814,7 @@
       <c r="X26" s="11"/>
       <c r="Y26" s="2"/>
       <c r="AA26" s="79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AB26" s="85">
         <v>1</v>
@@ -10639,13 +10823,13 @@
         <v>0.7</v>
       </c>
       <c r="AD26" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE26" s="75" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AF26" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10662,7 +10846,7 @@
       </c>
       <c r="H27" s="2"/>
       <c r="K27" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L27" s="9">
         <v>2.73</v>
@@ -10681,7 +10865,7 @@
       <c r="X27" s="69"/>
       <c r="Y27" s="67"/>
       <c r="AA27" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB27" s="85">
         <v>1</v>
@@ -10690,30 +10874,30 @@
         <v>1</v>
       </c>
       <c r="AD27" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE27" s="75" t="s">
         <v>175</v>
       </c>
       <c r="AF27" s="80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="23"/>
       <c r="E28" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F28" s="9">
         <f>174+46/375</f>
         <v>174.12266666666667</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H28" s="2"/>
       <c r="K28" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L28" s="9">
         <v>2.73</v>
@@ -10728,21 +10912,21 @@
       <c r="S28" s="67"/>
       <c r="T28" s="67"/>
       <c r="V28" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="W28" s="71">
         <f>SUM(V21:V22)</f>
         <v>214.07037037037037</v>
       </c>
       <c r="X28" s="70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Y28" s="71">
         <f>SUM(X21:X27)</f>
         <v>158.29333333333332</v>
       </c>
       <c r="AA28" s="79" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AB28" s="85">
         <v>1</v>
@@ -10751,7 +10935,7 @@
         <v>1.2</v>
       </c>
       <c r="AD28" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE28" s="75" t="s">
         <v>53</v>
@@ -10774,7 +10958,7 @@
       </c>
       <c r="H29" s="2"/>
       <c r="K29" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L29" s="9">
         <v>1.54</v>
@@ -10783,28 +10967,28 @@
         <v>8</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P29" s="68">
         <f>SUM(O21:O28)</f>
         <v>444.51788888888893</v>
       </c>
       <c r="Q29" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R29" s="68">
         <f>SUM(Q21:Q28)</f>
         <v>526.89777777777772</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T29" s="68">
         <f>SUM(S21:S28)</f>
         <v>400</v>
       </c>
       <c r="V29" s="47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="W29" s="121">
         <f>W28+Y28</f>
@@ -10813,7 +10997,7 @@
       <c r="X29" s="122"/>
       <c r="Y29" s="123"/>
       <c r="AA29" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB29" s="85">
         <v>1</v>
@@ -10822,13 +11006,13 @@
         <v>1.6</v>
       </c>
       <c r="AD29" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE29" s="75" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF29" s="80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10845,7 +11029,7 @@
       </c>
       <c r="H30" s="2"/>
       <c r="K30" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L30" s="9">
         <v>1</v>
@@ -10854,28 +11038,28 @@
         <v>8</v>
       </c>
       <c r="O30" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P30" s="66">
         <f>P29/600</f>
         <v>0.74086314814814824</v>
       </c>
       <c r="Q30" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R30" s="66">
         <f>R29/600</f>
         <v>0.87816296296296281</v>
       </c>
       <c r="S30" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T30" s="66">
         <f>T29/600</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AA30" s="79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB30" s="85">
         <v>2</v>
@@ -10884,13 +11068,13 @@
         <v>2.7</v>
       </c>
       <c r="AD30" s="75" t="s">
+        <v>330</v>
+      </c>
+      <c r="AE30" s="75" t="s">
+        <v>332</v>
+      </c>
+      <c r="AF30" s="80" t="s">
         <v>331</v>
-      </c>
-      <c r="AE30" s="75" t="s">
-        <v>333</v>
-      </c>
-      <c r="AF30" s="80" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="31" spans="3:32" x14ac:dyDescent="0.35">
@@ -10907,7 +11091,7 @@
       </c>
       <c r="H31" s="2"/>
       <c r="K31" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L31" s="9">
         <v>0.25</v>
@@ -10916,7 +11100,7 @@
         <v>8</v>
       </c>
       <c r="AA31" s="79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB31" s="85">
         <v>4</v>
@@ -10925,7 +11109,7 @@
         <v>2.8</v>
       </c>
       <c r="AD31" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE31" s="75" t="s">
         <v>72</v>
@@ -10947,7 +11131,7 @@
       </c>
       <c r="H32" s="2"/>
       <c r="K32" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L32" s="9">
         <v>0.21</v>
@@ -10956,7 +11140,7 @@
         <v>8</v>
       </c>
       <c r="AA32" s="79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB32" s="85">
         <v>12</v>
@@ -10965,7 +11149,7 @@
         <v>3.2</v>
       </c>
       <c r="AD32" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE32" s="75" t="s">
         <v>76</v>
@@ -10987,7 +11171,7 @@
       </c>
       <c r="H33" s="2"/>
       <c r="K33" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L33" s="9">
         <f>7/75</f>
@@ -10997,7 +11181,7 @@
         <v>8</v>
       </c>
       <c r="AA33" s="79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB33" s="85">
         <v>3</v>
@@ -11006,13 +11190,13 @@
         <v>3.3</v>
       </c>
       <c r="AD33" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE33" s="75" t="s">
         <v>76</v>
       </c>
       <c r="AF33" s="80" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="3:32" x14ac:dyDescent="0.35">
@@ -11031,7 +11215,7 @@
       <c r="L34" s="9"/>
       <c r="M34" s="4"/>
       <c r="AA34" s="79" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB34" s="85">
         <v>14</v>
@@ -11040,13 +11224,13 @@
         <v>3.4</v>
       </c>
       <c r="AD34" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE34" s="75" t="s">
         <v>70</v>
       </c>
       <c r="AF34" s="80" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="3:32" x14ac:dyDescent="0.35">
@@ -11062,13 +11246,13 @@
         <v>55</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K35" s="11"/>
       <c r="L35" s="9"/>
       <c r="M35" s="4"/>
       <c r="AA35" s="79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB35" s="85">
         <v>16</v>
@@ -11077,7 +11261,7 @@
         <v>3.7</v>
       </c>
       <c r="AD35" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE35" s="75" t="s">
         <v>76</v>
@@ -11089,20 +11273,20 @@
     <row r="36" spans="3:32" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
       <c r="E36" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F36" s="9">
         <v>480</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H36" s="2"/>
       <c r="K36" s="11"/>
       <c r="L36" s="9"/>
       <c r="M36" s="4"/>
       <c r="AA36" s="79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB36" s="85">
         <v>4</v>
@@ -11111,19 +11295,19 @@
         <v>3.7</v>
       </c>
       <c r="AD36" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE36" s="75" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF36" s="80" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="3:32" x14ac:dyDescent="0.35">
       <c r="C37" s="23"/>
       <c r="E37" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F37" s="9">
         <v>240</v>
@@ -11136,7 +11320,7 @@
       <c r="L37" s="9"/>
       <c r="M37" s="4"/>
       <c r="AA37" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB37" s="85">
         <v>1</v>
@@ -11145,13 +11329,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="AD37" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE37" s="75" t="s">
+        <v>301</v>
+      </c>
+      <c r="AF37" s="80" t="s">
         <v>302</v>
-      </c>
-      <c r="AF37" s="80" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="38" spans="3:32" x14ac:dyDescent="0.35">
@@ -11171,7 +11355,7 @@
       <c r="L38" s="9"/>
       <c r="M38" s="2"/>
       <c r="AA38" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB38" s="85">
         <v>8</v>
@@ -11180,33 +11364,33 @@
         <v>10.6</v>
       </c>
       <c r="AD38" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE38" s="75" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF38" s="80" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="3:32" x14ac:dyDescent="0.35">
       <c r="C39" s="23"/>
       <c r="E39" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F39" s="9">
         <f>1050+13/15</f>
         <v>1050.8666666666666</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H39" s="2"/>
       <c r="K39" s="11"/>
       <c r="L39" s="9"/>
       <c r="M39" s="2"/>
       <c r="AA39" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB39" s="85">
         <v>1</v>
@@ -11215,13 +11399,13 @@
         <v>11.2</v>
       </c>
       <c r="AD39" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE39" s="75" t="s">
         <v>70</v>
       </c>
       <c r="AF39" s="80" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="3:32" x14ac:dyDescent="0.35">
@@ -11233,14 +11417,14 @@
         <v>300</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H40" s="2"/>
       <c r="K40" s="11"/>
       <c r="L40" s="9"/>
       <c r="M40" s="2"/>
       <c r="AA40" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB40" s="85">
         <v>6</v>
@@ -11249,19 +11433,19 @@
         <v>11.3</v>
       </c>
       <c r="AD40" s="75" t="s">
+        <v>294</v>
+      </c>
+      <c r="AE40" s="75" t="s">
+        <v>299</v>
+      </c>
+      <c r="AF40" s="80" t="s">
         <v>295</v>
-      </c>
-      <c r="AE40" s="75" t="s">
-        <v>300</v>
-      </c>
-      <c r="AF40" s="80" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="41" spans="3:32" x14ac:dyDescent="0.35">
       <c r="C41" s="23"/>
       <c r="E41" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F41" s="9">
         <v>8.73</v>
@@ -11274,7 +11458,7 @@
       <c r="L41" s="9"/>
       <c r="M41" s="2"/>
       <c r="AA41" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB41" s="85">
         <v>5</v>
@@ -11283,13 +11467,13 @@
         <v>11.6</v>
       </c>
       <c r="AD41" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE41" s="75" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AF41" s="80" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="3:32" x14ac:dyDescent="0.35">
@@ -11307,7 +11491,7 @@
       <c r="L42" s="9"/>
       <c r="M42" s="2"/>
       <c r="AA42" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB42" s="85">
         <v>12</v>
@@ -11316,13 +11500,13 @@
         <v>11.6</v>
       </c>
       <c r="AD42" s="75" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AE42" s="75" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF42" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="3:32" x14ac:dyDescent="0.35">
@@ -11334,7 +11518,7 @@
       <c r="L43" s="9"/>
       <c r="M43" s="2"/>
       <c r="AA43" s="79" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB43" s="85">
         <v>4</v>
@@ -11343,13 +11527,13 @@
         <v>11.7</v>
       </c>
       <c r="AD43" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE43" s="75" t="s">
         <v>72</v>
       </c>
       <c r="AF43" s="80" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="3:32" x14ac:dyDescent="0.35">
@@ -11361,7 +11545,7 @@
       <c r="L44" s="9"/>
       <c r="M44" s="2"/>
       <c r="AA44" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB44" s="85">
         <v>4</v>
@@ -11370,7 +11554,7 @@
         <v>12.7</v>
       </c>
       <c r="AD44" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE44" s="75" t="s">
         <v>102</v>
@@ -11388,7 +11572,7 @@
       <c r="L45" s="9"/>
       <c r="M45" s="2"/>
       <c r="AA45" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB45" s="85">
         <v>12</v>
@@ -11397,7 +11581,7 @@
         <v>12.7</v>
       </c>
       <c r="AD45" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE45" s="75" t="s">
         <v>69</v>
@@ -11415,7 +11599,7 @@
       <c r="L46" s="9"/>
       <c r="M46" s="2"/>
       <c r="AA46" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB46" s="85">
         <v>5</v>
@@ -11424,13 +11608,13 @@
         <v>12.7</v>
       </c>
       <c r="AD46" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE46" s="75" t="s">
         <v>64</v>
       </c>
       <c r="AF46" s="80" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="47" spans="3:32" x14ac:dyDescent="0.35">
@@ -11442,7 +11626,7 @@
       <c r="L47" s="9"/>
       <c r="M47" s="2"/>
       <c r="AA47" s="79" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB47" s="85">
         <v>4</v>
@@ -11451,7 +11635,7 @@
         <v>12.9</v>
       </c>
       <c r="AD47" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE47" s="75" t="s">
         <v>72</v>
@@ -11469,7 +11653,7 @@
       <c r="L48" s="9"/>
       <c r="M48" s="2"/>
       <c r="AA48" s="79" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AB48" s="85">
         <v>1</v>
@@ -11478,7 +11662,7 @@
         <v>13.5</v>
       </c>
       <c r="AD48" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE48" s="75" t="s">
         <v>72</v>
@@ -11496,7 +11680,7 @@
       <c r="L49" s="9"/>
       <c r="M49" s="2"/>
       <c r="AA49" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB49" s="85">
         <v>10</v>
@@ -11505,13 +11689,13 @@
         <v>13.9</v>
       </c>
       <c r="AD49" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE49" s="75" t="s">
         <v>230</v>
       </c>
       <c r="AF49" s="80" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="5:32" x14ac:dyDescent="0.35">
@@ -11523,7 +11707,7 @@
       <c r="L50" s="9"/>
       <c r="M50" s="2"/>
       <c r="AA50" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB50" s="85">
         <v>8</v>
@@ -11532,13 +11716,13 @@
         <v>13.9</v>
       </c>
       <c r="AD50" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE50" s="75" t="s">
         <v>67</v>
       </c>
       <c r="AF50" s="80" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51" spans="5:32" x14ac:dyDescent="0.35">
@@ -11550,7 +11734,7 @@
       <c r="L51" s="9"/>
       <c r="M51" s="2"/>
       <c r="AA51" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB51" s="85">
         <v>28</v>
@@ -11559,13 +11743,13 @@
         <v>14.1</v>
       </c>
       <c r="AD51" s="75" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AE51" s="75" t="s">
         <v>87</v>
       </c>
       <c r="AF51" s="80" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11577,7 +11761,7 @@
       <c r="L52" s="10"/>
       <c r="M52" s="3"/>
       <c r="AA52" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB52" s="85">
         <v>5</v>
@@ -11586,18 +11770,18 @@
         <v>14.8</v>
       </c>
       <c r="AD52" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE52" s="75" t="s">
         <v>237</v>
       </c>
       <c r="AF52" s="80" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA53" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB53" s="85">
         <v>8</v>
@@ -11606,18 +11790,18 @@
         <v>15</v>
       </c>
       <c r="AD53" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE53" s="75" t="s">
         <v>70</v>
       </c>
       <c r="AF53" s="80" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="54" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA54" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB54" s="85">
         <v>2</v>
@@ -11626,7 +11810,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="AD54" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE54" s="75" t="s">
         <v>73</v>
@@ -11637,7 +11821,7 @@
     </row>
     <row r="55" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA55" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB55" s="85">
         <v>6</v>
@@ -11646,18 +11830,18 @@
         <v>18.100000000000001</v>
       </c>
       <c r="AD55" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE55" s="75" t="s">
         <v>53</v>
       </c>
       <c r="AF55" s="80" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA56" s="79" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB56" s="85">
         <v>2</v>
@@ -11666,18 +11850,18 @@
         <v>20.2</v>
       </c>
       <c r="AD56" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE56" s="75" t="s">
         <v>73</v>
       </c>
       <c r="AF56" s="80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA57" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB57" s="85">
         <v>2</v>
@@ -11686,7 +11870,7 @@
         <v>20.8</v>
       </c>
       <c r="AD57" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE57" s="75" t="s">
         <v>73</v>
@@ -11697,7 +11881,7 @@
     </row>
     <row r="58" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA58" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB58" s="85">
         <v>1</v>
@@ -11706,18 +11890,18 @@
         <v>22</v>
       </c>
       <c r="AD58" s="75" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AE58" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AF58" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA59" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB59" s="85">
         <v>4</v>
@@ -11726,10 +11910,10 @@
         <v>22.6</v>
       </c>
       <c r="AD59" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE59" s="75" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF59" s="80" t="s">
         <v>102</v>
@@ -11737,7 +11921,7 @@
     </row>
     <row r="60" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA60" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB60" s="85">
         <v>3</v>
@@ -11746,10 +11930,10 @@
         <v>23</v>
       </c>
       <c r="AD60" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE60" s="75" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF60" s="80" t="s">
         <v>53</v>
@@ -11757,7 +11941,7 @@
     </row>
     <row r="61" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA61" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB61" s="85">
         <v>6</v>
@@ -11766,7 +11950,7 @@
         <v>23.2</v>
       </c>
       <c r="AD61" s="75" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AE61" s="75" t="s">
         <v>103</v>
@@ -11777,7 +11961,7 @@
     </row>
     <row r="62" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA62" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB62" s="85">
         <v>6</v>
@@ -11786,18 +11970,18 @@
         <v>23.9</v>
       </c>
       <c r="AD62" s="75" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AE62" s="75" t="s">
         <v>103</v>
       </c>
       <c r="AF62" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA63" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB63" s="85">
         <v>5</v>
@@ -11806,18 +11990,18 @@
         <v>25.7</v>
       </c>
       <c r="AD63" s="75" t="s">
+        <v>350</v>
+      </c>
+      <c r="AE63" s="75" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF63" s="80" t="s">
         <v>351</v>
-      </c>
-      <c r="AE63" s="75" t="s">
-        <v>270</v>
-      </c>
-      <c r="AF63" s="80" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="64" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AA64" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB64" s="85">
         <v>12</v>
@@ -11826,18 +12010,18 @@
         <v>28.7</v>
       </c>
       <c r="AD64" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE64" s="75" t="s">
         <v>43</v>
       </c>
       <c r="AF64" s="80" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA65" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB65" s="85">
         <v>5</v>
@@ -11846,18 +12030,18 @@
         <v>30</v>
       </c>
       <c r="AD65" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="AE65" s="75" t="s">
         <v>322</v>
       </c>
-      <c r="AE65" s="75" t="s">
+      <c r="AF65" s="80" t="s">
         <v>323</v>
-      </c>
-      <c r="AF65" s="80" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="66" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA66" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB66" s="85">
         <v>10</v>
@@ -11866,7 +12050,7 @@
         <v>30</v>
       </c>
       <c r="AD66" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE66" s="75" t="s">
         <v>53</v>
@@ -11877,7 +12061,7 @@
     </row>
     <row r="67" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA67" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB67" s="85">
         <v>16</v>
@@ -11886,7 +12070,7 @@
         <v>30</v>
       </c>
       <c r="AD67" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE67" s="75" t="s">
         <v>43</v>
@@ -11906,18 +12090,18 @@
         <v>30.9</v>
       </c>
       <c r="AD68" s="75" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AE68" s="75" t="s">
         <v>19</v>
       </c>
       <c r="AF68" s="80" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="69" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA69" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB69" s="85">
         <v>3</v>
@@ -11926,7 +12110,7 @@
         <v>36.5</v>
       </c>
       <c r="AD69" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE69" s="75" t="s">
         <v>155</v>
@@ -11937,7 +12121,7 @@
     </row>
     <row r="70" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA70" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB70" s="85">
         <v>8</v>
@@ -11946,13 +12130,13 @@
         <v>38</v>
       </c>
       <c r="AD70" s="75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE70" s="75" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF70" s="80" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="27:32" x14ac:dyDescent="0.35">
@@ -11966,18 +12150,18 @@
         <v>39.299999999999997</v>
       </c>
       <c r="AD71" s="75" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AE71" s="75" t="s">
         <v>19</v>
       </c>
       <c r="AF71" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA72" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB72" s="85">
         <v>24</v>
@@ -11986,13 +12170,13 @@
         <v>41</v>
       </c>
       <c r="AD72" s="75" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AE72" s="75" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF72" s="80" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="73" spans="27:32" x14ac:dyDescent="0.35">
@@ -12006,18 +12190,18 @@
         <v>45.2</v>
       </c>
       <c r="AD73" s="75" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AE73" s="75" t="s">
         <v>19</v>
       </c>
       <c r="AF73" s="80" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA74" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB74" s="85">
         <v>2</v>
@@ -12026,10 +12210,10 @@
         <v>46.4</v>
       </c>
       <c r="AD74" s="75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE74" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF74" s="80" t="s">
         <v>155</v>
@@ -12037,7 +12221,7 @@
     </row>
     <row r="75" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA75" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB75" s="85">
         <v>2</v>
@@ -12046,18 +12230,18 @@
         <v>46.4</v>
       </c>
       <c r="AD75" s="75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE75" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AF75" s="80" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA76" s="79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AB76" s="85">
         <v>4</v>
@@ -12066,10 +12250,10 @@
         <v>48.5</v>
       </c>
       <c r="AD76" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE76" s="75" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AF76" s="80" t="s">
         <v>237</v>
@@ -12077,7 +12261,7 @@
     </row>
     <row r="77" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA77" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB77" s="85">
         <v>20</v>
@@ -12086,13 +12270,13 @@
         <v>51</v>
       </c>
       <c r="AD77" s="75" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AE77" s="75" t="s">
+        <v>353</v>
+      </c>
+      <c r="AF77" s="80" t="s">
         <v>354</v>
-      </c>
-      <c r="AF77" s="80" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="78" spans="27:32" x14ac:dyDescent="0.35">
@@ -12106,18 +12290,18 @@
         <v>56.6</v>
       </c>
       <c r="AD78" s="75" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AE78" s="75" t="s">
         <v>19</v>
       </c>
       <c r="AF78" s="80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="79" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA79" s="79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AB79" s="85">
         <v>8</v>
@@ -12126,18 +12310,18 @@
         <v>69.599999999999994</v>
       </c>
       <c r="AD79" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE79" s="75" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF79" s="80" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="80" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA80" s="79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AB80" s="85">
         <v>15</v>
@@ -12146,13 +12330,13 @@
         <v>73.900000000000006</v>
       </c>
       <c r="AD80" s="75" t="s">
+        <v>350</v>
+      </c>
+      <c r="AE80" s="75" t="s">
         <v>351</v>
       </c>
-      <c r="AE80" s="75" t="s">
+      <c r="AF80" s="80" t="s">
         <v>352</v>
-      </c>
-      <c r="AF80" s="80" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="81" spans="27:32" x14ac:dyDescent="0.35">
@@ -12166,7 +12350,7 @@
         <v>112.5</v>
       </c>
       <c r="AD81" s="75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AE81" s="75" t="s">
         <v>49</v>
@@ -12186,7 +12370,7 @@
         <v>118.7</v>
       </c>
       <c r="AD82" s="75" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE82" s="75" t="s">
         <v>61</v>
@@ -12206,7 +12390,7 @@
         <v>118.7</v>
       </c>
       <c r="AD83" s="75" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE83" s="75" t="s">
         <v>61</v>
@@ -12226,7 +12410,7 @@
         <v>134.30000000000001</v>
       </c>
       <c r="AD84" s="75" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE84" s="75" t="s">
         <v>20</v>
@@ -12246,7 +12430,7 @@
         <v>151.1</v>
       </c>
       <c r="AD85" s="75" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE85" s="75" t="s">
         <v>88</v>
@@ -12281,67 +12465,67 @@
     </row>
     <row r="89" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA89" s="79" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AB89" s="85">
         <v>1</v>
       </c>
       <c r="AC89" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="AD89" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="AE89" s="75" t="s">
+        <v>323</v>
+      </c>
+      <c r="AF89" s="80" t="s">
         <v>325</v>
-      </c>
-      <c r="AD89" s="75" t="s">
-        <v>322</v>
-      </c>
-      <c r="AE89" s="75" t="s">
-        <v>324</v>
-      </c>
-      <c r="AF89" s="80" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="90" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA90" s="79" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AB90" s="85">
         <v>2</v>
       </c>
       <c r="AC90" s="85" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD90" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="AE90" s="75" t="s">
         <v>329</v>
       </c>
-      <c r="AD90" s="75" t="s">
-        <v>322</v>
-      </c>
-      <c r="AE90" s="75" t="s">
-        <v>330</v>
-      </c>
       <c r="AF90" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA91" s="79" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AB91" s="85">
         <v>12</v>
       </c>
       <c r="AC91" s="75" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AD91" s="75" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AE91" s="75" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AF91" s="80" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="92" spans="27:32" x14ac:dyDescent="0.35">
       <c r="AA92" s="79" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AB92" s="85">
         <v>24</v>
@@ -12429,7 +12613,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -12437,7 +12621,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="29" x14ac:dyDescent="0.35">
@@ -12445,7 +12629,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -12459,7 +12643,7 @@
         <v>239</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -12467,7 +12651,7 @@
         <v>240</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -12475,7 +12659,7 @@
         <v>241</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -12483,7 +12667,7 @@
         <v>242</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
@@ -12491,7 +12675,7 @@
         <v>243</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
@@ -12499,23 +12683,23 @@
         <v>244</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12547,7 +12731,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>0</v>
@@ -12572,10 +12756,10 @@
         <v>33</v>
       </c>
       <c r="H17" s="71" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K17" s="8">
         <v>5</v>
@@ -12587,7 +12771,7 @@
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
       <c r="E18" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F18" s="9">
         <v>3000</v>
@@ -12597,7 +12781,7 @@
       </c>
       <c r="H18" s="2"/>
       <c r="J18" s="38" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K18" s="9">
         <v>1.75</v>
@@ -12620,7 +12804,7 @@
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="38" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K19" s="9">
         <v>2.91</v>
@@ -12642,7 +12826,7 @@
       </c>
       <c r="H20" s="2"/>
       <c r="J20" s="38" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K20" s="9">
         <v>2.83</v>
@@ -12661,11 +12845,11 @@
         <v>21.837037037037035</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H21" s="2"/>
       <c r="J21" s="38" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K21" s="9">
         <f>857+17/90-K22-K23</f>
@@ -12685,17 +12869,17 @@
         <v>543.62222222222226</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H22" s="2"/>
       <c r="J22" s="38" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K22" s="9">
         <v>80</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.35">
@@ -12705,13 +12889,13 @@
       <c r="G23" s="6"/>
       <c r="H23" s="2"/>
       <c r="J23" s="38" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K23" s="9">
         <v>760</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.35">
@@ -12999,7 +13183,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="87" x14ac:dyDescent="0.35">
@@ -13007,7 +13191,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -13027,7 +13211,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -13035,7 +13219,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -13043,7 +13227,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13051,7 +13235,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13080,7 +13264,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>0</v>
@@ -13105,7 +13289,7 @@
       </c>
       <c r="H13" s="89"/>
       <c r="J13" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K13" s="8">
         <v>4</v>
@@ -13176,7 +13360,7 @@
         <v>33</v>
       </c>
       <c r="H17" s="80" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="9"/>
@@ -13201,13 +13385,13 @@
     <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
       <c r="E19" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F19" s="9">
         <v>80</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H19" s="80"/>
       <c r="J19" s="4"/>
@@ -13227,7 +13411,7 @@
         <v>55</v>
       </c>
       <c r="H20" s="80" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="9"/>
@@ -13243,7 +13427,7 @@
         <v>128.33333333333334</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H21" s="80"/>
       <c r="J21" s="2"/>
@@ -13260,7 +13444,7 @@
         <v>146.41333333333333</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H22" s="80"/>
       <c r="J22" s="2"/>
@@ -13277,7 +13461,7 @@
         <v>172.6</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H23" s="80"/>
       <c r="J23" s="2"/>
@@ -13540,7 +13724,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="29" x14ac:dyDescent="0.35">
@@ -13548,7 +13732,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
@@ -13562,7 +13746,7 @@
         <v>239</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
@@ -13570,15 +13754,15 @@
         <v>240</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
@@ -13586,7 +13770,7 @@
         <v>242</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.35">
@@ -13594,15 +13778,15 @@
         <v>243</v>
       </c>
       <c r="C9" s="99" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="22" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13619,7 +13803,7 @@
       <c r="K11" s="102"/>
       <c r="L11" s="103"/>
       <c r="N11" s="118" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O11" s="119"/>
       <c r="P11" s="119"/>
@@ -13638,7 +13822,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>0</v>
@@ -13650,19 +13834,19 @@
         <v>24</v>
       </c>
       <c r="N12" s="90" t="s">
+        <v>287</v>
+      </c>
+      <c r="O12" s="91" t="s">
+        <v>430</v>
+      </c>
+      <c r="P12" s="91" t="s">
         <v>288</v>
       </c>
-      <c r="O12" s="91" t="s">
-        <v>431</v>
-      </c>
-      <c r="P12" s="91" t="s">
-        <v>289</v>
-      </c>
       <c r="Q12" s="91" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R12" s="92" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.35">
@@ -13674,11 +13858,11 @@
         <v>281.7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H13" s="89"/>
       <c r="J13" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K13" s="8">
         <f>597-K19</f>
@@ -13688,7 +13872,7 @@
         <v>25</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O13" s="19">
         <v>9</v>
@@ -13701,7 +13885,7 @@
         <v>4500</v>
       </c>
       <c r="R13" s="41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.35">
@@ -13717,7 +13901,7 @@
       </c>
       <c r="H14" s="80"/>
       <c r="J14" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K14" s="9">
         <v>72.25</v>
@@ -13726,7 +13910,7 @@
         <v>25</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O14" s="2">
         <v>1</v>
@@ -13739,7 +13923,7 @@
         <v>341</v>
       </c>
       <c r="R14" s="40" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.35">
@@ -13749,7 +13933,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="80"/>
       <c r="J15" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K15" s="9">
         <v>13.2</v>
@@ -13758,7 +13942,7 @@
         <v>8</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O15" s="2">
         <v>36</v>
@@ -13771,7 +13955,7 @@
         <v>7862.4000000000005</v>
       </c>
       <c r="R15" s="40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.35">
@@ -13781,7 +13965,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="80"/>
       <c r="J16" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K16" s="9">
         <v>0.1</v>
@@ -13790,7 +13974,7 @@
         <v>8</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O16" s="2">
         <v>4</v>
@@ -13804,7 +13988,7 @@
         <v>3884.8</v>
       </c>
       <c r="R16" s="40" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17" spans="3:18" x14ac:dyDescent="0.35">
@@ -13824,7 +14008,7 @@
         <v>8</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O17" s="2">
         <v>8</v>
@@ -13838,7 +14022,7 @@
         <v>5784.8</v>
       </c>
       <c r="R17" s="40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.35">
@@ -13848,7 +14032,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="80"/>
       <c r="J18" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K18" s="9">
         <v>1</v>
@@ -13857,7 +14041,7 @@
         <v>8</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O18" s="2">
         <v>8</v>
@@ -13871,7 +14055,7 @@
         <v>776.8</v>
       </c>
       <c r="R18" s="40" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.35">
@@ -13881,17 +14065,17 @@
       <c r="G19" s="6"/>
       <c r="H19" s="80"/>
       <c r="J19" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K19" s="9">
         <f>140+4/9</f>
         <v>140.44444444444446</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O19" s="2">
         <v>8</v>
@@ -13905,7 +14089,7 @@
         <v>282</v>
       </c>
       <c r="R19" s="40" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.35">
@@ -13918,7 +14102,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="4"/>
       <c r="N20" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O20" s="2">
         <v>8</v>
@@ -13932,7 +14116,7 @@
         <v>5541.6</v>
       </c>
       <c r="R20" s="40" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.35">
@@ -13945,7 +14129,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="4"/>
       <c r="N21" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O21" s="2">
         <v>4</v>
@@ -13959,7 +14143,7 @@
         <v>2063</v>
       </c>
       <c r="R21" s="40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="22" spans="3:18" x14ac:dyDescent="0.35">
@@ -13972,7 +14156,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="4"/>
       <c r="N22" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O22" s="2">
         <v>6</v>
@@ -13986,7 +14170,7 @@
         <v>3557.1000000000004</v>
       </c>
       <c r="R22" s="40" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.35">
@@ -13999,7 +14183,7 @@
       <c r="K23" s="9"/>
       <c r="L23" s="4"/>
       <c r="N23" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O23" s="2">
         <v>2</v>
@@ -14013,7 +14197,7 @@
         <v>257.90000000000003</v>
       </c>
       <c r="R23" s="40" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.35">
@@ -14026,7 +14210,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="4"/>
       <c r="N24" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O24" s="2">
         <v>3</v>
@@ -14040,7 +14224,7 @@
         <v>1324.1999999999998</v>
       </c>
       <c r="R24" s="40" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.35">
@@ -14053,7 +14237,7 @@
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
       <c r="N25" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="O25" s="2">
         <v>2</v>
@@ -14077,7 +14261,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
       <c r="N26" s="94" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O26" s="3">
         <v>4</v>
@@ -14101,7 +14285,7 @@
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
       <c r="N27" s="93" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O27" s="122">
         <f>SUM(Q13:Q26)</f>
@@ -14298,8 +14482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC07E90-6101-47F8-9701-BB9D283EFF37}">
   <dimension ref="B1:L47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14308,9 +14492,9 @@
     <col min="3" max="3" width="20.453125" customWidth="1"/>
     <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -14321,7 +14505,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="76" customHeight="1" x14ac:dyDescent="0.35">
@@ -14329,7 +14513,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -14352,13 +14536,13 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C7" s="25"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C8" s="25"/>
     </row>
@@ -14376,13 +14560,13 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="100" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C11" s="99"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C12" s="26"/>
     </row>
@@ -14412,7 +14596,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>0</v>
@@ -14427,7 +14611,7 @@
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
       <c r="E15" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F15" s="8">
         <f>4+64/75</f>
@@ -14438,7 +14622,7 @@
       </c>
       <c r="H15" s="89"/>
       <c r="J15" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K15" s="8">
         <f>364/1215</f>
@@ -14460,7 +14644,7 @@
         <v>62</v>
       </c>
       <c r="H16" s="80" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>86</v>
@@ -14486,7 +14670,7 @@
         <v>62</v>
       </c>
       <c r="H17" s="80" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>87</v>
@@ -14502,16 +14686,16 @@
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
       <c r="E18" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F18" s="9">
         <v>760</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H18" s="80" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>88</v>
@@ -14533,10 +14717,10 @@
         <v>280.88888888888891</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H19" s="80" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>61</v>
@@ -14552,17 +14736,17 @@
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
       <c r="E20" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F20" s="9">
         <f>140+4/9</f>
         <v>140.44444444444446</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H20" s="80" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>34</v>
@@ -14586,7 +14770,7 @@
         <v>60</v>
       </c>
       <c r="H21" s="80" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>41</v>
@@ -14613,9 +14797,16 @@
       <c r="H22" s="80" t="s">
         <v>230</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="4"/>
+      <c r="J22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="9">
+        <f>759+971/1350</f>
+        <v>759.71925925925927</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -14632,9 +14823,15 @@
       <c r="H23" s="80" t="s">
         <v>230</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="4"/>
+      <c r="J23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="9">
+        <v>5</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -14651,9 +14848,16 @@
       <c r="H24" s="80" t="s">
         <v>230</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="4"/>
+      <c r="J24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K24" s="9">
+        <f>996+25/36</f>
+        <v>996.69444444444446</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -14668,11 +14872,17 @@
         <v>62</v>
       </c>
       <c r="H25" s="80" t="s">
-        <v>462</v>
-      </c>
-      <c r="J25" s="2"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="4"/>
+        <v>461</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="K25" s="9">
+        <v>5</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -14686,11 +14896,17 @@
         <v>60</v>
       </c>
       <c r="H26" s="80" t="s">
-        <v>462</v>
-      </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="4"/>
+        <v>461</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K26" s="9">
+        <v>5</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -14704,78 +14920,154 @@
         <v>60</v>
       </c>
       <c r="H27" s="80" t="s">
-        <v>462</v>
-      </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="4"/>
+        <v>461</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" s="9">
+        <v>3.75</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="80"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="4"/>
+      <c r="E28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="9">
+        <f>367+10/13</f>
+        <v>367.76923076923077</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="80" t="s">
+        <v>471</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="9">
+        <v>590</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="80"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="4"/>
+      <c r="E29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="9">
+        <f>1411+21/52-712-3.75</f>
+        <v>695.65384615384619</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="80" t="s">
+        <v>471</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="K29" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="80"/>
+      <c r="E30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="9">
+        <v>200</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" s="80" t="s">
+        <v>471</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="9"/>
       <c r="L30" s="4"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="80"/>
+      <c r="E31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1200</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="80" t="s">
+        <v>471</v>
+      </c>
       <c r="J31" s="2"/>
       <c r="K31" s="9"/>
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="80"/>
+      <c r="E32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="9">
+        <v>600</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="80" t="s">
+        <v>471</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="9"/>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C33" s="23"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="80"/>
+      <c r="E33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1200</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="80" t="s">
+        <v>471</v>
+      </c>
       <c r="J33" s="2"/>
       <c r="K33" s="9"/>
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C34" s="23"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="80"/>
+      <c r="E34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H34" s="80" t="s">
+        <v>471</v>
+      </c>
       <c r="J34" s="2"/>
       <c r="K34" s="9"/>
       <c r="L34" s="2"/>
@@ -14956,7 +15248,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.35">
@@ -15254,7 +15546,7 @@
         <v>41.870370370370374</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N24" s="2"/>
       <c r="P24" s="104"/>
@@ -15276,10 +15568,10 @@
         <v>30.94650205761317</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="P25" s="104"/>
       <c r="Q25" s="104"/>
@@ -15299,11 +15591,11 @@
         <v>997.25</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N26" s="2"/>
       <c r="P26" s="104" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q26" s="104"/>
       <c r="R26" s="104"/>
@@ -15365,7 +15657,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="P30" s="104" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q30" s="104"/>
       <c r="R30" s="104"/>
@@ -15427,7 +15719,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="P34" s="104" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Q34" s="104"/>
       <c r="R34" s="104"/>
@@ -15631,7 +15923,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -15858,7 +16150,7 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.35">
@@ -16122,7 +16414,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
@@ -16644,7 +16936,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="2"/>
       <c r="O35" s="104" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P35" s="104"/>
       <c r="Q35" s="104"/>
@@ -16821,7 +17113,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
@@ -16902,7 +17194,7 @@
         <v>24</v>
       </c>
       <c r="M12" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O12" s="104" t="s">
         <v>84</v>
@@ -16985,7 +17277,7 @@
         <v>198</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O15" s="104"/>
       <c r="P15" s="104"/>
@@ -17009,7 +17301,7 @@
         <v>219</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
@@ -17027,7 +17319,7 @@
         <v>232</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -17046,7 +17338,7 @@
         <v>254</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -17065,7 +17357,7 @@
         <v>254</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O19" s="115" t="s">
         <v>147</v>
@@ -17089,13 +17381,13 @@
         <v>111.77777777777777</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O20" s="106" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P20" s="107"/>
       <c r="Q20" s="107"/>
@@ -17145,7 +17437,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
       <c r="O23" s="106" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P23" s="107"/>
       <c r="Q23" s="107"/>
@@ -17999,7 +18291,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
@@ -18309,7 +18601,7 @@
         <v>146.3777</v>
       </c>
       <c r="L22" s="87" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N22" s="105" t="s">
         <v>147</v>
@@ -18332,7 +18624,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="87" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.35">
@@ -18344,7 +18636,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="87"/>
       <c r="N24" s="104" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="O24" s="104"/>
       <c r="P24" s="104"/>

</xml_diff>

<commit_message>
Updated spreadsheet, added a couple of blueprints
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 5\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 6\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3289504-0E2B-44A5-8BBA-6D0E3004806B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C51BA1-F794-4B30-AC56-9A75A914CD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="16" activeTab="23" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="21" activeTab="23" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="488">
   <si>
     <t>Item</t>
   </si>
@@ -1495,10 +1495,34 @@
     <t>Kaladesh Refinery, Xantcha's Crucible, Oran-Rief Mines, Ketria Crystals, Riveteers District, Aetherflux Reactor</t>
   </si>
   <si>
-    <t>Tollarian Metldown, Jund Pyroclast, Urabrask Refinery, Kaladesh Refinery, Riveteers District, Phyrexian Datavault</t>
-  </si>
-  <si>
     <t>Alclad Aluminum Sheets</t>
+  </si>
+  <si>
+    <t>Singularity Cells</t>
+  </si>
+  <si>
+    <t>Dark Matter Crystals</t>
+  </si>
+  <si>
+    <t>Ydris' Nexus</t>
+  </si>
+  <si>
+    <t>Tollarian Metldown, Jund Pyroclast, Urabrask Refinery, Kaladesh Refinery, Riveteers District, Phyrexian Datavault, Ydri's Nexus</t>
+  </si>
+  <si>
+    <t>Packaged Oil</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Raw Quarts</t>
+  </si>
+  <si>
+    <t>MIners</t>
+  </si>
+  <si>
+    <t>Singularity Cells Module</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1563,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -2212,11 +2236,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2491,6 +2537,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2825,10 +2885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
-  <dimension ref="B2:T124"/>
+  <dimension ref="B2:T129"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3216,7 +3276,7 @@
         <v>448</v>
       </c>
       <c r="D22" s="11">
-        <v>72.25</v>
+        <v>2.25</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>418</v>
@@ -3236,8 +3296,8 @@
         <v>86</v>
       </c>
       <c r="D23" s="9">
-        <f>'Aetherflux Reactor'!K16</f>
-        <v>398.18666666666667</v>
+        <f>'Aetherflux Reactor'!K17</f>
+        <v>537.22400000000005</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>450</v>
@@ -3257,8 +3317,8 @@
         <v>87</v>
       </c>
       <c r="D24" s="9">
-        <f>'Aetherflux Reactor'!K17</f>
-        <v>537.22400000000005</v>
+        <f>'Aetherflux Reactor'!K18</f>
+        <v>5</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>450</v>
@@ -3357,9 +3417,15 @@
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C29" s="6"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="40"/>
+      <c r="C29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="11">
+        <v>194</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>450</v>
+      </c>
       <c r="H29" s="6" t="s">
         <v>99</v>
       </c>
@@ -4353,21 +4419,34 @@
       <c r="I110" s="11">
         <v>30</v>
       </c>
-      <c r="J110" s="40" t="s">
-        <v>8</v>
+      <c r="J110" s="4" t="s">
+        <v>450</v>
       </c>
       <c r="P110" s="1"/>
     </row>
     <row r="111" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H111" s="6"/>
-      <c r="I111" s="11"/>
-      <c r="J111" s="40"/>
+      <c r="H111" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="I111" s="9">
+        <v>15</v>
+      </c>
+      <c r="J111" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="P111" s="1"/>
     </row>
     <row r="112" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="H112" s="6"/>
-      <c r="I112" s="11"/>
-      <c r="J112" s="40"/>
+      <c r="H112" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="I112" s="9">
+        <f>14+2/3</f>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="J112" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="P112" s="1"/>
     </row>
     <row r="113" spans="4:16" x14ac:dyDescent="0.35">
@@ -4391,13 +4470,72 @@
       <c r="I116" s="44"/>
       <c r="J116" s="42"/>
     </row>
+    <row r="121" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="F121" s="132"/>
+      <c r="G121" s="133"/>
+      <c r="H121" s="132"/>
+      <c r="I121" s="133"/>
+      <c r="J121" s="132"/>
+    </row>
+    <row r="122" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="F122" s="132"/>
+      <c r="G122" s="133"/>
+      <c r="H122" s="132"/>
+      <c r="I122" s="133"/>
+      <c r="J122" s="132"/>
+    </row>
     <row r="123" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D123"/>
       <c r="E123" s="1"/>
+      <c r="F123" s="132"/>
+      <c r="G123" s="133"/>
+      <c r="H123" s="132"/>
+      <c r="I123" s="133"/>
+      <c r="J123" s="132"/>
     </row>
     <row r="124" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D124"/>
       <c r="E124" s="1"/>
+      <c r="F124" s="132"/>
+      <c r="G124" s="132"/>
+      <c r="H124" s="132"/>
+      <c r="I124" s="133"/>
+      <c r="J124" s="132"/>
+    </row>
+    <row r="125" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="F125" s="132"/>
+      <c r="G125" s="132"/>
+      <c r="H125" s="132"/>
+      <c r="I125" s="133"/>
+      <c r="J125" s="132"/>
+    </row>
+    <row r="126" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="F126" s="132"/>
+      <c r="G126" s="132"/>
+      <c r="H126" s="132"/>
+      <c r="I126" s="133"/>
+      <c r="J126" s="132"/>
+    </row>
+    <row r="127" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="F127" s="132"/>
+      <c r="G127" s="132"/>
+      <c r="H127" s="132"/>
+      <c r="I127" s="133"/>
+      <c r="J127" s="132"/>
+    </row>
+    <row r="128" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="F128" s="132"/>
+      <c r="G128" s="132"/>
+      <c r="H128" s="132"/>
+      <c r="I128" s="133"/>
+      <c r="J128" s="132"/>
+    </row>
+    <row r="129" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F129" s="132"/>
+      <c r="G129" s="132"/>
+      <c r="H129" s="132"/>
+      <c r="I129" s="133"/>
+      <c r="J129" s="132"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:E18">
@@ -13625,8 +13763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878EF637-2B1F-4BC8-A0FA-F77EC5044F15}">
   <dimension ref="B1:R45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13833,7 +13971,7 @@
         <v>448</v>
       </c>
       <c r="K14" s="9">
-        <v>72.25</v>
+        <v>2.25</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>25</v>
@@ -14027,9 +14165,15 @@
       <c r="F20" s="9"/>
       <c r="G20" s="6"/>
       <c r="H20" s="80"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="4"/>
+      <c r="J20" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="K20" s="9">
+        <v>70</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="N20" s="6" t="s">
         <v>429</v>
       </c>
@@ -14409,10 +14553,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC07E90-6101-47F8-9701-BB9D283EFF37}">
-  <dimension ref="B1:L47"/>
+  <dimension ref="B1:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14437,12 +14581,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B3" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -14515,16 +14659,16 @@
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="88" t="s">
+      <c r="G14" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="52" t="s">
+      <c r="H14" s="55" t="s">
         <v>406</v>
       </c>
       <c r="J14" s="14" t="s">
@@ -14539,17 +14683,17 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="46" t="s">
         <v>361</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="43">
         <f>4+64/75</f>
         <v>4.8533333333333335</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="137" t="s">
         <v>252</v>
       </c>
-      <c r="H15" s="89"/>
+      <c r="H15" s="19"/>
       <c r="J15" s="4" t="s">
         <v>455</v>
       </c>
@@ -14563,17 +14707,18 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
-      <c r="E16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="9">
-        <v>11648</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="80" t="s">
-        <v>454</v>
+      <c r="E16" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="F16" s="11">
+        <f>242+2/3</f>
+        <v>242.66666666666666</v>
+      </c>
+      <c r="G16" s="96" t="s">
+        <v>481</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>86</v>
@@ -14588,18 +14733,17 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="9">
-        <f>5752+8/81</f>
-        <v>5752.0987654320988</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="11">
+        <v>11648</v>
+      </c>
+      <c r="G17" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="80" t="s">
-        <v>453</v>
+      <c r="H17" s="2" t="s">
+        <v>454</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>87</v>
@@ -14614,17 +14758,18 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
-      <c r="E18" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="F18" s="9">
-        <v>760</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="H18" s="80" t="s">
-        <v>461</v>
+      <c r="E18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="11">
+        <f>5752+8/81</f>
+        <v>5752.0987654320988</v>
+      </c>
+      <c r="G18" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>88</v>
@@ -14638,18 +14783,17 @@
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
-      <c r="E19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F19" s="9">
-        <f>280 + 8/9</f>
-        <v>280.88888888888891</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="H19" s="80" t="s">
+      <c r="E19" s="6" t="s">
         <v>458</v>
+      </c>
+      <c r="F19" s="11">
+        <v>760</v>
+      </c>
+      <c r="G19" s="96" t="s">
+        <v>377</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>461</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>61</v>
@@ -14664,42 +14808,43 @@
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="11">
+        <f>280 + 8/9</f>
+        <v>280.88888888888891</v>
+      </c>
+      <c r="G20" s="96" t="s">
+        <v>384</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="9">
+        <v>45</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="23"/>
+      <c r="E21" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F21" s="11">
         <f>140+4/9</f>
         <v>140.44444444444446</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G21" s="96" t="s">
         <v>465</v>
       </c>
-      <c r="H20" s="80" t="s">
+      <c r="H21" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="9">
-        <v>45</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C21" s="23"/>
-      <c r="E21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="9">
-        <v>600</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="80" t="s">
-        <v>462</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>41</v>
@@ -14713,68 +14858,67 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="11">
+        <v>600</v>
+      </c>
+      <c r="G22" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="9">
+        <f>745+71/1350</f>
+        <v>745.05259259259265</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="23"/>
+      <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F23" s="11">
         <f>34+2/3</f>
         <v>34.666666666666664</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G23" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="H22" s="80" t="s">
+      <c r="H23" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="9">
-        <f>759+971/1350</f>
-        <v>759.71925925925927</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C23" s="23"/>
-      <c r="E23" s="2" t="s">
+      <c r="K23" s="9">
+        <v>5</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="23"/>
+      <c r="E24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F24" s="11">
         <f>597+13/15</f>
         <v>597.86666666666667</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G24" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="80" t="s">
-        <v>228</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K23" s="9">
-        <v>5</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C24" s="23"/>
-      <c r="E24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="9">
-        <f>299+1/15</f>
-        <v>299.06666666666666</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="80" t="s">
+      <c r="H24" s="2" t="s">
         <v>228</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -14790,41 +14934,42 @@
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="11">
+        <f>299+1/15</f>
+        <v>299.06666666666666</v>
+      </c>
+      <c r="G25" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="K25" s="9">
+        <v>5</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="23"/>
+      <c r="E26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F26" s="11">
         <f>333+1/3</f>
         <v>333.33333333333331</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G26" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="80" t="s">
-        <v>456</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="K25" s="9">
-        <v>5</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C26" s="23"/>
-      <c r="E26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" s="9">
-        <v>1800</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="80" t="s">
+      <c r="H26" s="2" t="s">
         <v>456</v>
       </c>
       <c r="J26" s="2" t="s">
@@ -14839,16 +14984,16 @@
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
-      <c r="E27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="9">
-        <v>2000</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="E27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="11">
+        <v>1800</v>
+      </c>
+      <c r="G27" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="80" t="s">
+      <c r="H27" s="2" t="s">
         <v>456</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -14863,66 +15008,66 @@
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="11">
+        <v>2000</v>
+      </c>
+      <c r="G28" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="9">
+        <v>590</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="23"/>
+      <c r="E29" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F29" s="11">
         <f>367+10/13</f>
         <v>367.76923076923077</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G29" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="80" t="s">
+      <c r="H29" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="9">
-        <v>590</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C29" s="23"/>
-      <c r="E29" s="2" t="s">
+      <c r="J29" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K29" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="23"/>
+      <c r="E30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F30" s="11">
         <f>1411+21/52-712-3.75</f>
         <v>695.65384615384619</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G30" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="80" t="s">
-        <v>466</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="K29" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C30" s="23"/>
-      <c r="E30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="9">
-        <v>200</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H30" s="80" t="s">
+      <c r="H30" s="2" t="s">
         <v>466</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -14937,16 +15082,16 @@
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="9">
-        <v>1200</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="80" t="s">
+      <c r="F31" s="11">
+        <v>200</v>
+      </c>
+      <c r="G31" s="96" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>466</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -14962,72 +15107,90 @@
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
-      <c r="E32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="9">
-        <v>600</v>
-      </c>
-      <c r="G32" s="6" t="s">
+      <c r="E32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="11">
+        <v>1200</v>
+      </c>
+      <c r="G32" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="80" t="s">
+      <c r="H32" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="4"/>
+      <c r="J32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K32" s="9">
+        <v>194</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C33" s="23"/>
-      <c r="E33" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="9">
-        <v>1200</v>
-      </c>
-      <c r="G33" s="6" t="s">
+      <c r="E33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="11">
+        <v>600</v>
+      </c>
+      <c r="G33" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="80" t="s">
+      <c r="H33" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="K33" s="9">
+        <v>15</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C34" s="23"/>
-      <c r="E34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H34" s="80" t="s">
+      <c r="E34" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="11">
+        <v>1200</v>
+      </c>
+      <c r="G34" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="J34" s="2"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="2"/>
+      <c r="J34" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="K34" s="9">
+        <f>14+2/3</f>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C35" s="23"/>
-      <c r="E35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="9">
-        <f>226+13834/50625</f>
-        <v>226.27326419753086</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H35" s="80" t="s">
-        <v>462</v>
+      <c r="E35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="G35" s="96" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>466</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="9"/>
@@ -15035,18 +15198,18 @@
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
-      <c r="E36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="9">
-        <f>30+718/1755</f>
-        <v>30.40911680911681</v>
-      </c>
-      <c r="G36" s="6" t="s">
+      <c r="E36" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="11">
+        <f>226+13834/50625</f>
+        <v>226.27326419753086</v>
+      </c>
+      <c r="G36" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="H36" s="80" t="s">
-        <v>474</v>
+      <c r="H36" s="2" t="s">
+        <v>462</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="9"/>
@@ -15054,17 +15217,17 @@
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C37" s="23"/>
-      <c r="E37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="9">
-        <f>1880+23059/315900-1411-21/52</f>
-        <v>468.66914846470405</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="80" t="s">
+      <c r="E37" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="11">
+        <f>30+718/1755</f>
+        <v>30.40911680911681</v>
+      </c>
+      <c r="G37" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>474</v>
       </c>
       <c r="J37" s="2"/>
@@ -15073,16 +15236,17 @@
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C38" s="23"/>
-      <c r="E38" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F38" s="9">
-        <v>1650</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="H38" s="80" t="s">
+      <c r="E38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="11">
+        <f>17+661/1775+66+3122/6075+385+98/225</f>
+        <v>469.32185938677333</v>
+      </c>
+      <c r="G38" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>474</v>
       </c>
       <c r="J38" s="2"/>
@@ -15091,52 +15255,54 @@
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C39" s="23"/>
-      <c r="E39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="9">
-        <f>64+628/1875+57+1/15+93+291/375</f>
-        <v>215.17760000000001</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H39" s="80" t="s">
-        <v>476</v>
+      <c r="E39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="11">
+        <f>462+392/1125</f>
+        <v>462.34844444444445</v>
+      </c>
+      <c r="G39" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="9"/>
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E40" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F40" s="9">
-        <v>7</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H40" s="80" t="s">
-        <v>476</v>
+      <c r="C40" s="23"/>
+      <c r="E40" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" s="11">
+        <v>1650</v>
+      </c>
+      <c r="G40" s="96" t="s">
+        <v>475</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="9"/>
       <c r="L40" s="2"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E41" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F41" s="9">
-        <f>114+2/15</f>
-        <v>114.13333333333334</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H41" s="80" t="s">
+      <c r="C41" s="23"/>
+      <c r="E41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="11">
+        <f>64+628/1875+57+1/15+93+221/375</f>
+        <v>214.99093333333334</v>
+      </c>
+      <c r="G41" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>476</v>
       </c>
       <c r="J41" s="2"/>
@@ -15144,65 +15310,433 @@
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E42" s="2"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="80"/>
+      <c r="E42" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="11">
+        <v>7</v>
+      </c>
+      <c r="G42" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="9"/>
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E43" s="2"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="80"/>
+      <c r="E43" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="F43" s="11">
+        <f>114+2/15</f>
+        <v>114.13333333333334</v>
+      </c>
+      <c r="G43" s="96" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="9"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E44" s="2"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="80"/>
+      <c r="E44" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="11">
+        <f>300+600+1200</f>
+        <v>2100</v>
+      </c>
+      <c r="G44" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="J44" s="2"/>
       <c r="K44" s="9"/>
       <c r="L44" s="2"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E45" s="2"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="80"/>
+      <c r="E45" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" s="11">
+        <v>3812</v>
+      </c>
+      <c r="G45" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="9"/>
       <c r="L45" s="2"/>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="E46" s="2"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="80"/>
+      <c r="E46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="11">
+        <f>3812+513+2/13</f>
+        <v>4325.1538461538457</v>
+      </c>
+      <c r="G46" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="J46" s="2"/>
       <c r="K46" s="9"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E47" s="3"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="83"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="3"/>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="11">
+        <f>293+3/13+1588+1/3</f>
+        <v>1881.5641025641025</v>
+      </c>
+      <c r="G47" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="J47" s="2"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E48" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="F48" s="11">
+        <v>70</v>
+      </c>
+      <c r="G48" s="96" t="s">
+        <v>481</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="J48" s="2"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="11">
+        <v>300</v>
+      </c>
+      <c r="G49" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="J49" s="3"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E50" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="F50" s="2">
+        <f>71+1/3</f>
+        <v>71.333333333333329</v>
+      </c>
+      <c r="G50" s="96" t="s">
+        <v>481</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="51" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E51" s="94"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="97"/>
+      <c r="H51" s="67"/>
+    </row>
+    <row r="52" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E52" s="118" t="s">
+        <v>484</v>
+      </c>
+      <c r="F52" s="119"/>
+      <c r="G52" s="119"/>
+      <c r="H52" s="120"/>
+    </row>
+    <row r="53" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E53" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G53" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H53" s="52" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E54" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F54" s="4">
+        <f>4+64/75</f>
+        <v>4.8533333333333335</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E55" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="2">
+        <f>F18+F19+F25+F27+F31+F39+F42+F48</f>
+        <v>9350.5138765432093</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E56" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F56" s="2">
+        <v>760</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E57" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F57" s="11">
+        <f>280 + 8/9</f>
+        <v>280.88888888888891</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E58" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F58" s="2">
+        <f>F51+F22+F17</f>
+        <v>12248</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E59" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="2">
+        <v>600</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="2">
+        <f>F24+F36</f>
+        <v>824.13993086419759</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" s="2">
+        <f>F26+F30+F38+F47</f>
+        <v>3379.8731414380554</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E62" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1800</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E63" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F63" s="2">
+        <f>F29+F45+F40</f>
+        <v>5829.7692307692305</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1400</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="2">
+        <v>600</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E66" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1200</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" s="2">
+        <f>F46+F37</f>
+        <v>4355.562962962963</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E68" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1650</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F69" s="2">
+        <v>7</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E70" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="F70" s="11">
+        <f>114+2/15</f>
+        <v>114.13333333333334</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E71" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="F71" s="2">
+        <v>70</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="3">
+        <v>300</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H72" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="J13:L13"/>
+    <mergeCell ref="E52:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated savefile, Spreadsheet, and added all of the diagrams as jpg. WE HAVE FICSONIUM NUCLEAR POWER!
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 6\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C51BA1-F794-4B30-AC56-9A75A914CD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F867011-79E7-4E0E-9B32-84D22445469B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="21" activeTab="23" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="504">
   <si>
     <t>Item</t>
   </si>
@@ -1507,9 +1507,6 @@
     <t>Ydris' Nexus</t>
   </si>
   <si>
-    <t>Tollarian Metldown, Jund Pyroclast, Urabrask Refinery, Kaladesh Refinery, Riveteers District, Phyrexian Datavault, Ydri's Nexus</t>
-  </si>
-  <si>
     <t>Packaged Oil</t>
   </si>
   <si>
@@ -1523,6 +1520,57 @@
   </si>
   <si>
     <t>Singularity Cells Module</t>
+  </si>
+  <si>
+    <t>Tollarian Metldown, Jund Pyroclast, Urabrask Refinery, Kaladesh Refinery, Riveteers District, Phyrexian Datavault, Ydri's Nexus, The Mirrodin Trigon</t>
+  </si>
+  <si>
+    <t>10.6 GW/h</t>
+  </si>
+  <si>
+    <t>10.4 GW/h</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unstable Consumptions</t>
+  </si>
+  <si>
+    <t>Dark Matter Residue for Ficsonium</t>
+  </si>
+  <si>
+    <t>Total Consumption</t>
+  </si>
+  <si>
+    <t>Ficsonium</t>
+  </si>
+  <si>
+    <t>Excited Photonic Matter for Ficsonium Fuel Rods</t>
+  </si>
+  <si>
+    <t>Trigon Module</t>
+  </si>
+  <si>
+    <t>Dark Matter Residue</t>
+  </si>
+  <si>
+    <t>19,329.2 MW</t>
+  </si>
+  <si>
+    <t>90,625.514 MW</t>
+  </si>
+  <si>
+    <t>71,296.31 MW</t>
+  </si>
+  <si>
+    <t>31,929.55 MW.</t>
+  </si>
+  <si>
+    <t>58,695.96 MW</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1611,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2258,11 +2306,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2444,6 +2529,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2537,20 +2629,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2885,10 +2984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
-  <dimension ref="B2:T129"/>
+  <dimension ref="B2:T124"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2906,18 +3005,18 @@
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="103"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="106"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="101" t="s">
+      <c r="H4" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="106"/>
     </row>
     <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="35" t="s">
@@ -4438,7 +4537,7 @@
     </row>
     <row r="112" spans="2:20" x14ac:dyDescent="0.35">
       <c r="H112" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I112" s="9">
         <f>14+2/3</f>
@@ -4450,15 +4549,27 @@
       <c r="P112" s="1"/>
     </row>
     <row r="113" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="H113" s="6"/>
-      <c r="I113" s="11"/>
-      <c r="J113" s="40"/>
+      <c r="H113" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I113" s="9">
+        <v>5</v>
+      </c>
+      <c r="J113" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="P113" s="1"/>
     </row>
     <row r="114" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="H114" s="6"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="40"/>
+      <c r="H114" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I114" s="9">
+        <v>5</v>
+      </c>
+      <c r="J114" s="4" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="115" spans="4:16" x14ac:dyDescent="0.35">
       <c r="H115" s="6"/>
@@ -4471,71 +4582,19 @@
       <c r="J116" s="42"/>
     </row>
     <row r="121" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="F121" s="132"/>
-      <c r="G121" s="133"/>
-      <c r="H121" s="132"/>
-      <c r="I121" s="133"/>
-      <c r="J121" s="132"/>
+      <c r="G121" s="1"/>
     </row>
     <row r="122" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="F122" s="132"/>
-      <c r="G122" s="133"/>
-      <c r="H122" s="132"/>
-      <c r="I122" s="133"/>
-      <c r="J122" s="132"/>
+      <c r="G122" s="1"/>
     </row>
     <row r="123" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D123"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="132"/>
-      <c r="G123" s="133"/>
-      <c r="H123" s="132"/>
-      <c r="I123" s="133"/>
-      <c r="J123" s="132"/>
+      <c r="G123" s="1"/>
     </row>
     <row r="124" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D124"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="132"/>
-      <c r="G124" s="132"/>
-      <c r="H124" s="132"/>
-      <c r="I124" s="133"/>
-      <c r="J124" s="132"/>
-    </row>
-    <row r="125" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="F125" s="132"/>
-      <c r="G125" s="132"/>
-      <c r="H125" s="132"/>
-      <c r="I125" s="133"/>
-      <c r="J125" s="132"/>
-    </row>
-    <row r="126" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="F126" s="132"/>
-      <c r="G126" s="132"/>
-      <c r="H126" s="132"/>
-      <c r="I126" s="133"/>
-      <c r="J126" s="132"/>
-    </row>
-    <row r="127" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="F127" s="132"/>
-      <c r="G127" s="132"/>
-      <c r="H127" s="132"/>
-      <c r="I127" s="133"/>
-      <c r="J127" s="132"/>
-    </row>
-    <row r="128" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="F128" s="132"/>
-      <c r="G128" s="132"/>
-      <c r="H128" s="132"/>
-      <c r="I128" s="133"/>
-      <c r="J128" s="132"/>
-    </row>
-    <row r="129" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F129" s="132"/>
-      <c r="G129" s="132"/>
-      <c r="H129" s="132"/>
-      <c r="I129" s="133"/>
-      <c r="J129" s="132"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:E18">
@@ -4636,16 +4695,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -5105,17 +5164,17 @@
     </row>
     <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="106"/>
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -5162,14 +5221,14 @@
         <v>8</v>
       </c>
       <c r="M12" s="19"/>
-      <c r="O12" s="104" t="s">
+      <c r="O12" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
+      <c r="S12" s="107"/>
+      <c r="T12" s="107"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -5193,12 +5252,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
+      <c r="S13" s="107"/>
+      <c r="T13" s="107"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -5216,12 +5275,12 @@
         <v>25</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -5238,12 +5297,12 @@
         <v>8</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -5260,14 +5319,14 @@
         <v>111</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="O16" s="104" t="s">
+      <c r="O16" s="107" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="107"/>
+      <c r="S16" s="107"/>
+      <c r="T16" s="107"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -5284,12 +5343,12 @@
         <v>111</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="O17" s="104"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
+      <c r="O17" s="107"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="107"/>
+      <c r="S17" s="107"/>
+      <c r="T17" s="107"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -5306,12 +5365,12 @@
         <v>147</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="104"/>
-      <c r="P18" s="104"/>
-      <c r="Q18" s="104"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
-      <c r="T18" s="104"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="107"/>
+      <c r="Q18" s="107"/>
+      <c r="R18" s="107"/>
+      <c r="S18" s="107"/>
+      <c r="T18" s="107"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -5328,12 +5387,12 @@
         <v>147</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="104"/>
-      <c r="P19" s="104"/>
-      <c r="Q19" s="104"/>
-      <c r="R19" s="104"/>
-      <c r="S19" s="104"/>
-      <c r="T19" s="104"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="107"/>
+      <c r="S19" s="107"/>
+      <c r="T19" s="107"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -5366,14 +5425,14 @@
         <v>200</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="O21" s="105" t="s">
+      <c r="O21" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="P21" s="105"/>
-      <c r="Q21" s="105"/>
-      <c r="R21" s="105"/>
-      <c r="S21" s="105"/>
-      <c r="T21" s="105"/>
+      <c r="P21" s="108"/>
+      <c r="Q21" s="108"/>
+      <c r="R21" s="108"/>
+      <c r="S21" s="108"/>
+      <c r="T21" s="108"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -5407,14 +5466,14 @@
         <v>399</v>
       </c>
       <c r="M23" s="2"/>
-      <c r="O23" s="104" t="s">
+      <c r="O23" s="107" t="s">
         <v>400</v>
       </c>
-      <c r="P23" s="104"/>
-      <c r="Q23" s="104"/>
-      <c r="R23" s="104"/>
-      <c r="S23" s="104"/>
-      <c r="T23" s="104"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
+      <c r="S23" s="107"/>
+      <c r="T23" s="107"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -5432,12 +5491,12 @@
         <v>450</v>
       </c>
       <c r="M24" s="2"/>
-      <c r="O24" s="104"/>
-      <c r="P24" s="104"/>
-      <c r="Q24" s="104"/>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
+      <c r="O24" s="107"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="107"/>
+      <c r="R24" s="107"/>
+      <c r="S24" s="107"/>
+      <c r="T24" s="107"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -5448,12 +5507,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104"/>
-      <c r="Q25" s="104"/>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="104"/>
+      <c r="O25" s="107"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="107"/>
+      <c r="T25" s="107"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -5464,12 +5523,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="104"/>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
-      <c r="S26" s="104"/>
-      <c r="T26" s="104"/>
+      <c r="O26" s="107"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="107"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -5480,14 +5539,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="104" t="s">
+      <c r="O27" s="107" t="s">
         <v>464</v>
       </c>
-      <c r="P27" s="104"/>
-      <c r="Q27" s="104"/>
-      <c r="R27" s="104"/>
-      <c r="S27" s="104"/>
-      <c r="T27" s="104"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="107"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -5498,12 +5557,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="104"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="104"/>
-      <c r="S28" s="104"/>
-      <c r="T28" s="104"/>
+      <c r="O28" s="107"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
+      <c r="T28" s="107"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -5514,12 +5573,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="104"/>
-      <c r="P29" s="104"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="104"/>
-      <c r="S29" s="104"/>
-      <c r="T29" s="104"/>
+      <c r="O29" s="107"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
+      <c r="T29" s="107"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -5530,12 +5589,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="104"/>
-      <c r="P30" s="104"/>
-      <c r="Q30" s="104"/>
-      <c r="R30" s="104"/>
-      <c r="S30" s="104"/>
-      <c r="T30" s="104"/>
+      <c r="O30" s="107"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
+      <c r="T30" s="107"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -5771,16 +5830,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6332,16 +6391,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6835,16 +6894,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -7356,16 +7415,16 @@
       </c>
     </row>
     <row r="12" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G12" s="118" t="s">
+      <c r="G12" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="119"/>
-      <c r="I12" s="120"/>
-      <c r="L12" s="118" t="s">
+      <c r="H12" s="122"/>
+      <c r="I12" s="123"/>
+      <c r="L12" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="119"/>
-      <c r="N12" s="120"/>
+      <c r="M12" s="122"/>
+      <c r="N12" s="123"/>
     </row>
     <row r="13" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G13" s="51" t="s">
@@ -7828,16 +7887,16 @@
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -8367,16 +8426,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -8882,16 +8941,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -9400,16 +9459,16 @@
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="23"/>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="102"/>
-      <c r="G13" s="103"/>
-      <c r="J13" s="101" t="s">
+      <c r="F13" s="105"/>
+      <c r="G13" s="106"/>
+      <c r="J13" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="102"/>
-      <c r="L13" s="103"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="106"/>
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
@@ -9821,16 +9880,16 @@
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="102"/>
-      <c r="H4" s="103"/>
-      <c r="K4" s="101" t="s">
+      <c r="G4" s="105"/>
+      <c r="H4" s="106"/>
+      <c r="K4" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="102"/>
-      <c r="M4" s="103"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="106"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="17" t="s">
@@ -10356,31 +10415,31 @@
     </row>
     <row r="18" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="23"/>
-      <c r="E18" s="101" t="s">
+      <c r="E18" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="103"/>
-      <c r="K18" s="101" t="s">
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="106"/>
+      <c r="K18" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="102"/>
-      <c r="M18" s="103"/>
-      <c r="O18" s="101" t="s">
+      <c r="L18" s="105"/>
+      <c r="M18" s="106"/>
+      <c r="O18" s="104" t="s">
         <v>264</v>
       </c>
-      <c r="P18" s="102"/>
-      <c r="Q18" s="102"/>
-      <c r="R18" s="102"/>
-      <c r="S18" s="102"/>
-      <c r="T18" s="103"/>
-      <c r="V18" s="101" t="s">
+      <c r="P18" s="105"/>
+      <c r="Q18" s="105"/>
+      <c r="R18" s="105"/>
+      <c r="S18" s="105"/>
+      <c r="T18" s="106"/>
+      <c r="V18" s="104" t="s">
         <v>275</v>
       </c>
-      <c r="W18" s="102"/>
-      <c r="X18" s="102"/>
-      <c r="Y18" s="103"/>
+      <c r="W18" s="105"/>
+      <c r="X18" s="105"/>
+      <c r="Y18" s="106"/>
       <c r="AA18" s="72" t="s">
         <v>285</v>
       </c>
@@ -10423,26 +10482,26 @@
       <c r="M19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="126" t="s">
+      <c r="O19" s="129" t="s">
         <v>265</v>
       </c>
-      <c r="P19" s="127"/>
-      <c r="Q19" s="124" t="s">
+      <c r="P19" s="130"/>
+      <c r="Q19" s="127" t="s">
         <v>266</v>
       </c>
-      <c r="R19" s="125"/>
-      <c r="S19" s="124" t="s">
+      <c r="R19" s="128"/>
+      <c r="S19" s="127" t="s">
         <v>272</v>
       </c>
-      <c r="T19" s="125"/>
-      <c r="V19" s="126" t="s">
+      <c r="T19" s="128"/>
+      <c r="V19" s="129" t="s">
         <v>256</v>
       </c>
-      <c r="W19" s="127"/>
-      <c r="X19" s="126" t="s">
+      <c r="W19" s="130"/>
+      <c r="X19" s="129" t="s">
         <v>274</v>
       </c>
-      <c r="Y19" s="128"/>
+      <c r="Y19" s="131"/>
       <c r="AA19" s="76" t="s">
         <v>304</v>
       </c>
@@ -11057,12 +11116,12 @@
       <c r="V29" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="W29" s="121">
+      <c r="W29" s="124">
         <f>W28+Y28</f>
         <v>372.36370370370366</v>
       </c>
-      <c r="X29" s="122"/>
-      <c r="Y29" s="123"/>
+      <c r="X29" s="125"/>
+      <c r="Y29" s="126"/>
       <c r="AA29" s="79" t="s">
         <v>291</v>
       </c>
@@ -12774,17 +12833,17 @@
     </row>
     <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="23"/>
-      <c r="E15" s="129" t="s">
+      <c r="E15" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="130"/>
-      <c r="G15" s="130"/>
-      <c r="H15" s="131"/>
-      <c r="J15" s="101" t="s">
+      <c r="F15" s="133"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="134"/>
+      <c r="J15" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="103"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="106"/>
     </row>
     <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="23"/>
@@ -13307,17 +13366,17 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="131"/>
-      <c r="J11" s="101" t="s">
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="134"/>
+      <c r="J11" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="106"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -13763,8 +13822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878EF637-2B1F-4BC8-A0FA-F77EC5044F15}">
   <dimension ref="B1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13781,7 +13840,7 @@
     <col min="14" max="14" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.6328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="40.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13858,24 +13917,24 @@
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="131"/>
-      <c r="J11" s="101" t="s">
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="134"/>
+      <c r="J11" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
-      <c r="N11" s="118" t="s">
+      <c r="K11" s="105"/>
+      <c r="L11" s="106"/>
+      <c r="N11" s="121" t="s">
         <v>426</v>
       </c>
-      <c r="O11" s="119"/>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="120"/>
+      <c r="O11" s="122"/>
+      <c r="P11" s="122"/>
+      <c r="Q11" s="122"/>
+      <c r="R11" s="123"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -14360,13 +14419,13 @@
       <c r="N27" s="93" t="s">
         <v>270</v>
       </c>
-      <c r="O27" s="122">
+      <c r="O27" s="125">
         <f>SUM(Q13:Q26)</f>
         <v>36259.599999999999</v>
       </c>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="123"/>
+      <c r="P27" s="125"/>
+      <c r="Q27" s="125"/>
+      <c r="R27" s="126"/>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -14553,16 +14612,16 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC07E90-6101-47F8-9701-BB9D283EFF37}">
-  <dimension ref="B1:L72"/>
+  <dimension ref="B1:S75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
@@ -14570,10 +14629,16 @@
     <col min="10" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
@@ -14581,91 +14646,115 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:19" ht="116" x14ac:dyDescent="0.35">
       <c r="B3" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="25"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C5" s="25" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="25"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C6" s="25" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="C7" s="25"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C7" s="25" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
         <v>451</v>
       </c>
-      <c r="C8" s="25"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C8" s="25" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="C9" s="25"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C9" s="25" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="99"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C10" s="99" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B11" s="100" t="s">
         <v>358</v>
       </c>
-      <c r="C11" s="99"/>
-    </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="99" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="C12" s="26"/>
-    </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="26" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="23"/>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="131"/>
-      <c r="J13" s="101" t="s">
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="134"/>
+      <c r="J13" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="102"/>
-      <c r="L13" s="103"/>
-    </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K13" s="105"/>
+      <c r="L13" s="106"/>
+      <c r="N13" s="127" t="s">
+        <v>492</v>
+      </c>
+      <c r="O13" s="138"/>
+      <c r="P13" s="138"/>
+      <c r="Q13" s="138"/>
+      <c r="R13" s="138"/>
+      <c r="S13" s="141"/>
+    </row>
+    <row r="14" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
-      <c r="E14" s="134" t="s">
+      <c r="E14" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="135" t="s">
+      <c r="F14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="136" t="s">
+      <c r="G14" s="102" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="55" t="s">
@@ -14680,8 +14769,26 @@
       <c r="L14" s="14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N14" s="143" t="s">
+        <v>285</v>
+      </c>
+      <c r="O14" s="143" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="143" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q14" s="143" t="s">
+        <v>491</v>
+      </c>
+      <c r="R14" s="143" t="s">
+        <v>286</v>
+      </c>
+      <c r="S14" s="143" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
       <c r="E15" s="46" t="s">
         <v>361</v>
@@ -14690,7 +14797,7 @@
         <f>4+64/75</f>
         <v>4.8533333333333335</v>
       </c>
-      <c r="G15" s="137" t="s">
+      <c r="G15" s="103" t="s">
         <v>252</v>
       </c>
       <c r="H15" s="19"/>
@@ -14704,8 +14811,28 @@
       <c r="L15" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N15" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="O15" s="4">
+        <v>5</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="R15" s="4">
+        <f>(384.6+96.1)/2</f>
+        <v>240.35000000000002</v>
+      </c>
+      <c r="S15" s="4">
+        <f>R15*O15</f>
+        <v>1201.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
       <c r="E16" s="6" t="s">
         <v>386</v>
@@ -14730,8 +14857,28 @@
       <c r="L16" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N16" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="O16" s="2">
+        <v>10</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="R16" s="2">
+        <f>1922.8/2</f>
+        <v>961.4</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" ref="S16:S31" si="0">R16*O16</f>
+        <v>9614</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
       <c r="E17" s="6" t="s">
         <v>19</v>
@@ -14755,8 +14902,28 @@
       <c r="L17" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N17" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="O17" s="2">
+        <v>5</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="R17" s="2">
+        <f>(1442.1+480.7)/2</f>
+        <v>961.4</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="0"/>
+        <v>4807</v>
+      </c>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
       <c r="E18" s="6" t="s">
         <v>19</v>
@@ -14780,8 +14947,28 @@
       <c r="L18" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N18" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="O18" s="2">
+        <v>10</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="R18" s="2">
+        <f>(61.5+15.4)/2</f>
+        <v>38.450000000000003</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="0"/>
+        <v>384.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
       <c r="E19" s="6" t="s">
         <v>458</v>
@@ -14805,8 +14992,28 @@
       <c r="L19" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N19" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="O19" s="2">
+        <v>3</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="R19" s="2">
+        <f>(288.1+72)/2</f>
+        <v>180.05</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="0"/>
+        <v>540.15000000000009</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
       <c r="E20" s="6" t="s">
         <v>137</v>
@@ -14830,8 +15037,28 @@
       <c r="L20" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N20" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="O20" s="2">
+        <v>14</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="R20" s="2">
+        <f>(1319.6+439.9)/2</f>
+        <v>879.75</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="0"/>
+        <v>12316.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
       <c r="E21" s="6" t="s">
         <v>386</v>
@@ -14855,8 +15082,28 @@
       <c r="L21" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N21" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="O21" s="2">
+        <v>2</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="R21" s="2">
+        <f>(479.9+160)/2</f>
+        <v>319.95</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="0"/>
+        <v>639.9</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
       <c r="E22" s="6" t="s">
         <v>52</v>
@@ -14880,8 +15127,28 @@
       <c r="L22" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N22" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="O22" s="2">
+        <v>5</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="R22" s="2">
+        <f>(374.4+93.6)/2</f>
+        <v>234</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="0"/>
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
       <c r="E23" s="6" t="s">
         <v>5</v>
@@ -14905,8 +15172,28 @@
       <c r="L23" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N23" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="O23" s="2">
+        <v>2</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R23" s="2">
+        <f>(255.9+64)/2</f>
+        <v>159.94999999999999</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="0"/>
+        <v>319.89999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="23"/>
       <c r="E24" s="6" t="s">
         <v>19</v>
@@ -14931,8 +15218,28 @@
       <c r="L24" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N24" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="O24" s="3">
+        <v>1</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="R24" s="3">
+        <f>(1403.8+467.9)/2</f>
+        <v>935.84999999999991</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="0"/>
+        <v>935.84999999999991</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="23"/>
       <c r="E25" s="6" t="s">
         <v>34</v>
@@ -14956,8 +15263,19 @@
       <c r="L25" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="N25" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="O25" s="139">
+        <f>SUM(S15:S24)</f>
+        <v>31929.550000000003</v>
+      </c>
+      <c r="P25" s="140"/>
+      <c r="Q25" s="140"/>
+      <c r="R25" s="140"/>
+      <c r="S25" s="142"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
       <c r="E26" s="6" t="s">
         <v>19</v>
@@ -14982,7 +15300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
       <c r="E27" s="6" t="s">
         <v>88</v>
@@ -15006,7 +15324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
       <c r="E28" s="6" t="s">
         <v>61</v>
@@ -15030,7 +15348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
       <c r="E29" s="6" t="s">
         <v>34</v>
@@ -15055,7 +15373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
       <c r="E30" s="6" t="s">
         <v>19</v>
@@ -15080,7 +15398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
       <c r="E31" s="6" t="s">
         <v>17</v>
@@ -15105,7 +15423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
       <c r="E32" s="6" t="s">
         <v>17</v>
@@ -15168,7 +15486,7 @@
         <v>466</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K34" s="9">
         <f>14+2/3</f>
@@ -15192,9 +15510,15 @@
       <c r="H35" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="9">
+        <v>5</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
@@ -15211,9 +15535,15 @@
       <c r="H36" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="J36" s="2"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="2"/>
+      <c r="J36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" s="9">
+        <v>5</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C37" s="23"/>
@@ -15356,7 +15686,7 @@
         <v>60</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="9"/>
@@ -15373,7 +15703,7 @@
         <v>60</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="9"/>
@@ -15391,7 +15721,7 @@
         <v>60</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="9"/>
@@ -15409,7 +15739,7 @@
         <v>62</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="9"/>
@@ -15426,13 +15756,13 @@
         <v>481</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="9"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E49" s="6" t="s">
         <v>20</v>
       </c>
@@ -15443,13 +15773,13 @@
         <v>23</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="10"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E50" s="6" t="s">
         <v>386</v>
       </c>
@@ -15461,24 +15791,30 @@
         <v>481</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="51" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="51" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E51" s="94"/>
       <c r="F51" s="67"/>
       <c r="G51" s="97"/>
       <c r="H51" s="67"/>
     </row>
-    <row r="52" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E52" s="118" t="s">
-        <v>484</v>
-      </c>
-      <c r="F52" s="119"/>
-      <c r="G52" s="119"/>
-      <c r="H52" s="120"/>
-    </row>
-    <row r="53" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E52" s="121" t="s">
+        <v>483</v>
+      </c>
+      <c r="F52" s="122"/>
+      <c r="G52" s="122"/>
+      <c r="H52" s="123"/>
+      <c r="J52" s="121" t="s">
+        <v>483</v>
+      </c>
+      <c r="K52" s="122"/>
+      <c r="L52" s="123"/>
+      <c r="M52" s="135"/>
+    </row>
+    <row r="53" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E53" s="14" t="s">
         <v>0</v>
       </c>
@@ -15491,8 +15827,18 @@
       <c r="H53" s="52" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="J53" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L53" s="53" t="s">
+        <v>406</v>
+      </c>
+      <c r="M53" s="136"/>
+    </row>
+    <row r="54" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E54" s="4" t="s">
         <v>361</v>
       </c>
@@ -15504,236 +15850,420 @@
         <v>252</v>
       </c>
       <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="J54" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="K54" s="38">
+        <f>364/1215</f>
+        <v>0.29958847736625516</v>
+      </c>
+      <c r="L54" s="41"/>
+      <c r="M54" s="136"/>
+    </row>
+    <row r="55" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E55" s="2" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="F55" s="2">
-        <f>F18+F19+F25+F27+F31+F39+F42+F48</f>
-        <v>9350.5138765432093</v>
+        <v>7</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
       <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="J55" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="K55" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="L55" s="40"/>
+      <c r="M55" s="136"/>
+    </row>
+    <row r="56" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E56" s="2" t="s">
-        <v>458</v>
+        <v>5</v>
       </c>
       <c r="F56" s="2">
-        <v>760</v>
+        <f>$F$35+$F$23</f>
+        <v>37.166666666666664</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>377</v>
+        <v>106</v>
       </c>
       <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="J56" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K56" s="11">
+        <v>5</v>
+      </c>
+      <c r="L56" s="40"/>
+      <c r="M56" s="136"/>
+    </row>
+    <row r="57" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E57" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="F57" s="2">
+        <v>70</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="H57" s="2"/>
+      <c r="J57" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="K57" s="11">
+        <v>5</v>
+      </c>
+      <c r="L57" s="40"/>
+      <c r="M57" s="136"/>
+    </row>
+    <row r="58" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E58" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="F58" s="11">
+        <f>114+2/15</f>
+        <v>114.13333333333334</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H58" s="2"/>
+      <c r="J58" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K58" s="11">
+        <v>5</v>
+      </c>
+      <c r="L58" s="40"/>
+      <c r="M58" s="136"/>
+    </row>
+    <row r="59" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E59" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F57" s="11">
+      <c r="F59" s="11">
         <f>280 + 8/9</f>
         <v>280.88888888888891</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E58" s="2" t="s">
+      <c r="H59" s="2"/>
+      <c r="J59" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K59" s="11">
+        <v>5</v>
+      </c>
+      <c r="L59" s="40"/>
+      <c r="M59" s="136"/>
+    </row>
+    <row r="60" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="2">
+        <v>300</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60" s="2"/>
+      <c r="J60" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K60" s="11">
+        <v>5</v>
+      </c>
+      <c r="L60" s="40"/>
+      <c r="M60" s="136"/>
+    </row>
+    <row r="61" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E61" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="F58" s="2">
-        <f>F51+F22+F17</f>
-        <v>12248</v>
-      </c>
-      <c r="G58" s="2" t="s">
+      <c r="F61" s="2">
+        <f>$F$50+$F$21+$F$16</f>
+        <v>454.44444444444446</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E59" s="2" t="s">
+      <c r="H61" s="2"/>
+      <c r="J61" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="K61" s="11">
+        <f>14+2/3</f>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="L61" s="40"/>
+      <c r="M61" s="136"/>
+    </row>
+    <row r="62" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E62" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F62" s="2">
         <v>600</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E60" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="2">
-        <f>F24+F36</f>
-        <v>824.13993086419759</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E61" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F61" s="2">
-        <f>F26+F30+F38+F47</f>
-        <v>3379.8731414380554</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E62" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="F62" s="2">
-        <v>1800</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="J62" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="K62" s="11">
+        <v>15</v>
+      </c>
+      <c r="L62" s="40"/>
+      <c r="M62" s="136"/>
+    </row>
+    <row r="63" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E63" s="2" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F63" s="2">
-        <f>F29+F45+F40</f>
-        <v>5829.7692307692305</v>
+        <v>600</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="J63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K63" s="11">
+        <v>30</v>
+      </c>
+      <c r="L63" s="40"/>
+      <c r="M63" s="136"/>
+    </row>
+    <row r="64" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E64" s="2" t="s">
-        <v>17</v>
+        <v>458</v>
       </c>
       <c r="F64" s="2">
-        <v>1400</v>
+        <v>760</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>60</v>
+        <v>377</v>
       </c>
       <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="J64" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K64" s="11">
+        <v>45</v>
+      </c>
+      <c r="L64" s="40"/>
+      <c r="M64" s="136"/>
+    </row>
+    <row r="65" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E65" s="2" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="F65" s="2">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="J65" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K65" s="11">
+        <v>45</v>
+      </c>
+      <c r="L65" s="40"/>
+      <c r="M65" s="136"/>
+    </row>
+    <row r="66" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E66" s="2" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="F66" s="2">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="J66" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K66" s="11">
+        <f>$K$32+$K$19</f>
+        <v>202.33333333333334</v>
+      </c>
+      <c r="L66" s="40"/>
+      <c r="M66" s="136"/>
+    </row>
+    <row r="67" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E67" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1650</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H67" s="2"/>
+      <c r="J67" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K67" s="11">
+        <f>398+14/75</f>
+        <v>398.18666666666667</v>
+      </c>
+      <c r="L67" s="40"/>
+      <c r="M67" s="136"/>
+    </row>
+    <row r="68" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E68" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1800</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H68" s="2"/>
+      <c r="J68" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K68" s="11">
+        <f>537+28/125</f>
+        <v>537.22400000000005</v>
+      </c>
+      <c r="L68" s="40"/>
+      <c r="M68" s="136"/>
+    </row>
+    <row r="69" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E69" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F67" s="2">
-        <f>F46+F37</f>
-        <v>4355.562962962963</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E68" s="2" t="s">
+      <c r="F69" s="2">
+        <f>$F$45+$F$36</f>
+        <v>4038.2732641975308</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="H69" s="2"/>
+      <c r="J69" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" s="11">
+        <v>593.75</v>
+      </c>
+      <c r="L69" s="40"/>
+      <c r="M69" s="136"/>
+    </row>
+    <row r="70" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E70" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" s="2">
+        <f>$F$39+$F$28+$F$44</f>
+        <v>4562.3484444444439</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="J70" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K70" s="11">
+        <f>$K$22+$K$23</f>
+        <v>750.05259259259265</v>
+      </c>
+      <c r="L70" s="40"/>
+      <c r="M70" s="136"/>
+    </row>
+    <row r="71" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E71" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" s="2">
+        <f>$F$46+$F$37+$F$29+$F$25</f>
+        <v>5022.3988603988601</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H71" s="2"/>
+      <c r="J71" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K71" s="9">
+        <f>996+25/36</f>
+        <v>996.69444444444446</v>
+      </c>
+      <c r="L71" s="2"/>
+      <c r="M71" s="136"/>
+    </row>
+    <row r="72" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="3">
+        <f>$F$17+$F$18+$F$24+$F$26+$F$30+$F$38+$F$41+$F$47</f>
+        <v>21592.829506870155</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H72" s="3"/>
+      <c r="J72" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F68" s="2">
-        <v>1650</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E69" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F69" s="2">
-        <v>7</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E70" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="F70" s="11">
-        <f>114+2/15</f>
-        <v>114.13333333333334</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E71" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="F71" s="2">
-        <v>70</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E72" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" s="3">
-        <v>300</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H72" s="3"/>
+      <c r="K72" s="9">
+        <f>1650-158-5/6</f>
+        <v>1491.1666666666667</v>
+      </c>
+      <c r="L72" s="2"/>
+      <c r="M72" s="136"/>
+    </row>
+    <row r="73" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="J73" s="136"/>
+      <c r="K73" s="137"/>
+      <c r="L73" s="136"/>
+      <c r="M73" s="136"/>
+    </row>
+    <row r="74" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="J74" s="136"/>
+      <c r="K74" s="136"/>
+      <c r="L74" s="136"/>
+      <c r="M74" s="136"/>
+    </row>
+    <row r="75" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="J75" s="136"/>
+      <c r="K75" s="136"/>
+      <c r="L75" s="136"/>
+      <c r="M75" s="136"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J54:L72">
+    <sortCondition ref="K54:K72"/>
+  </sortState>
+  <mergeCells count="6">
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="O25:S25"/>
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="E52:H52"/>
+    <mergeCell ref="J52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15830,17 +16360,17 @@
     </row>
     <row r="12" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="102"/>
-      <c r="H13" s="103"/>
-      <c r="K13" s="101" t="s">
+      <c r="G13" s="105"/>
+      <c r="H13" s="106"/>
+      <c r="K13" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="103"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="106"/>
     </row>
     <row r="14" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="14" t="s">
@@ -15864,14 +16394,14 @@
       <c r="N14" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="P14" s="104" t="s">
+      <c r="P14" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
-      <c r="U14" s="104"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
+      <c r="U14" s="107"/>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
@@ -15894,12 +16424,12 @@
         <v>25</v>
       </c>
       <c r="N15" s="19"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="104"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
+      <c r="U15" s="107"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
@@ -15923,12 +16453,12 @@
       <c r="N16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
-      <c r="U16" s="104"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="107"/>
+      <c r="S16" s="107"/>
+      <c r="T16" s="107"/>
+      <c r="U16" s="107"/>
     </row>
     <row r="17" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
@@ -15946,12 +16476,12 @@
       <c r="N17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
-      <c r="U17" s="104"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="107"/>
+      <c r="S17" s="107"/>
+      <c r="T17" s="107"/>
+      <c r="U17" s="107"/>
     </row>
     <row r="18" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
@@ -16001,14 +16531,14 @@
         <v>170</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="P20" s="105" t="s">
+      <c r="P20" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="Q20" s="105"/>
-      <c r="R20" s="105"/>
-      <c r="S20" s="105"/>
-      <c r="T20" s="105"/>
-      <c r="U20" s="105"/>
+      <c r="Q20" s="108"/>
+      <c r="R20" s="108"/>
+      <c r="S20" s="108"/>
+      <c r="T20" s="108"/>
+      <c r="U20" s="108"/>
     </row>
     <row r="21" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
@@ -16040,14 +16570,14 @@
         <v>159</v>
       </c>
       <c r="N22" s="2"/>
-      <c r="P22" s="104" t="s">
+      <c r="P22" s="107" t="s">
         <v>172</v>
       </c>
-      <c r="Q22" s="104"/>
-      <c r="R22" s="104"/>
-      <c r="S22" s="104"/>
-      <c r="T22" s="104"/>
-      <c r="U22" s="104"/>
+      <c r="Q22" s="107"/>
+      <c r="R22" s="107"/>
+      <c r="S22" s="107"/>
+      <c r="T22" s="107"/>
+      <c r="U22" s="107"/>
     </row>
     <row r="23" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
@@ -16064,12 +16594,12 @@
         <v>252</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="P23" s="104"/>
-      <c r="Q23" s="104"/>
-      <c r="R23" s="104"/>
-      <c r="S23" s="104"/>
-      <c r="T23" s="104"/>
-      <c r="U23" s="104"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
+      <c r="S23" s="107"/>
+      <c r="T23" s="107"/>
+      <c r="U23" s="107"/>
     </row>
     <row r="24" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
@@ -16086,12 +16616,12 @@
         <v>377</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="P24" s="104"/>
-      <c r="Q24" s="104"/>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
-      <c r="U24" s="104"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="107"/>
+      <c r="R24" s="107"/>
+      <c r="S24" s="107"/>
+      <c r="T24" s="107"/>
+      <c r="U24" s="107"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
@@ -16110,12 +16640,12 @@
       <c r="N25" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="P25" s="104"/>
-      <c r="Q25" s="104"/>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="104"/>
-      <c r="U25" s="104"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="107"/>
+      <c r="T25" s="107"/>
+      <c r="U25" s="107"/>
     </row>
     <row r="26" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
@@ -16131,14 +16661,14 @@
         <v>418</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="P26" s="104" t="s">
+      <c r="P26" s="107" t="s">
         <v>263</v>
       </c>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
-      <c r="S26" s="104"/>
-      <c r="T26" s="104"/>
-      <c r="U26" s="104"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="107"/>
+      <c r="U26" s="107"/>
     </row>
     <row r="27" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
@@ -16148,12 +16678,12 @@
       <c r="L27" s="9"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="P27" s="104"/>
-      <c r="Q27" s="104"/>
-      <c r="R27" s="104"/>
-      <c r="S27" s="104"/>
-      <c r="T27" s="104"/>
-      <c r="U27" s="104"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="107"/>
+      <c r="U27" s="107"/>
     </row>
     <row r="28" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
@@ -16163,12 +16693,12 @@
       <c r="L28" s="9"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="104"/>
-      <c r="S28" s="104"/>
-      <c r="T28" s="104"/>
-      <c r="U28" s="104"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
+      <c r="T28" s="107"/>
+      <c r="U28" s="107"/>
     </row>
     <row r="29" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
@@ -16178,12 +16708,12 @@
       <c r="L29" s="9"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="P29" s="104"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="104"/>
-      <c r="S29" s="104"/>
-      <c r="T29" s="104"/>
-      <c r="U29" s="104"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
+      <c r="T29" s="107"/>
+      <c r="U29" s="107"/>
     </row>
     <row r="30" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
@@ -16193,14 +16723,14 @@
       <c r="L30" s="9"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="P30" s="104" t="s">
+      <c r="P30" s="107" t="s">
         <v>409</v>
       </c>
-      <c r="Q30" s="104"/>
-      <c r="R30" s="104"/>
-      <c r="S30" s="104"/>
-      <c r="T30" s="104"/>
-      <c r="U30" s="104"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
+      <c r="T30" s="107"/>
+      <c r="U30" s="107"/>
     </row>
     <row r="31" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
@@ -16210,12 +16740,12 @@
       <c r="L31" s="9"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="P31" s="104"/>
-      <c r="Q31" s="104"/>
-      <c r="R31" s="104"/>
-      <c r="S31" s="104"/>
-      <c r="T31" s="104"/>
-      <c r="U31" s="104"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
+      <c r="T31" s="107"/>
+      <c r="U31" s="107"/>
     </row>
     <row r="32" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
@@ -16225,12 +16755,12 @@
       <c r="L32" s="9"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="P32" s="104"/>
-      <c r="Q32" s="104"/>
-      <c r="R32" s="104"/>
-      <c r="S32" s="104"/>
-      <c r="T32" s="104"/>
-      <c r="U32" s="104"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="107"/>
+      <c r="S32" s="107"/>
+      <c r="T32" s="107"/>
+      <c r="U32" s="107"/>
     </row>
     <row r="33" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
@@ -16240,12 +16770,12 @@
       <c r="L33" s="9"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="P33" s="104"/>
-      <c r="Q33" s="104"/>
-      <c r="R33" s="104"/>
-      <c r="S33" s="104"/>
-      <c r="T33" s="104"/>
-      <c r="U33" s="104"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="107"/>
+      <c r="U33" s="107"/>
     </row>
     <row r="34" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
@@ -16255,14 +16785,14 @@
       <c r="L34" s="9"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="P34" s="104" t="s">
+      <c r="P34" s="107" t="s">
         <v>419</v>
       </c>
-      <c r="Q34" s="104"/>
-      <c r="R34" s="104"/>
-      <c r="S34" s="104"/>
-      <c r="T34" s="104"/>
-      <c r="U34" s="104"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="107"/>
+      <c r="T34" s="107"/>
+      <c r="U34" s="107"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
@@ -16272,12 +16802,12 @@
       <c r="L35" s="9"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="P35" s="104"/>
-      <c r="Q35" s="104"/>
-      <c r="R35" s="104"/>
-      <c r="S35" s="104"/>
-      <c r="T35" s="104"/>
-      <c r="U35" s="104"/>
+      <c r="P35" s="107"/>
+      <c r="Q35" s="107"/>
+      <c r="R35" s="107"/>
+      <c r="S35" s="107"/>
+      <c r="T35" s="107"/>
+      <c r="U35" s="107"/>
     </row>
     <row r="36" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
@@ -16287,12 +16817,12 @@
       <c r="L36" s="9"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="P36" s="104"/>
-      <c r="Q36" s="104"/>
-      <c r="R36" s="104"/>
-      <c r="S36" s="104"/>
-      <c r="T36" s="104"/>
-      <c r="U36" s="104"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="107"/>
+      <c r="R36" s="107"/>
+      <c r="S36" s="107"/>
+      <c r="T36" s="107"/>
+      <c r="U36" s="107"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
@@ -16302,12 +16832,12 @@
       <c r="L37" s="9"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="P37" s="104"/>
-      <c r="Q37" s="104"/>
-      <c r="R37" s="104"/>
-      <c r="S37" s="104"/>
-      <c r="T37" s="104"/>
-      <c r="U37" s="104"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="107"/>
+      <c r="R37" s="107"/>
+      <c r="S37" s="107"/>
+      <c r="T37" s="107"/>
+      <c r="U37" s="107"/>
     </row>
     <row r="38" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
@@ -16508,16 +17038,16 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
-      <c r="J11" s="101" t="s">
+      <c r="F11" s="105"/>
+      <c r="G11" s="106"/>
+      <c r="J11" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="106"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -16999,17 +17529,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
-      <c r="J11" s="101" t="s">
+      <c r="F11" s="105"/>
+      <c r="G11" s="106"/>
+      <c r="J11" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="103"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="106"/>
     </row>
     <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -17034,14 +17564,14 @@
       <c r="M12" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O12" s="104" t="s">
+      <c r="O12" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
+      <c r="S12" s="107"/>
+      <c r="T12" s="107"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -17065,12 +17595,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
+      <c r="S13" s="107"/>
+      <c r="T13" s="107"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -17095,12 +17625,12 @@
       <c r="M14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -17119,12 +17649,12 @@
       <c r="M15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -17143,14 +17673,14 @@
       <c r="M16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O16" s="104" t="s">
+      <c r="O16" s="107" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="107"/>
+      <c r="S16" s="107"/>
+      <c r="T16" s="107"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -17169,12 +17699,12 @@
       <c r="M17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="O17" s="104"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
+      <c r="O17" s="107"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="107"/>
+      <c r="S17" s="107"/>
+      <c r="T17" s="107"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -17191,12 +17721,12 @@
         <v>147</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="104"/>
-      <c r="P18" s="104"/>
-      <c r="Q18" s="104"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
-      <c r="T18" s="104"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="107"/>
+      <c r="Q18" s="107"/>
+      <c r="R18" s="107"/>
+      <c r="S18" s="107"/>
+      <c r="T18" s="107"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -17213,12 +17743,12 @@
         <v>170</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="104"/>
-      <c r="P19" s="104"/>
-      <c r="Q19" s="104"/>
-      <c r="R19" s="104"/>
-      <c r="S19" s="104"/>
-      <c r="T19" s="104"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="107"/>
+      <c r="S19" s="107"/>
+      <c r="T19" s="107"/>
     </row>
     <row r="20" spans="3:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -17246,14 +17776,14 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="105" t="s">
+      <c r="O21" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="P21" s="105"/>
-      <c r="Q21" s="105"/>
-      <c r="R21" s="105"/>
-      <c r="S21" s="105"/>
-      <c r="T21" s="105"/>
+      <c r="P21" s="108"/>
+      <c r="Q21" s="108"/>
+      <c r="R21" s="108"/>
+      <c r="S21" s="108"/>
+      <c r="T21" s="108"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -17274,14 +17804,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="104" t="s">
+      <c r="O23" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="P23" s="104"/>
-      <c r="Q23" s="104"/>
-      <c r="R23" s="104"/>
-      <c r="S23" s="104"/>
-      <c r="T23" s="104"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
+      <c r="S23" s="107"/>
+      <c r="T23" s="107"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -17292,12 +17822,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="104"/>
-      <c r="P24" s="104"/>
-      <c r="Q24" s="104"/>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
+      <c r="O24" s="107"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="107"/>
+      <c r="R24" s="107"/>
+      <c r="S24" s="107"/>
+      <c r="T24" s="107"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -17308,12 +17838,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104"/>
-      <c r="Q25" s="104"/>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="104"/>
+      <c r="O25" s="107"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="107"/>
+      <c r="T25" s="107"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -17324,12 +17854,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="6"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="104"/>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
-      <c r="S26" s="104"/>
-      <c r="T26" s="104"/>
+      <c r="O26" s="107"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="107"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -17340,14 +17870,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="6"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="104" t="s">
+      <c r="O27" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="P27" s="104"/>
-      <c r="Q27" s="104"/>
-      <c r="R27" s="104"/>
-      <c r="S27" s="104"/>
-      <c r="T27" s="104"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="107"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -17358,12 +17888,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="6"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="104"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="104"/>
-      <c r="S28" s="104"/>
-      <c r="T28" s="104"/>
+      <c r="O28" s="107"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
+      <c r="T28" s="107"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -17374,12 +17904,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="6"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="104"/>
-      <c r="P29" s="104"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="104"/>
-      <c r="S29" s="104"/>
-      <c r="T29" s="104"/>
+      <c r="O29" s="107"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
+      <c r="T29" s="107"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -17390,12 +17920,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="6"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="104"/>
-      <c r="P30" s="104"/>
-      <c r="Q30" s="104"/>
-      <c r="R30" s="104"/>
-      <c r="S30" s="104"/>
-      <c r="T30" s="104"/>
+      <c r="O30" s="107"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
+      <c r="T30" s="107"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -17406,14 +17936,14 @@
       <c r="K31" s="9"/>
       <c r="L31" s="6"/>
       <c r="M31" s="2"/>
-      <c r="O31" s="104" t="s">
+      <c r="O31" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="P31" s="104"/>
-      <c r="Q31" s="104"/>
-      <c r="R31" s="104"/>
-      <c r="S31" s="104"/>
-      <c r="T31" s="104"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
+      <c r="T31" s="107"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -17424,12 +17954,12 @@
       <c r="K32" s="9"/>
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
-      <c r="O32" s="104"/>
-      <c r="P32" s="104"/>
-      <c r="Q32" s="104"/>
-      <c r="R32" s="104"/>
-      <c r="S32" s="104"/>
-      <c r="T32" s="104"/>
+      <c r="O32" s="107"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="107"/>
+      <c r="S32" s="107"/>
+      <c r="T32" s="107"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C33" s="23"/>
@@ -17440,12 +17970,12 @@
       <c r="K33" s="9"/>
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
-      <c r="O33" s="104"/>
-      <c r="P33" s="104"/>
-      <c r="Q33" s="104"/>
-      <c r="R33" s="104"/>
-      <c r="S33" s="104"/>
-      <c r="T33" s="104"/>
+      <c r="O33" s="107"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="107"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C34" s="23"/>
@@ -17456,12 +17986,12 @@
       <c r="K34" s="9"/>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
-      <c r="O34" s="104"/>
-      <c r="P34" s="104"/>
-      <c r="Q34" s="104"/>
-      <c r="R34" s="104"/>
-      <c r="S34" s="104"/>
-      <c r="T34" s="104"/>
+      <c r="O34" s="107"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="107"/>
+      <c r="T34" s="107"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C35" s="23"/>
@@ -17472,14 +18002,14 @@
       <c r="K35" s="9"/>
       <c r="L35" s="6"/>
       <c r="M35" s="2"/>
-      <c r="O35" s="104" t="s">
+      <c r="O35" s="107" t="s">
         <v>261</v>
       </c>
-      <c r="P35" s="104"/>
-      <c r="Q35" s="104"/>
-      <c r="R35" s="104"/>
-      <c r="S35" s="104"/>
-      <c r="T35" s="104"/>
+      <c r="P35" s="107"/>
+      <c r="Q35" s="107"/>
+      <c r="R35" s="107"/>
+      <c r="S35" s="107"/>
+      <c r="T35" s="107"/>
     </row>
     <row r="36" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
@@ -17490,12 +18020,12 @@
       <c r="K36" s="9"/>
       <c r="L36" s="6"/>
       <c r="M36" s="2"/>
-      <c r="O36" s="104"/>
-      <c r="P36" s="104"/>
-      <c r="Q36" s="104"/>
-      <c r="R36" s="104"/>
-      <c r="S36" s="104"/>
-      <c r="T36" s="104"/>
+      <c r="O36" s="107"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="107"/>
+      <c r="R36" s="107"/>
+      <c r="S36" s="107"/>
+      <c r="T36" s="107"/>
     </row>
     <row r="37" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E37" s="2"/>
@@ -17505,12 +18035,12 @@
       <c r="K37" s="9"/>
       <c r="L37" s="6"/>
       <c r="M37" s="2"/>
-      <c r="O37" s="104"/>
-      <c r="P37" s="104"/>
-      <c r="Q37" s="104"/>
-      <c r="R37" s="104"/>
-      <c r="S37" s="104"/>
-      <c r="T37" s="104"/>
+      <c r="O37" s="107"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="107"/>
+      <c r="R37" s="107"/>
+      <c r="S37" s="107"/>
+      <c r="T37" s="107"/>
     </row>
     <row r="38" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E38" s="2"/>
@@ -17520,12 +18050,12 @@
       <c r="K38" s="9"/>
       <c r="L38" s="6"/>
       <c r="M38" s="2"/>
-      <c r="O38" s="104"/>
-      <c r="P38" s="104"/>
-      <c r="Q38" s="104"/>
-      <c r="R38" s="104"/>
-      <c r="S38" s="104"/>
-      <c r="T38" s="104"/>
+      <c r="O38" s="107"/>
+      <c r="P38" s="107"/>
+      <c r="Q38" s="107"/>
+      <c r="R38" s="107"/>
+      <c r="S38" s="107"/>
+      <c r="T38" s="107"/>
     </row>
     <row r="39" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E39" s="2"/>
@@ -17698,17 +18228,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
-      <c r="J11" s="101" t="s">
+      <c r="F11" s="105"/>
+      <c r="G11" s="106"/>
+      <c r="J11" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="103"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="106"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -17733,14 +18263,14 @@
       <c r="M12" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="O12" s="104" t="s">
+      <c r="O12" s="107" t="s">
         <v>84</v>
       </c>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
+      <c r="S12" s="107"/>
+      <c r="T12" s="107"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -17764,12 +18294,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
+      <c r="S13" s="107"/>
+      <c r="T13" s="107"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -17792,12 +18322,12 @@
         <v>81</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -17816,12 +18346,12 @@
       <c r="M15" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -17896,14 +18426,14 @@
       <c r="M19" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="O19" s="115" t="s">
+      <c r="O19" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="P19" s="116"/>
-      <c r="Q19" s="116"/>
-      <c r="R19" s="116"/>
-      <c r="S19" s="116"/>
-      <c r="T19" s="117"/>
+      <c r="P19" s="119"/>
+      <c r="Q19" s="119"/>
+      <c r="R19" s="119"/>
+      <c r="S19" s="119"/>
+      <c r="T19" s="120"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -17923,14 +18453,14 @@
       <c r="M20" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="O20" s="106" t="s">
+      <c r="O20" s="109" t="s">
         <v>405</v>
       </c>
-      <c r="P20" s="107"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="107"/>
-      <c r="S20" s="107"/>
-      <c r="T20" s="108"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="110"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="111"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -17941,12 +18471,12 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="109"/>
-      <c r="P21" s="110"/>
-      <c r="Q21" s="110"/>
-      <c r="R21" s="110"/>
-      <c r="S21" s="110"/>
-      <c r="T21" s="111"/>
+      <c r="O21" s="112"/>
+      <c r="P21" s="113"/>
+      <c r="Q21" s="113"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="113"/>
+      <c r="T21" s="114"/>
     </row>
     <row r="22" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="23"/>
@@ -17957,12 +18487,12 @@
       <c r="K22" s="9"/>
       <c r="L22" s="6"/>
       <c r="M22" s="2"/>
-      <c r="O22" s="112"/>
-      <c r="P22" s="113"/>
-      <c r="Q22" s="113"/>
-      <c r="R22" s="113"/>
-      <c r="S22" s="113"/>
-      <c r="T22" s="114"/>
+      <c r="O22" s="115"/>
+      <c r="P22" s="116"/>
+      <c r="Q22" s="116"/>
+      <c r="R22" s="116"/>
+      <c r="S22" s="116"/>
+      <c r="T22" s="117"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -17973,14 +18503,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="106" t="s">
+      <c r="O23" s="109" t="s">
         <v>281</v>
       </c>
-      <c r="P23" s="107"/>
-      <c r="Q23" s="107"/>
-      <c r="R23" s="107"/>
-      <c r="S23" s="107"/>
-      <c r="T23" s="108"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="110"/>
+      <c r="T23" s="111"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -17991,12 +18521,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="109"/>
-      <c r="P24" s="110"/>
-      <c r="Q24" s="110"/>
-      <c r="R24" s="110"/>
-      <c r="S24" s="110"/>
-      <c r="T24" s="111"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="113"/>
+      <c r="Q24" s="113"/>
+      <c r="R24" s="113"/>
+      <c r="S24" s="113"/>
+      <c r="T24" s="114"/>
     </row>
     <row r="25" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="23"/>
@@ -18007,12 +18537,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="112"/>
-      <c r="P25" s="113"/>
-      <c r="Q25" s="113"/>
-      <c r="R25" s="113"/>
-      <c r="S25" s="113"/>
-      <c r="T25" s="114"/>
+      <c r="O25" s="115"/>
+      <c r="P25" s="116"/>
+      <c r="Q25" s="116"/>
+      <c r="R25" s="116"/>
+      <c r="S25" s="116"/>
+      <c r="T25" s="117"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -18307,16 +18837,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -18873,16 +19403,16 @@
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -18946,14 +19476,14 @@
       <c r="L13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="104" t="s">
+      <c r="N13" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
+      <c r="S13" s="107"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -18976,12 +19506,12 @@
       <c r="L14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="104"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -18997,12 +19527,12 @@
       <c r="L15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="104"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
+      <c r="N15" s="107"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
     </row>
     <row r="16" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -19018,12 +19548,12 @@
       <c r="L16" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="107"/>
+      <c r="S16" s="107"/>
     </row>
     <row r="17" spans="3:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -19039,14 +19569,14 @@
       <c r="L17" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="N17" s="104" t="s">
+      <c r="N17" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="O17" s="104"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
+      <c r="O17" s="107"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="107"/>
+      <c r="S17" s="107"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -19062,12 +19592,12 @@
       <c r="L18" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="N18" s="104"/>
-      <c r="O18" s="104"/>
-      <c r="P18" s="104"/>
-      <c r="Q18" s="104"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="107"/>
+      <c r="Q18" s="107"/>
+      <c r="R18" s="107"/>
+      <c r="S18" s="107"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -19083,12 +19613,12 @@
       <c r="L19" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="N19" s="104"/>
-      <c r="O19" s="104"/>
-      <c r="P19" s="104"/>
-      <c r="Q19" s="104"/>
-      <c r="R19" s="104"/>
-      <c r="S19" s="104"/>
+      <c r="N19" s="107"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="107"/>
+      <c r="S19" s="107"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -19104,12 +19634,12 @@
       <c r="L20" s="87" t="s">
         <v>170</v>
       </c>
-      <c r="N20" s="104"/>
-      <c r="O20" s="104"/>
-      <c r="P20" s="104"/>
-      <c r="Q20" s="104"/>
-      <c r="R20" s="104"/>
-      <c r="S20" s="104"/>
+      <c r="N20" s="107"/>
+      <c r="O20" s="107"/>
+      <c r="P20" s="107"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="107"/>
+      <c r="S20" s="107"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -19140,14 +19670,14 @@
       <c r="L22" s="87" t="s">
         <v>254</v>
       </c>
-      <c r="N22" s="105" t="s">
+      <c r="N22" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="O22" s="105"/>
-      <c r="P22" s="105"/>
-      <c r="Q22" s="105"/>
-      <c r="R22" s="105"/>
-      <c r="S22" s="105"/>
+      <c r="O22" s="108"/>
+      <c r="P22" s="108"/>
+      <c r="Q22" s="108"/>
+      <c r="R22" s="108"/>
+      <c r="S22" s="108"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -19172,14 +19702,14 @@
       <c r="J24" s="2"/>
       <c r="K24" s="9"/>
       <c r="L24" s="87"/>
-      <c r="N24" s="104" t="s">
+      <c r="N24" s="107" t="s">
         <v>401</v>
       </c>
-      <c r="O24" s="104"/>
-      <c r="P24" s="104"/>
-      <c r="Q24" s="104"/>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
+      <c r="O24" s="107"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="107"/>
+      <c r="R24" s="107"/>
+      <c r="S24" s="107"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -19189,12 +19719,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="9"/>
       <c r="L25" s="87"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104"/>
-      <c r="Q25" s="104"/>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
+      <c r="N25" s="107"/>
+      <c r="O25" s="107"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="107"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -19204,12 +19734,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
-      <c r="N26" s="104"/>
-      <c r="O26" s="104"/>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
-      <c r="S26" s="104"/>
+      <c r="N26" s="107"/>
+      <c r="O26" s="107"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
+      <c r="S26" s="107"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -19219,12 +19749,12 @@
       <c r="J27" s="2"/>
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
-      <c r="N27" s="104"/>
-      <c r="O27" s="104"/>
-      <c r="P27" s="104"/>
-      <c r="Q27" s="104"/>
-      <c r="R27" s="104"/>
-      <c r="S27" s="104"/>
+      <c r="N27" s="107"/>
+      <c r="O27" s="107"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -19234,14 +19764,14 @@
       <c r="J28" s="2"/>
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="104" t="s">
+      <c r="N28" s="107" t="s">
         <v>148</v>
       </c>
-      <c r="O28" s="104"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="104"/>
-      <c r="S28" s="104"/>
+      <c r="O28" s="107"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -19251,12 +19781,12 @@
       <c r="J29" s="2"/>
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
-      <c r="N29" s="104"/>
-      <c r="O29" s="104"/>
-      <c r="P29" s="104"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="104"/>
-      <c r="S29" s="104"/>
+      <c r="N29" s="107"/>
+      <c r="O29" s="107"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -19266,12 +19796,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
-      <c r="N30" s="104"/>
-      <c r="O30" s="104"/>
-      <c r="P30" s="104"/>
-      <c r="Q30" s="104"/>
-      <c r="R30" s="104"/>
-      <c r="S30" s="104"/>
+      <c r="N30" s="107"/>
+      <c r="O30" s="107"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -19281,12 +19811,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="9"/>
       <c r="L31" s="2"/>
-      <c r="N31" s="104"/>
-      <c r="O31" s="104"/>
-      <c r="P31" s="104"/>
-      <c r="Q31" s="104"/>
-      <c r="R31" s="104"/>
-      <c r="S31" s="104"/>
+      <c r="N31" s="107"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -19498,16 +20028,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="J10" s="101" t="s">
+      <c r="F10" s="105"/>
+      <c r="G10" s="106"/>
+      <c r="J10" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>

</xml_diff>

<commit_message>
Fixed Issue on Spreadsheet
</commit_message>
<xml_diff>
--- a/Game Stuff/Spreadsheet.xlsx
+++ b/Game Stuff/Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 6\Game Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Aetherflux Reactor 7\Game Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F867011-79E7-4E0E-9B32-84D22445469B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4675A012-5E13-429B-A70A-1B60FC8F334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="21" activeTab="23" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
+    <workbookView xWindow="45972" yWindow="-4944" windowWidth="17496" windowHeight="30216" firstSheet="20" activeTab="22" xr2:uid="{E9D95B66-7EA4-4203-9BE9-B35EAC251241}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Summary" sheetId="1" r:id="rId1"/>
@@ -2347,7 +2347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2536,6 +2536,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2629,11 +2630,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2643,11 +2639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2986,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEAD1A-BE12-4BD3-A45F-18807DFF108B}">
   <dimension ref="B2:T124"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3005,18 +2997,18 @@
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="105"/>
-      <c r="E4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="107"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="104" t="s">
+      <c r="H4" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="107"/>
     </row>
     <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="35" t="s">
@@ -3355,7 +3347,7 @@
       </c>
       <c r="D21" s="38">
         <f>'Ydris’ Nexus'!K13</f>
-        <v>456.55555555555554</v>
+        <v>142.55555555555554</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>418</v>
@@ -4695,16 +4687,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -5164,17 +5156,17 @@
     </row>
     <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
-      <c r="M10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="106"/>
+      <c r="M10" s="107"/>
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -5221,14 +5213,14 @@
         <v>8</v>
       </c>
       <c r="M12" s="19"/>
-      <c r="O12" s="107" t="s">
+      <c r="O12" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="P12" s="107"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="108"/>
+      <c r="T12" s="108"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -5252,12 +5244,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="O13" s="107"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="107"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="108"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="108"/>
+      <c r="T13" s="108"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -5275,12 +5267,12 @@
         <v>25</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107"/>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -5297,12 +5289,12 @@
         <v>8</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
+      <c r="O15" s="108"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
+      <c r="T15" s="108"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -5319,14 +5311,14 @@
         <v>111</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="O16" s="107" t="s">
+      <c r="O16" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107"/>
-      <c r="T16" s="107"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="108"/>
+      <c r="T16" s="108"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -5343,12 +5335,12 @@
         <v>111</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="O17" s="107"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="108"/>
+      <c r="T17" s="108"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -5365,12 +5357,12 @@
         <v>147</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="107"/>
-      <c r="P18" s="107"/>
-      <c r="Q18" s="107"/>
-      <c r="R18" s="107"/>
-      <c r="S18" s="107"/>
-      <c r="T18" s="107"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="108"/>
+      <c r="T18" s="108"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -5387,12 +5379,12 @@
         <v>147</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="107"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="107"/>
-      <c r="S19" s="107"/>
-      <c r="T19" s="107"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="108"/>
+      <c r="T19" s="108"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -5425,14 +5417,14 @@
         <v>200</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="O21" s="108" t="s">
+      <c r="O21" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="P21" s="108"/>
-      <c r="Q21" s="108"/>
-      <c r="R21" s="108"/>
-      <c r="S21" s="108"/>
-      <c r="T21" s="108"/>
+      <c r="P21" s="109"/>
+      <c r="Q21" s="109"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="109"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -5466,14 +5458,14 @@
         <v>399</v>
       </c>
       <c r="M23" s="2"/>
-      <c r="O23" s="107" t="s">
+      <c r="O23" s="108" t="s">
         <v>400</v>
       </c>
-      <c r="P23" s="107"/>
-      <c r="Q23" s="107"/>
-      <c r="R23" s="107"/>
-      <c r="S23" s="107"/>
-      <c r="T23" s="107"/>
+      <c r="P23" s="108"/>
+      <c r="Q23" s="108"/>
+      <c r="R23" s="108"/>
+      <c r="S23" s="108"/>
+      <c r="T23" s="108"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -5491,12 +5483,12 @@
         <v>450</v>
       </c>
       <c r="M24" s="2"/>
-      <c r="O24" s="107"/>
-      <c r="P24" s="107"/>
-      <c r="Q24" s="107"/>
-      <c r="R24" s="107"/>
-      <c r="S24" s="107"/>
-      <c r="T24" s="107"/>
+      <c r="O24" s="108"/>
+      <c r="P24" s="108"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="108"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -5507,12 +5499,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="4"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="108"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="108"/>
+      <c r="S25" s="108"/>
+      <c r="T25" s="108"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -5523,12 +5515,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="108"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="108"/>
+      <c r="S26" s="108"/>
+      <c r="T26" s="108"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -5539,14 +5531,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="107" t="s">
+      <c r="O27" s="108" t="s">
         <v>464</v>
       </c>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
+      <c r="P27" s="108"/>
+      <c r="Q27" s="108"/>
+      <c r="R27" s="108"/>
+      <c r="S27" s="108"/>
+      <c r="T27" s="108"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -5557,12 +5549,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
-      <c r="T28" s="107"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
+      <c r="Q28" s="108"/>
+      <c r="R28" s="108"/>
+      <c r="S28" s="108"/>
+      <c r="T28" s="108"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -5573,12 +5565,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="108"/>
+      <c r="T29" s="108"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -5589,12 +5581,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
-      <c r="T30" s="107"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="108"/>
+      <c r="T30" s="108"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -5830,16 +5822,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6391,16 +6383,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -6894,16 +6886,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -7415,16 +7407,16 @@
       </c>
     </row>
     <row r="12" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G12" s="121" t="s">
+      <c r="G12" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="122"/>
-      <c r="I12" s="123"/>
-      <c r="L12" s="121" t="s">
+      <c r="H12" s="123"/>
+      <c r="I12" s="124"/>
+      <c r="L12" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="122"/>
-      <c r="N12" s="123"/>
+      <c r="M12" s="123"/>
+      <c r="N12" s="124"/>
     </row>
     <row r="13" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G13" s="51" t="s">
@@ -7887,16 +7879,16 @@
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -8426,16 +8418,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -8941,16 +8933,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -9459,16 +9451,16 @@
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="23"/>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="105"/>
-      <c r="G13" s="106"/>
-      <c r="J13" s="104" t="s">
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
+      <c r="J13" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="105"/>
-      <c r="L13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="107"/>
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
@@ -9880,16 +9872,16 @@
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="104" t="s">
+      <c r="F4" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
-      <c r="K4" s="104" t="s">
+      <c r="G4" s="106"/>
+      <c r="H4" s="107"/>
+      <c r="K4" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="105"/>
-      <c r="M4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="107"/>
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="17" t="s">
@@ -10415,31 +10407,31 @@
     </row>
     <row r="18" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="23"/>
-      <c r="E18" s="104" t="s">
+      <c r="E18" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="106"/>
-      <c r="K18" s="104" t="s">
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="107"/>
+      <c r="K18" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="105"/>
-      <c r="M18" s="106"/>
-      <c r="O18" s="104" t="s">
+      <c r="L18" s="106"/>
+      <c r="M18" s="107"/>
+      <c r="O18" s="105" t="s">
         <v>264</v>
       </c>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="106"/>
-      <c r="V18" s="104" t="s">
+      <c r="P18" s="106"/>
+      <c r="Q18" s="106"/>
+      <c r="R18" s="106"/>
+      <c r="S18" s="106"/>
+      <c r="T18" s="107"/>
+      <c r="V18" s="105" t="s">
         <v>275</v>
       </c>
-      <c r="W18" s="105"/>
-      <c r="X18" s="105"/>
-      <c r="Y18" s="106"/>
+      <c r="W18" s="106"/>
+      <c r="X18" s="106"/>
+      <c r="Y18" s="107"/>
       <c r="AA18" s="72" t="s">
         <v>285</v>
       </c>
@@ -10482,26 +10474,26 @@
       <c r="M19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="129" t="s">
+      <c r="O19" s="130" t="s">
         <v>265</v>
       </c>
-      <c r="P19" s="130"/>
-      <c r="Q19" s="127" t="s">
+      <c r="P19" s="131"/>
+      <c r="Q19" s="128" t="s">
         <v>266</v>
       </c>
-      <c r="R19" s="128"/>
-      <c r="S19" s="127" t="s">
+      <c r="R19" s="129"/>
+      <c r="S19" s="128" t="s">
         <v>272</v>
       </c>
-      <c r="T19" s="128"/>
-      <c r="V19" s="129" t="s">
+      <c r="T19" s="129"/>
+      <c r="V19" s="130" t="s">
         <v>256</v>
       </c>
-      <c r="W19" s="130"/>
-      <c r="X19" s="129" t="s">
+      <c r="W19" s="131"/>
+      <c r="X19" s="130" t="s">
         <v>274</v>
       </c>
-      <c r="Y19" s="131"/>
+      <c r="Y19" s="132"/>
       <c r="AA19" s="76" t="s">
         <v>304</v>
       </c>
@@ -11116,12 +11108,12 @@
       <c r="V29" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="W29" s="124">
+      <c r="W29" s="125">
         <f>W28+Y28</f>
         <v>372.36370370370366</v>
       </c>
-      <c r="X29" s="125"/>
-      <c r="Y29" s="126"/>
+      <c r="X29" s="126"/>
+      <c r="Y29" s="127"/>
       <c r="AA29" s="79" t="s">
         <v>291</v>
       </c>
@@ -12833,17 +12825,17 @@
     </row>
     <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="23"/>
-      <c r="E15" s="132" t="s">
+      <c r="E15" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="133"/>
-      <c r="G15" s="133"/>
-      <c r="H15" s="134"/>
-      <c r="J15" s="104" t="s">
+      <c r="F15" s="134"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="135"/>
+      <c r="J15" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="106"/>
+      <c r="K15" s="106"/>
+      <c r="L15" s="107"/>
     </row>
     <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="23"/>
@@ -13366,17 +13358,17 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="134"/>
-      <c r="J11" s="104" t="s">
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="135"/>
+      <c r="J11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="106"/>
+      <c r="K11" s="106"/>
+      <c r="L11" s="107"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -13822,8 +13814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878EF637-2B1F-4BC8-A0FA-F77EC5044F15}">
   <dimension ref="B1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13917,24 +13909,24 @@
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="134"/>
-      <c r="J11" s="104" t="s">
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="135"/>
+      <c r="J11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="106"/>
-      <c r="N11" s="121" t="s">
+      <c r="K11" s="106"/>
+      <c r="L11" s="107"/>
+      <c r="N11" s="122" t="s">
         <v>426</v>
       </c>
-      <c r="O11" s="122"/>
-      <c r="P11" s="122"/>
-      <c r="Q11" s="122"/>
-      <c r="R11" s="123"/>
+      <c r="O11" s="123"/>
+      <c r="P11" s="123"/>
+      <c r="Q11" s="123"/>
+      <c r="R11" s="124"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -13992,7 +13984,7 @@
       </c>
       <c r="K13" s="8">
         <f>597-K19</f>
-        <v>456.55555555555554</v>
+        <v>142.55555555555554</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>25</v>
@@ -14194,8 +14186,8 @@
         <v>447</v>
       </c>
       <c r="K19" s="9">
-        <f>140+4/9</f>
-        <v>140.44444444444446</v>
+        <f>4090/9</f>
+        <v>454.44444444444446</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>450</v>
@@ -14419,13 +14411,13 @@
       <c r="N27" s="93" t="s">
         <v>270</v>
       </c>
-      <c r="O27" s="125">
+      <c r="O27" s="126">
         <f>SUM(Q13:Q26)</f>
         <v>36259.599999999999</v>
       </c>
-      <c r="P27" s="125"/>
-      <c r="Q27" s="125"/>
-      <c r="R27" s="126"/>
+      <c r="P27" s="126"/>
+      <c r="Q27" s="126"/>
+      <c r="R27" s="127"/>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -14612,10 +14604,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC07E90-6101-47F8-9701-BB9D283EFF37}">
-  <dimension ref="B1:S75"/>
+  <dimension ref="B1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14726,25 +14718,25 @@
     </row>
     <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="23"/>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="134"/>
-      <c r="J13" s="104" t="s">
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="135"/>
+      <c r="J13" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="105"/>
-      <c r="L13" s="106"/>
-      <c r="N13" s="127" t="s">
+      <c r="K13" s="106"/>
+      <c r="L13" s="107"/>
+      <c r="N13" s="128" t="s">
         <v>492</v>
       </c>
-      <c r="O13" s="138"/>
-      <c r="P13" s="138"/>
-      <c r="Q13" s="138"/>
-      <c r="R13" s="138"/>
-      <c r="S13" s="141"/>
+      <c r="O13" s="136"/>
+      <c r="P13" s="136"/>
+      <c r="Q13" s="136"/>
+      <c r="R13" s="136"/>
+      <c r="S13" s="104"/>
     </row>
     <row r="14" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
@@ -14769,22 +14761,22 @@
       <c r="L14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="143" t="s">
+      <c r="N14" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="O14" s="143" t="s">
+      <c r="O14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P14" s="143" t="s">
+      <c r="P14" s="14" t="s">
         <v>490</v>
       </c>
-      <c r="Q14" s="143" t="s">
+      <c r="Q14" s="14" t="s">
         <v>491</v>
       </c>
-      <c r="R14" s="143" t="s">
+      <c r="R14" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="S14" s="143" t="s">
+      <c r="S14" s="14" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14874,7 +14866,7 @@
         <v>961.4</v>
       </c>
       <c r="S16" s="2">
-        <f t="shared" ref="S16:S31" si="0">R16*O16</f>
+        <f t="shared" ref="S16:S24" si="0">R16*O16</f>
         <v>9614</v>
       </c>
     </row>
@@ -15266,14 +15258,14 @@
       <c r="N25" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="O25" s="139">
+      <c r="O25" s="137">
         <f>SUM(S15:S24)</f>
         <v>31929.550000000003</v>
       </c>
-      <c r="P25" s="140"/>
-      <c r="Q25" s="140"/>
-      <c r="R25" s="140"/>
-      <c r="S25" s="142"/>
+      <c r="P25" s="138"/>
+      <c r="Q25" s="138"/>
+      <c r="R25" s="138"/>
+      <c r="S25" s="139"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -15801,18 +15793,18 @@
       <c r="H51" s="67"/>
     </row>
     <row r="52" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E52" s="121" t="s">
+      <c r="E52" s="122" t="s">
         <v>483</v>
       </c>
-      <c r="F52" s="122"/>
-      <c r="G52" s="122"/>
-      <c r="H52" s="123"/>
-      <c r="J52" s="121" t="s">
+      <c r="F52" s="123"/>
+      <c r="G52" s="123"/>
+      <c r="H52" s="124"/>
+      <c r="J52" s="122" t="s">
         <v>483</v>
       </c>
-      <c r="K52" s="122"/>
-      <c r="L52" s="123"/>
-      <c r="M52" s="135"/>
+      <c r="K52" s="123"/>
+      <c r="L52" s="124"/>
+      <c r="M52" s="13"/>
     </row>
     <row r="53" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E53" s="14" t="s">
@@ -15836,7 +15828,6 @@
       <c r="L53" s="53" t="s">
         <v>406</v>
       </c>
-      <c r="M53" s="136"/>
     </row>
     <row r="54" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E54" s="4" t="s">
@@ -15858,7 +15849,6 @@
         <v>0.29958847736625516</v>
       </c>
       <c r="L54" s="41"/>
-      <c r="M54" s="136"/>
     </row>
     <row r="55" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E55" s="2" t="s">
@@ -15878,7 +15868,6 @@
         <v>2.5</v>
       </c>
       <c r="L55" s="40"/>
-      <c r="M55" s="136"/>
     </row>
     <row r="56" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E56" s="2" t="s">
@@ -15899,7 +15888,6 @@
         <v>5</v>
       </c>
       <c r="L56" s="40"/>
-      <c r="M56" s="136"/>
     </row>
     <row r="57" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E57" s="2" t="s">
@@ -15919,7 +15907,6 @@
         <v>5</v>
       </c>
       <c r="L57" s="40"/>
-      <c r="M57" s="136"/>
     </row>
     <row r="58" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E58" s="2" t="s">
@@ -15940,7 +15927,6 @@
         <v>5</v>
       </c>
       <c r="L58" s="40"/>
-      <c r="M58" s="136"/>
     </row>
     <row r="59" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E59" s="2" t="s">
@@ -15961,7 +15947,6 @@
         <v>5</v>
       </c>
       <c r="L59" s="40"/>
-      <c r="M59" s="136"/>
     </row>
     <row r="60" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E60" s="2" t="s">
@@ -15981,7 +15966,6 @@
         <v>5</v>
       </c>
       <c r="L60" s="40"/>
-      <c r="M60" s="136"/>
     </row>
     <row r="61" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E61" s="2" t="s">
@@ -16003,7 +15987,6 @@
         <v>14.666666666666666</v>
       </c>
       <c r="L61" s="40"/>
-      <c r="M61" s="136"/>
     </row>
     <row r="62" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E62" s="2" t="s">
@@ -16023,7 +16006,6 @@
         <v>15</v>
       </c>
       <c r="L62" s="40"/>
-      <c r="M62" s="136"/>
     </row>
     <row r="63" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E63" s="2" t="s">
@@ -16043,7 +16025,6 @@
         <v>30</v>
       </c>
       <c r="L63" s="40"/>
-      <c r="M63" s="136"/>
     </row>
     <row r="64" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E64" s="2" t="s">
@@ -16063,9 +16044,8 @@
         <v>45</v>
       </c>
       <c r="L64" s="40"/>
-      <c r="M64" s="136"/>
-    </row>
-    <row r="65" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E65" s="2" t="s">
         <v>132</v>
       </c>
@@ -16083,9 +16063,8 @@
         <v>45</v>
       </c>
       <c r="L65" s="40"/>
-      <c r="M65" s="136"/>
-    </row>
-    <row r="66" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E66" s="2" t="s">
         <v>17</v>
       </c>
@@ -16104,9 +16083,8 @@
         <v>202.33333333333334</v>
       </c>
       <c r="L66" s="40"/>
-      <c r="M66" s="136"/>
-    </row>
-    <row r="67" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E67" s="2" t="s">
         <v>164</v>
       </c>
@@ -16125,9 +16103,8 @@
         <v>398.18666666666667</v>
       </c>
       <c r="L67" s="40"/>
-      <c r="M67" s="136"/>
-    </row>
-    <row r="68" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E68" s="2" t="s">
         <v>484</v>
       </c>
@@ -16146,9 +16123,8 @@
         <v>537.22400000000005</v>
       </c>
       <c r="L68" s="40"/>
-      <c r="M68" s="136"/>
-    </row>
-    <row r="69" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E69" s="2" t="s">
         <v>49</v>
       </c>
@@ -16167,9 +16143,8 @@
         <v>593.75</v>
       </c>
       <c r="L69" s="40"/>
-      <c r="M69" s="136"/>
-    </row>
-    <row r="70" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E70" s="2" t="s">
         <v>61</v>
       </c>
@@ -16189,9 +16164,8 @@
         <v>750.05259259259265</v>
       </c>
       <c r="L70" s="40"/>
-      <c r="M70" s="136"/>
-    </row>
-    <row r="71" spans="5:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E71" s="2" t="s">
         <v>34</v>
       </c>
@@ -16211,9 +16185,8 @@
         <v>996.69444444444446</v>
       </c>
       <c r="L71" s="2"/>
-      <c r="M71" s="136"/>
-    </row>
-    <row r="72" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="72" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E72" s="3" t="s">
         <v>19</v>
       </c>
@@ -16233,25 +16206,9 @@
         <v>1491.1666666666667</v>
       </c>
       <c r="L72" s="2"/>
-      <c r="M72" s="136"/>
-    </row>
-    <row r="73" spans="5:13" x14ac:dyDescent="0.35">
-      <c r="J73" s="136"/>
-      <c r="K73" s="137"/>
-      <c r="L73" s="136"/>
-      <c r="M73" s="136"/>
-    </row>
-    <row r="74" spans="5:13" x14ac:dyDescent="0.35">
-      <c r="J74" s="136"/>
-      <c r="K74" s="136"/>
-      <c r="L74" s="136"/>
-      <c r="M74" s="136"/>
-    </row>
-    <row r="75" spans="5:13" x14ac:dyDescent="0.35">
-      <c r="J75" s="136"/>
-      <c r="K75" s="136"/>
-      <c r="L75" s="136"/>
-      <c r="M75" s="136"/>
+    </row>
+    <row r="73" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="K73" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J54:L72">
@@ -16360,17 +16317,17 @@
     </row>
     <row r="12" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F13" s="104" t="s">
+      <c r="F13" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="106"/>
-      <c r="K13" s="104" t="s">
+      <c r="G13" s="106"/>
+      <c r="H13" s="107"/>
+      <c r="K13" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="107"/>
     </row>
     <row r="14" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F14" s="14" t="s">
@@ -16394,14 +16351,14 @@
       <c r="N14" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="P14" s="107" t="s">
+      <c r="P14" s="108" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
-      <c r="U14" s="107"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F15" s="4" t="s">
@@ -16424,12 +16381,12 @@
         <v>25</v>
       </c>
       <c r="N15" s="19"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
-      <c r="U15" s="107"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
+      <c r="T15" s="108"/>
+      <c r="U15" s="108"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.35">
       <c r="F16" s="2" t="s">
@@ -16453,12 +16410,12 @@
       <c r="N16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107"/>
-      <c r="T16" s="107"/>
-      <c r="U16" s="107"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="108"/>
+      <c r="T16" s="108"/>
+      <c r="U16" s="108"/>
     </row>
     <row r="17" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
@@ -16476,12 +16433,12 @@
       <c r="N17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
-      <c r="U17" s="107"/>
+      <c r="P17" s="108"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="108"/>
+      <c r="T17" s="108"/>
+      <c r="U17" s="108"/>
     </row>
     <row r="18" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
@@ -16531,14 +16488,14 @@
         <v>170</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="P20" s="108" t="s">
+      <c r="P20" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="Q20" s="108"/>
-      <c r="R20" s="108"/>
-      <c r="S20" s="108"/>
-      <c r="T20" s="108"/>
-      <c r="U20" s="108"/>
+      <c r="Q20" s="109"/>
+      <c r="R20" s="109"/>
+      <c r="S20" s="109"/>
+      <c r="T20" s="109"/>
+      <c r="U20" s="109"/>
     </row>
     <row r="21" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
@@ -16570,14 +16527,14 @@
         <v>159</v>
       </c>
       <c r="N22" s="2"/>
-      <c r="P22" s="107" t="s">
+      <c r="P22" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="Q22" s="107"/>
-      <c r="R22" s="107"/>
-      <c r="S22" s="107"/>
-      <c r="T22" s="107"/>
-      <c r="U22" s="107"/>
+      <c r="Q22" s="108"/>
+      <c r="R22" s="108"/>
+      <c r="S22" s="108"/>
+      <c r="T22" s="108"/>
+      <c r="U22" s="108"/>
     </row>
     <row r="23" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
@@ -16594,12 +16551,12 @@
         <v>252</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="P23" s="107"/>
-      <c r="Q23" s="107"/>
-      <c r="R23" s="107"/>
-      <c r="S23" s="107"/>
-      <c r="T23" s="107"/>
-      <c r="U23" s="107"/>
+      <c r="P23" s="108"/>
+      <c r="Q23" s="108"/>
+      <c r="R23" s="108"/>
+      <c r="S23" s="108"/>
+      <c r="T23" s="108"/>
+      <c r="U23" s="108"/>
     </row>
     <row r="24" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
@@ -16616,12 +16573,12 @@
         <v>377</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="P24" s="107"/>
-      <c r="Q24" s="107"/>
-      <c r="R24" s="107"/>
-      <c r="S24" s="107"/>
-      <c r="T24" s="107"/>
-      <c r="U24" s="107"/>
+      <c r="P24" s="108"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="108"/>
+      <c r="U24" s="108"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
@@ -16640,12 +16597,12 @@
       <c r="N25" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
-      <c r="U25" s="107"/>
+      <c r="P25" s="108"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="108"/>
+      <c r="S25" s="108"/>
+      <c r="T25" s="108"/>
+      <c r="U25" s="108"/>
     </row>
     <row r="26" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
@@ -16661,14 +16618,14 @@
         <v>418</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="P26" s="107" t="s">
+      <c r="P26" s="108" t="s">
         <v>263</v>
       </c>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
-      <c r="U26" s="107"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="108"/>
+      <c r="S26" s="108"/>
+      <c r="T26" s="108"/>
+      <c r="U26" s="108"/>
     </row>
     <row r="27" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
@@ -16678,12 +16635,12 @@
       <c r="L27" s="9"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
-      <c r="U27" s="107"/>
+      <c r="P27" s="108"/>
+      <c r="Q27" s="108"/>
+      <c r="R27" s="108"/>
+      <c r="S27" s="108"/>
+      <c r="T27" s="108"/>
+      <c r="U27" s="108"/>
     </row>
     <row r="28" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
@@ -16693,12 +16650,12 @@
       <c r="L28" s="9"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
-      <c r="T28" s="107"/>
-      <c r="U28" s="107"/>
+      <c r="P28" s="108"/>
+      <c r="Q28" s="108"/>
+      <c r="R28" s="108"/>
+      <c r="S28" s="108"/>
+      <c r="T28" s="108"/>
+      <c r="U28" s="108"/>
     </row>
     <row r="29" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
@@ -16708,12 +16665,12 @@
       <c r="L29" s="9"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
-      <c r="U29" s="107"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="108"/>
+      <c r="T29" s="108"/>
+      <c r="U29" s="108"/>
     </row>
     <row r="30" spans="6:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
@@ -16723,14 +16680,14 @@
       <c r="L30" s="9"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="P30" s="107" t="s">
+      <c r="P30" s="108" t="s">
         <v>409</v>
       </c>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
-      <c r="T30" s="107"/>
-      <c r="U30" s="107"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="108"/>
+      <c r="T30" s="108"/>
+      <c r="U30" s="108"/>
     </row>
     <row r="31" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
@@ -16740,12 +16697,12 @@
       <c r="L31" s="9"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
-      <c r="T31" s="107"/>
-      <c r="U31" s="107"/>
+      <c r="P31" s="108"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="108"/>
+      <c r="S31" s="108"/>
+      <c r="T31" s="108"/>
+      <c r="U31" s="108"/>
     </row>
     <row r="32" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
@@ -16755,12 +16712,12 @@
       <c r="L32" s="9"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
-      <c r="U32" s="107"/>
+      <c r="P32" s="108"/>
+      <c r="Q32" s="108"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="108"/>
+      <c r="T32" s="108"/>
+      <c r="U32" s="108"/>
     </row>
     <row r="33" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
@@ -16770,12 +16727,12 @@
       <c r="L33" s="9"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="P33" s="107"/>
-      <c r="Q33" s="107"/>
-      <c r="R33" s="107"/>
-      <c r="S33" s="107"/>
-      <c r="T33" s="107"/>
-      <c r="U33" s="107"/>
+      <c r="P33" s="108"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="108"/>
+      <c r="S33" s="108"/>
+      <c r="T33" s="108"/>
+      <c r="U33" s="108"/>
     </row>
     <row r="34" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
@@ -16785,14 +16742,14 @@
       <c r="L34" s="9"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="P34" s="107" t="s">
+      <c r="P34" s="108" t="s">
         <v>419</v>
       </c>
-      <c r="Q34" s="107"/>
-      <c r="R34" s="107"/>
-      <c r="S34" s="107"/>
-      <c r="T34" s="107"/>
-      <c r="U34" s="107"/>
+      <c r="Q34" s="108"/>
+      <c r="R34" s="108"/>
+      <c r="S34" s="108"/>
+      <c r="T34" s="108"/>
+      <c r="U34" s="108"/>
     </row>
     <row r="35" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
@@ -16802,12 +16759,12 @@
       <c r="L35" s="9"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="P35" s="107"/>
-      <c r="Q35" s="107"/>
-      <c r="R35" s="107"/>
-      <c r="S35" s="107"/>
-      <c r="T35" s="107"/>
-      <c r="U35" s="107"/>
+      <c r="P35" s="108"/>
+      <c r="Q35" s="108"/>
+      <c r="R35" s="108"/>
+      <c r="S35" s="108"/>
+      <c r="T35" s="108"/>
+      <c r="U35" s="108"/>
     </row>
     <row r="36" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
@@ -16817,12 +16774,12 @@
       <c r="L36" s="9"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="P36" s="107"/>
-      <c r="Q36" s="107"/>
-      <c r="R36" s="107"/>
-      <c r="S36" s="107"/>
-      <c r="T36" s="107"/>
-      <c r="U36" s="107"/>
+      <c r="P36" s="108"/>
+      <c r="Q36" s="108"/>
+      <c r="R36" s="108"/>
+      <c r="S36" s="108"/>
+      <c r="T36" s="108"/>
+      <c r="U36" s="108"/>
     </row>
     <row r="37" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
@@ -16832,12 +16789,12 @@
       <c r="L37" s="9"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="P37" s="107"/>
-      <c r="Q37" s="107"/>
-      <c r="R37" s="107"/>
-      <c r="S37" s="107"/>
-      <c r="T37" s="107"/>
-      <c r="U37" s="107"/>
+      <c r="P37" s="108"/>
+      <c r="Q37" s="108"/>
+      <c r="R37" s="108"/>
+      <c r="S37" s="108"/>
+      <c r="T37" s="108"/>
+      <c r="U37" s="108"/>
     </row>
     <row r="38" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
@@ -17038,16 +16995,16 @@
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-      <c r="J11" s="104" t="s">
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
+      <c r="J11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="106"/>
+      <c r="K11" s="106"/>
+      <c r="L11" s="107"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -17529,17 +17486,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-      <c r="J11" s="104" t="s">
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
+      <c r="J11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="106"/>
+      <c r="K11" s="106"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="107"/>
     </row>
     <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -17564,14 +17521,14 @@
       <c r="M12" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O12" s="107" t="s">
+      <c r="O12" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="107"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="108"/>
+      <c r="T12" s="108"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -17595,12 +17552,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="107"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="107"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="108"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="108"/>
+      <c r="T13" s="108"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -17625,12 +17582,12 @@
       <c r="M14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107"/>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -17649,12 +17606,12 @@
       <c r="M15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
+      <c r="O15" s="108"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
+      <c r="T15" s="108"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -17673,14 +17630,14 @@
       <c r="M16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O16" s="107" t="s">
+      <c r="O16" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107"/>
-      <c r="T16" s="107"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="108"/>
+      <c r="T16" s="108"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -17699,12 +17656,12 @@
       <c r="M17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="O17" s="107"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="108"/>
+      <c r="T17" s="108"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -17721,12 +17678,12 @@
         <v>147</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="O18" s="107"/>
-      <c r="P18" s="107"/>
-      <c r="Q18" s="107"/>
-      <c r="R18" s="107"/>
-      <c r="S18" s="107"/>
-      <c r="T18" s="107"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="108"/>
+      <c r="T18" s="108"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -17743,12 +17700,12 @@
         <v>170</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="107"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="107"/>
-      <c r="S19" s="107"/>
-      <c r="T19" s="107"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="108"/>
+      <c r="T19" s="108"/>
     </row>
     <row r="20" spans="3:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -17776,14 +17733,14 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="108" t="s">
+      <c r="O21" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="P21" s="108"/>
-      <c r="Q21" s="108"/>
-      <c r="R21" s="108"/>
-      <c r="S21" s="108"/>
-      <c r="T21" s="108"/>
+      <c r="P21" s="109"/>
+      <c r="Q21" s="109"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="109"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -17804,14 +17761,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="107" t="s">
+      <c r="O23" s="108" t="s">
         <v>171</v>
       </c>
-      <c r="P23" s="107"/>
-      <c r="Q23" s="107"/>
-      <c r="R23" s="107"/>
-      <c r="S23" s="107"/>
-      <c r="T23" s="107"/>
+      <c r="P23" s="108"/>
+      <c r="Q23" s="108"/>
+      <c r="R23" s="108"/>
+      <c r="S23" s="108"/>
+      <c r="T23" s="108"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -17822,12 +17779,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="107"/>
-      <c r="P24" s="107"/>
-      <c r="Q24" s="107"/>
-      <c r="R24" s="107"/>
-      <c r="S24" s="107"/>
-      <c r="T24" s="107"/>
+      <c r="O24" s="108"/>
+      <c r="P24" s="108"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="108"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -17838,12 +17795,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="108"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="108"/>
+      <c r="S25" s="108"/>
+      <c r="T25" s="108"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -17854,12 +17811,12 @@
       <c r="K26" s="9"/>
       <c r="L26" s="6"/>
       <c r="M26" s="2"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="108"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="108"/>
+      <c r="S26" s="108"/>
+      <c r="T26" s="108"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -17870,14 +17827,14 @@
       <c r="K27" s="9"/>
       <c r="L27" s="6"/>
       <c r="M27" s="2"/>
-      <c r="O27" s="107" t="s">
+      <c r="O27" s="108" t="s">
         <v>149</v>
       </c>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
+      <c r="P27" s="108"/>
+      <c r="Q27" s="108"/>
+      <c r="R27" s="108"/>
+      <c r="S27" s="108"/>
+      <c r="T27" s="108"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -17888,12 +17845,12 @@
       <c r="K28" s="9"/>
       <c r="L28" s="6"/>
       <c r="M28" s="2"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
-      <c r="T28" s="107"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
+      <c r="Q28" s="108"/>
+      <c r="R28" s="108"/>
+      <c r="S28" s="108"/>
+      <c r="T28" s="108"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -17904,12 +17861,12 @@
       <c r="K29" s="9"/>
       <c r="L29" s="6"/>
       <c r="M29" s="2"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="108"/>
+      <c r="T29" s="108"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -17920,12 +17877,12 @@
       <c r="K30" s="9"/>
       <c r="L30" s="6"/>
       <c r="M30" s="2"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
-      <c r="T30" s="107"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="108"/>
+      <c r="T30" s="108"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -17936,14 +17893,14 @@
       <c r="K31" s="9"/>
       <c r="L31" s="6"/>
       <c r="M31" s="2"/>
-      <c r="O31" s="107" t="s">
+      <c r="O31" s="108" t="s">
         <v>150</v>
       </c>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
-      <c r="T31" s="107"/>
+      <c r="P31" s="108"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="108"/>
+      <c r="S31" s="108"/>
+      <c r="T31" s="108"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -17954,12 +17911,12 @@
       <c r="K32" s="9"/>
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
+      <c r="O32" s="108"/>
+      <c r="P32" s="108"/>
+      <c r="Q32" s="108"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="108"/>
+      <c r="T32" s="108"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C33" s="23"/>
@@ -17970,12 +17927,12 @@
       <c r="K33" s="9"/>
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
-      <c r="O33" s="107"/>
-      <c r="P33" s="107"/>
-      <c r="Q33" s="107"/>
-      <c r="R33" s="107"/>
-      <c r="S33" s="107"/>
-      <c r="T33" s="107"/>
+      <c r="O33" s="108"/>
+      <c r="P33" s="108"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="108"/>
+      <c r="S33" s="108"/>
+      <c r="T33" s="108"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C34" s="23"/>
@@ -17986,12 +17943,12 @@
       <c r="K34" s="9"/>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
-      <c r="O34" s="107"/>
-      <c r="P34" s="107"/>
-      <c r="Q34" s="107"/>
-      <c r="R34" s="107"/>
-      <c r="S34" s="107"/>
-      <c r="T34" s="107"/>
+      <c r="O34" s="108"/>
+      <c r="P34" s="108"/>
+      <c r="Q34" s="108"/>
+      <c r="R34" s="108"/>
+      <c r="S34" s="108"/>
+      <c r="T34" s="108"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C35" s="23"/>
@@ -18002,14 +17959,14 @@
       <c r="K35" s="9"/>
       <c r="L35" s="6"/>
       <c r="M35" s="2"/>
-      <c r="O35" s="107" t="s">
+      <c r="O35" s="108" t="s">
         <v>261</v>
       </c>
-      <c r="P35" s="107"/>
-      <c r="Q35" s="107"/>
-      <c r="R35" s="107"/>
-      <c r="S35" s="107"/>
-      <c r="T35" s="107"/>
+      <c r="P35" s="108"/>
+      <c r="Q35" s="108"/>
+      <c r="R35" s="108"/>
+      <c r="S35" s="108"/>
+      <c r="T35" s="108"/>
     </row>
     <row r="36" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C36" s="23"/>
@@ -18020,12 +17977,12 @@
       <c r="K36" s="9"/>
       <c r="L36" s="6"/>
       <c r="M36" s="2"/>
-      <c r="O36" s="107"/>
-      <c r="P36" s="107"/>
-      <c r="Q36" s="107"/>
-      <c r="R36" s="107"/>
-      <c r="S36" s="107"/>
-      <c r="T36" s="107"/>
+      <c r="O36" s="108"/>
+      <c r="P36" s="108"/>
+      <c r="Q36" s="108"/>
+      <c r="R36" s="108"/>
+      <c r="S36" s="108"/>
+      <c r="T36" s="108"/>
     </row>
     <row r="37" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E37" s="2"/>
@@ -18035,12 +17992,12 @@
       <c r="K37" s="9"/>
       <c r="L37" s="6"/>
       <c r="M37" s="2"/>
-      <c r="O37" s="107"/>
-      <c r="P37" s="107"/>
-      <c r="Q37" s="107"/>
-      <c r="R37" s="107"/>
-      <c r="S37" s="107"/>
-      <c r="T37" s="107"/>
+      <c r="O37" s="108"/>
+      <c r="P37" s="108"/>
+      <c r="Q37" s="108"/>
+      <c r="R37" s="108"/>
+      <c r="S37" s="108"/>
+      <c r="T37" s="108"/>
     </row>
     <row r="38" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E38" s="2"/>
@@ -18050,12 +18007,12 @@
       <c r="K38" s="9"/>
       <c r="L38" s="6"/>
       <c r="M38" s="2"/>
-      <c r="O38" s="107"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-      <c r="S38" s="107"/>
-      <c r="T38" s="107"/>
+      <c r="O38" s="108"/>
+      <c r="P38" s="108"/>
+      <c r="Q38" s="108"/>
+      <c r="R38" s="108"/>
+      <c r="S38" s="108"/>
+      <c r="T38" s="108"/>
     </row>
     <row r="39" spans="3:20" x14ac:dyDescent="0.35">
       <c r="E39" s="2"/>
@@ -18228,17 +18185,17 @@
     </row>
     <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-      <c r="J11" s="104" t="s">
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
+      <c r="J11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="106"/>
+      <c r="K11" s="106"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="107"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="23"/>
@@ -18263,14 +18220,14 @@
       <c r="M12" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="O12" s="107" t="s">
+      <c r="O12" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="P12" s="107"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="108"/>
+      <c r="T12" s="108"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
@@ -18294,12 +18251,12 @@
         <v>25</v>
       </c>
       <c r="M13" s="19"/>
-      <c r="O13" s="107"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="107"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="108"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="108"/>
+      <c r="T13" s="108"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -18322,12 +18279,12 @@
         <v>81</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107"/>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -18346,12 +18303,12 @@
       <c r="M15" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
+      <c r="O15" s="108"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
+      <c r="T15" s="108"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -18426,14 +18383,14 @@
       <c r="M19" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="O19" s="118" t="s">
+      <c r="O19" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="P19" s="119"/>
-      <c r="Q19" s="119"/>
-      <c r="R19" s="119"/>
-      <c r="S19" s="119"/>
-      <c r="T19" s="120"/>
+      <c r="P19" s="120"/>
+      <c r="Q19" s="120"/>
+      <c r="R19" s="120"/>
+      <c r="S19" s="120"/>
+      <c r="T19" s="121"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -18453,14 +18410,14 @@
       <c r="M20" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="O20" s="109" t="s">
+      <c r="O20" s="110" t="s">
         <v>405</v>
       </c>
-      <c r="P20" s="110"/>
-      <c r="Q20" s="110"/>
-      <c r="R20" s="110"/>
-      <c r="S20" s="110"/>
-      <c r="T20" s="111"/>
+      <c r="P20" s="111"/>
+      <c r="Q20" s="111"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="111"/>
+      <c r="T20" s="112"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -18471,12 +18428,12 @@
       <c r="K21" s="9"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2"/>
-      <c r="O21" s="112"/>
-      <c r="P21" s="113"/>
-      <c r="Q21" s="113"/>
-      <c r="R21" s="113"/>
-      <c r="S21" s="113"/>
-      <c r="T21" s="114"/>
+      <c r="O21" s="113"/>
+      <c r="P21" s="114"/>
+      <c r="Q21" s="114"/>
+      <c r="R21" s="114"/>
+      <c r="S21" s="114"/>
+      <c r="T21" s="115"/>
     </row>
     <row r="22" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="23"/>
@@ -18487,12 +18444,12 @@
       <c r="K22" s="9"/>
       <c r="L22" s="6"/>
       <c r="M22" s="2"/>
-      <c r="O22" s="115"/>
-      <c r="P22" s="116"/>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="116"/>
-      <c r="T22" s="117"/>
+      <c r="O22" s="116"/>
+      <c r="P22" s="117"/>
+      <c r="Q22" s="117"/>
+      <c r="R22" s="117"/>
+      <c r="S22" s="117"/>
+      <c r="T22" s="118"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -18503,14 +18460,14 @@
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2"/>
-      <c r="O23" s="109" t="s">
+      <c r="O23" s="110" t="s">
         <v>281</v>
       </c>
-      <c r="P23" s="110"/>
-      <c r="Q23" s="110"/>
-      <c r="R23" s="110"/>
-      <c r="S23" s="110"/>
-      <c r="T23" s="111"/>
+      <c r="P23" s="111"/>
+      <c r="Q23" s="111"/>
+      <c r="R23" s="111"/>
+      <c r="S23" s="111"/>
+      <c r="T23" s="112"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="23"/>
@@ -18521,12 +18478,12 @@
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
       <c r="M24" s="2"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="113"/>
-      <c r="Q24" s="113"/>
-      <c r="R24" s="113"/>
-      <c r="S24" s="113"/>
-      <c r="T24" s="114"/>
+      <c r="O24" s="113"/>
+      <c r="P24" s="114"/>
+      <c r="Q24" s="114"/>
+      <c r="R24" s="114"/>
+      <c r="S24" s="114"/>
+      <c r="T24" s="115"/>
     </row>
     <row r="25" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="23"/>
@@ -18537,12 +18494,12 @@
       <c r="K25" s="9"/>
       <c r="L25" s="6"/>
       <c r="M25" s="2"/>
-      <c r="O25" s="115"/>
-      <c r="P25" s="116"/>
-      <c r="Q25" s="116"/>
-      <c r="R25" s="116"/>
-      <c r="S25" s="116"/>
-      <c r="T25" s="117"/>
+      <c r="O25" s="116"/>
+      <c r="P25" s="117"/>
+      <c r="Q25" s="117"/>
+      <c r="R25" s="117"/>
+      <c r="S25" s="117"/>
+      <c r="T25" s="118"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -18837,16 +18794,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -19403,16 +19360,16 @@
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>
@@ -19476,14 +19433,14 @@
       <c r="L13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="107" t="s">
+      <c r="N13" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="107"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="108"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="108"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C14" s="23"/>
@@ -19506,12 +19463,12 @@
       <c r="L14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="107"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107"/>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C15" s="23"/>
@@ -19527,12 +19484,12 @@
       <c r="L15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="107"/>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
+      <c r="N15" s="108"/>
+      <c r="O15" s="108"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
     </row>
     <row r="16" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
@@ -19548,12 +19505,12 @@
       <c r="L16" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="N16" s="107"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107"/>
+      <c r="N16" s="108"/>
+      <c r="O16" s="108"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="108"/>
     </row>
     <row r="17" spans="3:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="23"/>
@@ -19569,14 +19526,14 @@
       <c r="L17" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="N17" s="107" t="s">
+      <c r="N17" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="O17" s="107"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="108"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="23"/>
@@ -19592,12 +19549,12 @@
       <c r="L18" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="N18" s="107"/>
-      <c r="O18" s="107"/>
-      <c r="P18" s="107"/>
-      <c r="Q18" s="107"/>
-      <c r="R18" s="107"/>
-      <c r="S18" s="107"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="108"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="23"/>
@@ -19613,12 +19570,12 @@
       <c r="L19" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="N19" s="107"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="107"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="107"/>
-      <c r="S19" s="107"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="108"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C20" s="23"/>
@@ -19634,12 +19591,12 @@
       <c r="L20" s="87" t="s">
         <v>170</v>
       </c>
-      <c r="N20" s="107"/>
-      <c r="O20" s="107"/>
-      <c r="P20" s="107"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="107"/>
-      <c r="S20" s="107"/>
+      <c r="N20" s="108"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="108"/>
+      <c r="Q20" s="108"/>
+      <c r="R20" s="108"/>
+      <c r="S20" s="108"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -19670,14 +19627,14 @@
       <c r="L22" s="87" t="s">
         <v>254</v>
       </c>
-      <c r="N22" s="108" t="s">
+      <c r="N22" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="O22" s="108"/>
-      <c r="P22" s="108"/>
-      <c r="Q22" s="108"/>
-      <c r="R22" s="108"/>
-      <c r="S22" s="108"/>
+      <c r="O22" s="109"/>
+      <c r="P22" s="109"/>
+      <c r="Q22" s="109"/>
+      <c r="R22" s="109"/>
+      <c r="S22" s="109"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -19702,14 +19659,14 @@
       <c r="J24" s="2"/>
       <c r="K24" s="9"/>
       <c r="L24" s="87"/>
-      <c r="N24" s="107" t="s">
+      <c r="N24" s="108" t="s">
         <v>401</v>
       </c>
-      <c r="O24" s="107"/>
-      <c r="P24" s="107"/>
-      <c r="Q24" s="107"/>
-      <c r="R24" s="107"/>
-      <c r="S24" s="107"/>
+      <c r="O24" s="108"/>
+      <c r="P24" s="108"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C25" s="23"/>
@@ -19719,12 +19676,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="9"/>
       <c r="L25" s="87"/>
-      <c r="N25" s="107"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
+      <c r="N25" s="108"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="108"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="108"/>
+      <c r="S25" s="108"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C26" s="23"/>
@@ -19734,12 +19691,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="9"/>
       <c r="L26" s="4"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
+      <c r="N26" s="108"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="108"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="108"/>
+      <c r="S26" s="108"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -19749,12 +19706,12 @@
       <c r="J27" s="2"/>
       <c r="K27" s="9"/>
       <c r="L27" s="4"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
+      <c r="N27" s="108"/>
+      <c r="O27" s="108"/>
+      <c r="P27" s="108"/>
+      <c r="Q27" s="108"/>
+      <c r="R27" s="108"/>
+      <c r="S27" s="108"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -19764,14 +19721,14 @@
       <c r="J28" s="2"/>
       <c r="K28" s="9"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="107" t="s">
+      <c r="N28" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
+      <c r="Q28" s="108"/>
+      <c r="R28" s="108"/>
+      <c r="S28" s="108"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C29" s="23"/>
@@ -19781,12 +19738,12 @@
       <c r="J29" s="2"/>
       <c r="K29" s="9"/>
       <c r="L29" s="4"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="108"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C30" s="23"/>
@@ -19796,12 +19753,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="9"/>
       <c r="L30" s="2"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="108"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="23"/>
@@ -19811,12 +19768,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="9"/>
       <c r="L31" s="2"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
+      <c r="N31" s="108"/>
+      <c r="O31" s="108"/>
+      <c r="P31" s="108"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="108"/>
+      <c r="S31" s="108"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C32" s="23"/>
@@ -20028,16 +19985,16 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="23"/>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="J10" s="104" t="s">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="J10" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="23"/>

</xml_diff>